<commit_message>
Added function to useless cards in binder
</commit_message>
<xml_diff>
--- a/data/binder/Binder.xlsx
+++ b/data/binder/Binder.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Dados/MTG/data/binder/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Dados/MTG/EDH-DeckHelper/data/binder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BAB7EFE-8FDD-5543-BC09-ED37DDFF77EE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22936C48-9DF7-134B-BB3F-E9A2E2B78B36}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7280" yWindow="460" windowWidth="18300" windowHeight="15540" activeTab="1" xr2:uid="{7ABBCC85-5F92-6F41-92E4-65212D317CF6}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="12680" windowHeight="15540" activeTab="1" xr2:uid="{7ABBCC85-5F92-6F41-92E4-65212D317CF6}"/>
   </bookViews>
   <sheets>
     <sheet name="Dual" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="426">
   <si>
     <t>Slot</t>
   </si>
@@ -1264,23 +1264,63 @@
     <t>Jace, Vryn's Prodigy // Jace, Telepath Unbound</t>
   </si>
   <si>
-    <t>Command the Dreadhore</t>
-  </si>
-  <si>
     <t>Ashiok, Dream Render</t>
   </si>
   <si>
-    <t>Saheeli, the Gifted</t>
+    <t>Dovin's Veto</t>
+  </si>
+  <si>
+    <t>Lim-Dûl's Vault</t>
+  </si>
+  <si>
+    <t>Cephalid Coliseum</t>
+  </si>
+  <si>
+    <t>Nihil Spellbomb</t>
+  </si>
+  <si>
+    <t>Gilded Drake</t>
+  </si>
+  <si>
+    <t>Sai, Master Thopterist</t>
+  </si>
+  <si>
+    <t>Spellseeker</t>
+  </si>
+  <si>
+    <t>Jace, Wielder of Mysteries</t>
+  </si>
+  <si>
+    <t>Copy Artifact</t>
+  </si>
+  <si>
+    <t>Narset's Reversal</t>
+  </si>
+  <si>
+    <t>Plunge into Darkness</t>
+  </si>
+  <si>
+    <t>Fact or Fiction</t>
+  </si>
+  <si>
+    <t>Command the Dreadhorde</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1332,11 +1372,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1656,7 +1697,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97699D74-A98B-734B-9D41-B21A5DBE7339}">
   <dimension ref="A1:F270"/>
   <sheetViews>
-    <sheetView topLeftCell="A208" zoomScale="93" workbookViewId="0">
+    <sheetView topLeftCell="A171" zoomScale="93" workbookViewId="0">
       <selection activeCell="A226" sqref="A226:C257"/>
     </sheetView>
   </sheetViews>
@@ -1671,10 +1712,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="4"/>
+      <c r="B1" s="5"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1">
         <v>44</v>
@@ -6309,8 +6350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5953B7FC-4B75-B146-8A26-6CA09B5F3C99}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A452" workbookViewId="0">
-      <selection activeCell="B457" sqref="B457"/>
+    <sheetView tabSelected="1" topLeftCell="A445" workbookViewId="0">
+      <selection activeCell="B470" sqref="B470:C470"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7542,7 +7583,7 @@
         <v>121</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>316</v>
+        <v>415</v>
       </c>
       <c r="C122" s="1">
         <v>1</v>
@@ -7553,16 +7594,18 @@
         <v>122</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="C123" s="1"/>
+        <v>288</v>
+      </c>
+      <c r="C123" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
         <v>123</v>
       </c>
-      <c r="B124" s="1" t="s">
-        <v>317</v>
+      <c r="B124" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="C124" s="1">
         <v>1</v>
@@ -7573,7 +7616,7 @@
         <v>124</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>318</v>
+        <v>256</v>
       </c>
       <c r="C125" s="1">
         <v>1</v>
@@ -7583,8 +7626,8 @@
       <c r="A126" s="1">
         <v>125</v>
       </c>
-      <c r="B126" s="1" t="s">
-        <v>288</v>
+      <c r="B126" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="C126" s="1">
         <v>1</v>
@@ -7595,7 +7638,7 @@
         <v>126</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C127" s="1">
         <v>1</v>
@@ -7605,8 +7648,8 @@
       <c r="A128" s="1">
         <v>127</v>
       </c>
-      <c r="B128" s="1" t="s">
-        <v>256</v>
+      <c r="B128" s="2" t="s">
+        <v>397</v>
       </c>
       <c r="C128" s="1">
         <v>1</v>
@@ -7617,7 +7660,7 @@
         <v>128</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>65</v>
+        <v>336</v>
       </c>
       <c r="C129" s="1">
         <v>1</v>
@@ -7627,8 +7670,8 @@
       <c r="A130" s="1">
         <v>129</v>
       </c>
-      <c r="B130" s="2" t="s">
-        <v>67</v>
+      <c r="B130" s="1" t="s">
+        <v>291</v>
       </c>
       <c r="C130" s="1">
         <v>1</v>
@@ -7638,8 +7681,8 @@
       <c r="A131" s="1">
         <v>130</v>
       </c>
-      <c r="B131" s="2" t="s">
-        <v>72</v>
+      <c r="B131" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="C131" s="1">
         <v>1</v>
@@ -7650,18 +7693,16 @@
         <v>131</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="C132" s="1">
-        <v>1</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="C132" s="1"/>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
         <v>132</v>
       </c>
-      <c r="B133" s="2" t="s">
-        <v>397</v>
+      <c r="B133" s="1" t="s">
+        <v>312</v>
       </c>
       <c r="C133" s="1">
         <v>1</v>
@@ -7672,7 +7713,7 @@
         <v>133</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>336</v>
+        <v>64</v>
       </c>
       <c r="C134" s="1">
         <v>1</v>
@@ -7682,8 +7723,8 @@
       <c r="A135" s="1">
         <v>134</v>
       </c>
-      <c r="B135" s="1" t="s">
-        <v>291</v>
+      <c r="B135" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="C135" s="1">
         <v>1</v>
@@ -7694,106 +7735,72 @@
         <v>135</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C136" s="1">
-        <v>1</v>
-      </c>
+        <v>250</v>
+      </c>
+      <c r="C136" s="1"/>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
         <v>136</v>
       </c>
-      <c r="B137" s="2" t="s">
-        <v>68</v>
-      </c>
+      <c r="B137" s="1"/>
       <c r="C137" s="1"/>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
         <v>137</v>
       </c>
-      <c r="B138" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="C138" s="1">
-        <v>1</v>
-      </c>
+      <c r="B138" s="1"/>
+      <c r="C138" s="1"/>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
         <v>138</v>
       </c>
-      <c r="B139" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C139" s="1">
-        <v>1</v>
-      </c>
+      <c r="B139" s="1"/>
+      <c r="C139" s="1"/>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" s="1">
         <v>139</v>
       </c>
-      <c r="B140" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C140" s="1">
-        <v>1</v>
-      </c>
+      <c r="B140" s="1"/>
+      <c r="C140" s="1"/>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
         <v>140</v>
       </c>
-      <c r="B141" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="C141" s="1">
-        <v>1</v>
-      </c>
+      <c r="B141" s="1"/>
+      <c r="C141" s="1"/>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
         <v>141</v>
       </c>
-      <c r="B142" s="2" t="s">
-        <v>250</v>
-      </c>
+      <c r="B142" s="1"/>
       <c r="C142" s="1"/>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
         <v>142</v>
       </c>
-      <c r="B143" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="C143" s="1">
-        <v>1</v>
-      </c>
+      <c r="B143" s="1"/>
+      <c r="C143" s="1"/>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
         <v>143</v>
       </c>
-      <c r="B144" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="C144" s="1">
-        <v>1</v>
-      </c>
+      <c r="B144" s="1"/>
+      <c r="C144" s="1"/>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
         <v>144</v>
       </c>
-      <c r="B145" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="C145" s="1">
-        <v>1</v>
-      </c>
+      <c r="B145" s="1"/>
+      <c r="C145" s="1"/>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
@@ -7906,7 +7913,7 @@
         <v>159</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>383</v>
+        <v>104</v>
       </c>
       <c r="C160" s="1">
         <v>1</v>
@@ -7917,16 +7924,18 @@
         <v>160</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="C161" s="1"/>
+        <v>374</v>
+      </c>
+      <c r="C161" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162" s="1">
         <v>161</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="C162" s="1">
         <v>1</v>
@@ -7937,7 +7946,7 @@
         <v>162</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>374</v>
+        <v>225</v>
       </c>
       <c r="C163" s="1">
         <v>1</v>
@@ -7948,7 +7957,7 @@
         <v>163</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C164" s="1">
         <v>1</v>
@@ -7959,18 +7968,16 @@
         <v>164</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="C165" s="1">
-        <v>1</v>
-      </c>
+        <v>280</v>
+      </c>
+      <c r="C165" s="1"/>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
         <v>165</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C166" s="1">
         <v>1</v>
@@ -7981,16 +7988,18 @@
         <v>166</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="C167" s="1"/>
+        <v>376</v>
+      </c>
+      <c r="C167" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168" s="1">
         <v>167</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="C168" s="1">
         <v>1</v>
@@ -8001,7 +8010,7 @@
         <v>168</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>376</v>
+        <v>227</v>
       </c>
       <c r="C169" s="1">
         <v>1</v>
@@ -8012,7 +8021,7 @@
         <v>169</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="C170" s="1">
         <v>1</v>
@@ -8023,7 +8032,7 @@
         <v>170</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>227</v>
+        <v>109</v>
       </c>
       <c r="C171" s="1">
         <v>1</v>
@@ -8034,7 +8043,7 @@
         <v>171</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>85</v>
+        <v>384</v>
       </c>
       <c r="C172" s="1">
         <v>1</v>
@@ -8045,7 +8054,7 @@
         <v>172</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="C173" s="1">
         <v>1</v>
@@ -8056,7 +8065,7 @@
         <v>173</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>384</v>
+        <v>110</v>
       </c>
       <c r="C174" s="1">
         <v>1</v>
@@ -8067,7 +8076,7 @@
         <v>174</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>214</v>
+        <v>385</v>
       </c>
       <c r="C175" s="1">
         <v>1</v>
@@ -8078,18 +8087,16 @@
         <v>175</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C176" s="1">
-        <v>1</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="C176" s="1"/>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
         <v>176</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="C177" s="1">
         <v>1</v>
@@ -8100,7 +8107,7 @@
         <v>177</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>281</v>
+        <v>89</v>
       </c>
       <c r="C178" s="1">
         <v>1</v>
@@ -8111,7 +8118,7 @@
         <v>178</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>385</v>
+        <v>90</v>
       </c>
       <c r="C179" s="1">
         <v>1</v>
@@ -8122,16 +8129,18 @@
         <v>179</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C180" s="1"/>
+        <v>91</v>
+      </c>
+      <c r="C180" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A181" s="1">
         <v>180</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C181" s="1">
         <v>1</v>
@@ -8142,7 +8151,7 @@
         <v>181</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C182" s="1">
         <v>1</v>
@@ -8153,7 +8162,7 @@
         <v>182</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>90</v>
+        <v>387</v>
       </c>
       <c r="C183" s="1">
         <v>1</v>
@@ -8164,7 +8173,7 @@
         <v>183</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>233</v>
+        <v>416</v>
       </c>
       <c r="C184" s="1">
         <v>1</v>
@@ -8175,18 +8184,16 @@
         <v>184</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C185" s="1">
-        <v>1</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="C185" s="1"/>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A186" s="1">
         <v>185</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="C186" s="1">
         <v>1</v>
@@ -8197,7 +8204,7 @@
         <v>186</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C187" s="1">
         <v>1</v>
@@ -8208,7 +8215,7 @@
         <v>187</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>386</v>
+        <v>105</v>
       </c>
       <c r="C188" s="1">
         <v>1</v>
@@ -8219,7 +8226,7 @@
         <v>188</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="C189" s="1">
         <v>1</v>
@@ -8230,16 +8237,18 @@
         <v>189</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C190" s="1"/>
+        <v>249</v>
+      </c>
+      <c r="C190" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A191" s="1">
         <v>190</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C191" s="1">
         <v>1</v>
@@ -8250,7 +8259,7 @@
         <v>191</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C192" s="1">
         <v>1</v>
@@ -8261,7 +8270,7 @@
         <v>192</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>282</v>
+        <v>106</v>
       </c>
       <c r="C193" s="1">
         <v>1</v>
@@ -8272,7 +8281,7 @@
         <v>193</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C194" s="1">
         <v>1</v>
@@ -8283,7 +8292,7 @@
         <v>194</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>388</v>
+        <v>98</v>
       </c>
       <c r="C195" s="1">
         <v>1</v>
@@ -8293,10 +8302,10 @@
       <c r="A196" s="1">
         <v>195</v>
       </c>
-      <c r="B196" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="C196" s="1">
+      <c r="B196" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="C196" s="3">
         <v>1</v>
       </c>
     </row>
@@ -8305,7 +8314,7 @@
         <v>196</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>112</v>
+        <v>378</v>
       </c>
       <c r="C197" s="1">
         <v>1</v>
@@ -8316,7 +8325,7 @@
         <v>197</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>96</v>
+        <v>379</v>
       </c>
       <c r="C198" s="1">
         <v>1</v>
@@ -8327,7 +8336,7 @@
         <v>198</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>106</v>
+        <v>380</v>
       </c>
       <c r="C199" s="1">
         <v>1</v>
@@ -8338,7 +8347,7 @@
         <v>199</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C200" s="1">
         <v>1</v>
@@ -8349,7 +8358,7 @@
         <v>200</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>98</v>
+        <v>381</v>
       </c>
       <c r="C201" s="1">
         <v>1</v>
@@ -8360,7 +8369,7 @@
         <v>201</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>239</v>
+        <v>113</v>
       </c>
       <c r="C202" s="1">
         <v>1</v>
@@ -8371,7 +8380,7 @@
         <v>202</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>263</v>
+        <v>100</v>
       </c>
       <c r="C203" s="1">
         <v>1</v>
@@ -8381,10 +8390,10 @@
       <c r="A204" s="1">
         <v>203</v>
       </c>
-      <c r="B204" s="3" t="s">
-        <v>389</v>
-      </c>
-      <c r="C204" s="3">
+      <c r="B204" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C204" s="1">
         <v>1</v>
       </c>
     </row>
@@ -8393,7 +8402,7 @@
         <v>204</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="C205" s="1">
         <v>1</v>
@@ -8404,7 +8413,7 @@
         <v>205</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>379</v>
+        <v>115</v>
       </c>
       <c r="C206" s="1">
         <v>1</v>
@@ -8415,7 +8424,7 @@
         <v>206</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>380</v>
+        <v>285</v>
       </c>
       <c r="C207" s="1">
         <v>1</v>
@@ -8426,7 +8435,7 @@
         <v>207</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>99</v>
+        <v>390</v>
       </c>
       <c r="C208" s="1">
         <v>1</v>
@@ -8437,7 +8446,7 @@
         <v>208</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>381</v>
+        <v>391</v>
       </c>
       <c r="C209" s="1">
         <v>1</v>
@@ -8448,7 +8457,7 @@
         <v>209</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>113</v>
+        <v>393</v>
       </c>
       <c r="C210" s="1">
         <v>1</v>
@@ -8459,7 +8468,7 @@
         <v>210</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C211" s="1">
         <v>1</v>
@@ -8470,7 +8479,7 @@
         <v>211</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="C212" s="1">
         <v>1</v>
@@ -8481,7 +8490,7 @@
         <v>212</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>382</v>
+        <v>103</v>
       </c>
       <c r="C213" s="1">
         <v>1</v>
@@ -8491,168 +8500,112 @@
       <c r="A214" s="1">
         <v>213</v>
       </c>
-      <c r="B214" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C214" s="1">
-        <v>1</v>
-      </c>
+      <c r="B214" s="1"/>
+      <c r="C214" s="1"/>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A215" s="1">
         <v>214</v>
       </c>
-      <c r="B215" s="1" t="s">
-        <v>275</v>
-      </c>
+      <c r="B215" s="1"/>
       <c r="C215" s="1"/>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A216" s="1">
         <v>215</v>
       </c>
-      <c r="B216" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="C216" s="1">
-        <v>1</v>
-      </c>
+      <c r="B216" s="1"/>
+      <c r="C216" s="1"/>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A217" s="1">
         <v>216</v>
       </c>
-      <c r="B217" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="C217" s="1">
-        <v>1</v>
-      </c>
+      <c r="B217" s="1"/>
+      <c r="C217" s="1"/>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A218" s="1">
         <v>217</v>
       </c>
-      <c r="B218" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="C218" s="1">
-        <v>1</v>
-      </c>
+      <c r="B218" s="1"/>
+      <c r="C218" s="1"/>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A219" s="1">
         <v>218</v>
       </c>
-      <c r="B219" s="1" t="s">
-        <v>391</v>
-      </c>
-      <c r="C219" s="1">
-        <v>1</v>
-      </c>
+      <c r="B219" s="1"/>
+      <c r="C219" s="1"/>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A220" s="1">
         <v>219</v>
       </c>
-      <c r="B220" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="C220" s="1">
-        <v>1</v>
-      </c>
+      <c r="B220" s="1"/>
+      <c r="C220" s="1"/>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A221" s="1">
         <v>220</v>
       </c>
-      <c r="B221" s="3" t="s">
-        <v>392</v>
-      </c>
-      <c r="C221" s="3">
-        <v>1</v>
-      </c>
+      <c r="B221" s="1"/>
+      <c r="C221" s="1"/>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A222" s="1">
         <v>221</v>
       </c>
-      <c r="B222" s="1" t="s">
-        <v>276</v>
-      </c>
+      <c r="B222" s="1"/>
       <c r="C222" s="1"/>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A223" s="1">
         <v>222</v>
       </c>
-      <c r="B223" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="C223" s="1">
-        <v>1</v>
-      </c>
+      <c r="B223" s="1"/>
+      <c r="C223" s="1"/>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A224" s="1">
         <v>223</v>
       </c>
-      <c r="B224" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="C224" s="1">
-        <v>1</v>
-      </c>
+      <c r="B224" s="1"/>
+      <c r="C224" s="1"/>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A225" s="1">
         <v>224</v>
       </c>
-      <c r="B225" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C225" s="1">
-        <v>1</v>
-      </c>
+      <c r="B225" s="1"/>
+      <c r="C225" s="1"/>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A226" s="1">
         <v>225</v>
       </c>
-      <c r="B226" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C226" s="1">
-        <v>1</v>
-      </c>
+      <c r="B226" s="1"/>
+      <c r="C226" s="1"/>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A227" s="1">
         <v>226</v>
       </c>
-      <c r="B227" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C227" s="1">
-        <v>1</v>
-      </c>
+      <c r="B227" s="1"/>
+      <c r="C227" s="1"/>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A228" s="1">
         <v>227</v>
       </c>
-      <c r="B228" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="C228" s="1">
-        <v>1</v>
-      </c>
+      <c r="B228" s="1"/>
+      <c r="C228" s="1"/>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A229" s="1">
         <v>228</v>
       </c>
-      <c r="B229" s="1"/>
+      <c r="B229" s="2"/>
       <c r="C229" s="1"/>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.2">
@@ -8660,7 +8613,7 @@
         <v>229</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>244</v>
+        <v>117</v>
       </c>
       <c r="C230" s="1">
         <v>1</v>
@@ -8671,7 +8624,7 @@
         <v>230</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C231" s="1">
         <v>1</v>
@@ -8682,7 +8635,7 @@
         <v>231</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>253</v>
+        <v>272</v>
       </c>
       <c r="C232" s="1">
         <v>1</v>
@@ -8693,7 +8646,7 @@
         <v>232</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="C233" s="1">
         <v>1</v>
@@ -8704,7 +8657,7 @@
         <v>233</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="C234" s="1">
         <v>1</v>
@@ -8715,7 +8668,7 @@
         <v>234</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>116</v>
+        <v>340</v>
       </c>
       <c r="C235" s="1">
         <v>1</v>
@@ -8726,7 +8679,7 @@
         <v>235</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>255</v>
+        <v>289</v>
       </c>
       <c r="C236" s="1">
         <v>1</v>
@@ -8737,7 +8690,7 @@
         <v>236</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C237" s="1">
         <v>1</v>
@@ -8748,7 +8701,7 @@
         <v>237</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>257</v>
+        <v>405</v>
       </c>
       <c r="C238" s="1">
         <v>1</v>
@@ -8759,7 +8712,7 @@
         <v>238</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>272</v>
+        <v>310</v>
       </c>
       <c r="C239" s="1">
         <v>1</v>
@@ -8770,7 +8723,7 @@
         <v>239</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>260</v>
+        <v>118</v>
       </c>
       <c r="C240" s="1">
         <v>1</v>
@@ -8781,7 +8734,7 @@
         <v>240</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>261</v>
+        <v>119</v>
       </c>
       <c r="C241" s="1">
         <v>1</v>
@@ -8792,7 +8745,7 @@
         <v>241</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>262</v>
+        <v>120</v>
       </c>
       <c r="C242" s="1">
         <v>1</v>
@@ -8803,7 +8756,7 @@
         <v>242</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>273</v>
+        <v>252</v>
       </c>
       <c r="C243" s="1">
         <v>1</v>
@@ -8814,7 +8767,7 @@
         <v>243</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="C244" s="1">
         <v>1</v>
@@ -8824,186 +8777,120 @@
       <c r="A245" s="1">
         <v>244</v>
       </c>
-      <c r="B245" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="C245" s="1">
-        <v>1</v>
-      </c>
+      <c r="B245" s="1"/>
+      <c r="C245" s="1"/>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A246" s="1">
         <v>245</v>
       </c>
-      <c r="B246" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="C246" s="1">
-        <v>1</v>
-      </c>
+      <c r="B246" s="1"/>
+      <c r="C246" s="1"/>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A247" s="1">
         <v>246</v>
       </c>
-      <c r="B247" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="C247" s="1">
-        <v>1</v>
-      </c>
+      <c r="B247" s="1"/>
+      <c r="C247" s="1"/>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A248" s="1">
         <v>247</v>
       </c>
-      <c r="B248" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="C248" s="1">
-        <v>1</v>
-      </c>
+      <c r="B248" s="1"/>
+      <c r="C248" s="1"/>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A249" s="1">
         <v>248</v>
       </c>
-      <c r="B249" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="C249" s="1">
-        <v>1</v>
-      </c>
+      <c r="B249" s="1"/>
+      <c r="C249" s="1"/>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A250" s="1">
         <v>249</v>
       </c>
-      <c r="B250" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="C250" s="1">
-        <v>1</v>
-      </c>
+      <c r="B250" s="1"/>
+      <c r="C250" s="1"/>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A251" s="1">
         <v>250</v>
       </c>
-      <c r="B251" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="C251" s="1">
-        <v>1</v>
-      </c>
+      <c r="B251" s="1"/>
+      <c r="C251" s="1"/>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A252" s="1">
         <v>251</v>
       </c>
-      <c r="B252" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="C252" s="1">
-        <v>1</v>
-      </c>
+      <c r="B252" s="1"/>
+      <c r="C252" s="1"/>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A253" s="1">
         <v>252</v>
       </c>
-      <c r="B253" s="1" t="s">
-        <v>405</v>
-      </c>
-      <c r="C253" s="1">
-        <v>1</v>
-      </c>
+      <c r="B253" s="1"/>
+      <c r="C253" s="1"/>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A254" s="1">
         <v>253</v>
       </c>
-      <c r="B254" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="C254" s="1">
-        <v>1</v>
-      </c>
+      <c r="B254" s="1"/>
+      <c r="C254" s="1"/>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A255" s="1">
         <v>254</v>
       </c>
-      <c r="B255" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C255" s="1">
-        <v>1</v>
-      </c>
+      <c r="B255" s="1"/>
+      <c r="C255" s="1"/>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A256" s="1">
         <v>255</v>
       </c>
-      <c r="B256" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="C256" s="1">
-        <v>1</v>
-      </c>
+      <c r="B256" s="1"/>
+      <c r="C256" s="1"/>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A257" s="1">
         <v>256</v>
       </c>
-      <c r="B257" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C257" s="1">
-        <v>1</v>
-      </c>
+      <c r="B257" s="1"/>
+      <c r="C257" s="1"/>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A258" s="1">
         <v>257</v>
       </c>
-      <c r="B258" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C258" s="1">
-        <v>1</v>
-      </c>
+      <c r="B258" s="1"/>
+      <c r="C258" s="1"/>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A259" s="1">
         <v>258</v>
       </c>
-      <c r="B259" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="C259" s="1">
-        <v>1</v>
-      </c>
+      <c r="B259" s="1"/>
+      <c r="C259" s="1"/>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A260" s="1">
         <v>259</v>
       </c>
-      <c r="B260" s="1" t="s">
-        <v>274</v>
-      </c>
+      <c r="B260" s="1"/>
       <c r="C260" s="1"/>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A261" s="1">
         <v>260</v>
       </c>
-      <c r="B261" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="C261" s="1">
-        <v>1</v>
-      </c>
+      <c r="B261" s="1"/>
+      <c r="C261" s="1"/>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A262" s="1">
@@ -9038,7 +8925,7 @@
         <v>265</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>215</v>
+        <v>226</v>
       </c>
       <c r="C266" s="1">
         <v>1</v>
@@ -9049,11 +8936,9 @@
         <v>266</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="C267" s="1">
-        <v>1</v>
-      </c>
+        <v>417</v>
+      </c>
+      <c r="C267" s="1"/>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A268" s="1">
@@ -9081,12 +8966,10 @@
       <c r="A270" s="1">
         <v>269</v>
       </c>
-      <c r="B270" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="C270" s="1">
-        <v>1</v>
-      </c>
+      <c r="B270" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="C270" s="1"/>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A271" s="1">
@@ -9104,7 +8987,7 @@
         <v>271</v>
       </c>
       <c r="B272" s="1" t="s">
-        <v>123</v>
+        <v>419</v>
       </c>
       <c r="C272" s="1">
         <v>1</v>
@@ -9115,7 +8998,7 @@
         <v>272</v>
       </c>
       <c r="B273" s="1" t="s">
-        <v>284</v>
+        <v>123</v>
       </c>
       <c r="C273" s="1">
         <v>1</v>
@@ -9126,7 +9009,7 @@
         <v>273</v>
       </c>
       <c r="B274" s="1" t="s">
-        <v>223</v>
+        <v>420</v>
       </c>
       <c r="C274" s="1">
         <v>1</v>
@@ -9137,7 +9020,7 @@
         <v>274</v>
       </c>
       <c r="B275" s="1" t="s">
-        <v>124</v>
+        <v>284</v>
       </c>
       <c r="C275" s="1">
         <v>1</v>
@@ -9148,7 +9031,7 @@
         <v>275</v>
       </c>
       <c r="B276" s="1" t="s">
-        <v>283</v>
+        <v>421</v>
       </c>
       <c r="C276" s="1">
         <v>1</v>
@@ -9159,7 +9042,7 @@
         <v>276</v>
       </c>
       <c r="B277" s="1" t="s">
-        <v>295</v>
+        <v>124</v>
       </c>
       <c r="C277" s="1">
         <v>1</v>
@@ -9170,7 +9053,7 @@
         <v>277</v>
       </c>
       <c r="B278" s="1" t="s">
-        <v>394</v>
+        <v>283</v>
       </c>
       <c r="C278" s="1">
         <v>1</v>
@@ -9181,7 +9064,7 @@
         <v>278</v>
       </c>
       <c r="B279" s="1" t="s">
-        <v>125</v>
+        <v>394</v>
       </c>
       <c r="C279" s="1">
         <v>1</v>
@@ -9192,7 +9075,7 @@
         <v>279</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C280" s="1">
         <v>1</v>
@@ -9203,7 +9086,7 @@
         <v>280</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C281" s="1">
         <v>1</v>
@@ -9214,7 +9097,7 @@
         <v>281</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C282" s="1">
         <v>1</v>
@@ -9225,7 +9108,7 @@
         <v>282</v>
       </c>
       <c r="B283" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C283" s="1">
         <v>1</v>
@@ -9236,7 +9119,7 @@
         <v>283</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C284" s="1">
         <v>1</v>
@@ -9247,7 +9130,7 @@
         <v>284</v>
       </c>
       <c r="B285" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C285" s="1">
         <v>1</v>
@@ -9258,7 +9141,7 @@
         <v>285</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C286" s="1">
         <v>1</v>
@@ -9269,7 +9152,7 @@
         <v>286</v>
       </c>
       <c r="B287" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C287" s="1">
         <v>1</v>
@@ -9280,7 +9163,7 @@
         <v>287</v>
       </c>
       <c r="B288" s="1" t="s">
-        <v>134</v>
+        <v>424</v>
       </c>
       <c r="C288" s="1">
         <v>1</v>
@@ -9291,7 +9174,7 @@
         <v>288</v>
       </c>
       <c r="B289" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C289" s="1">
         <v>1</v>
@@ -9302,7 +9185,7 @@
         <v>289</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>216</v>
+        <v>134</v>
       </c>
       <c r="C290" s="1">
         <v>1</v>
@@ -9313,7 +9196,7 @@
         <v>290</v>
       </c>
       <c r="B291" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C291" s="1">
         <v>1</v>
@@ -9324,7 +9207,7 @@
         <v>291</v>
       </c>
       <c r="B292" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C292" s="1">
         <v>1</v>
@@ -9335,7 +9218,7 @@
         <v>292</v>
       </c>
       <c r="B293" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C293" s="1">
         <v>1</v>
@@ -9346,7 +9229,7 @@
         <v>293</v>
       </c>
       <c r="B294" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C294" s="1">
         <v>1</v>
@@ -9357,7 +9240,7 @@
         <v>294</v>
       </c>
       <c r="B295" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C295" s="1">
         <v>1</v>
@@ -9368,7 +9251,7 @@
         <v>295</v>
       </c>
       <c r="B296" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C296" s="1">
         <v>1</v>
@@ -9379,7 +9262,7 @@
         <v>296</v>
       </c>
       <c r="B297" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C297" s="1">
         <v>1</v>
@@ -9390,7 +9273,7 @@
         <v>297</v>
       </c>
       <c r="B298" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C298" s="1">
         <v>1</v>
@@ -9401,7 +9284,7 @@
         <v>298</v>
       </c>
       <c r="B299" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C299" s="1">
         <v>1</v>
@@ -9412,7 +9295,7 @@
         <v>299</v>
       </c>
       <c r="B300" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C300" s="1">
         <v>1</v>
@@ -9423,7 +9306,7 @@
         <v>300</v>
       </c>
       <c r="B301" s="1" t="s">
-        <v>306</v>
+        <v>422</v>
       </c>
       <c r="C301" s="1">
         <v>1</v>
@@ -9434,7 +9317,7 @@
         <v>301</v>
       </c>
       <c r="B302" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C302" s="1">
         <v>1</v>
@@ -9445,7 +9328,7 @@
         <v>302</v>
       </c>
       <c r="B303" s="1" t="s">
-        <v>409</v>
+        <v>306</v>
       </c>
       <c r="C303" s="1">
         <v>1</v>
@@ -9456,7 +9339,7 @@
         <v>303</v>
       </c>
       <c r="B304" s="1" t="s">
-        <v>217</v>
+        <v>146</v>
       </c>
       <c r="C304" s="1">
         <v>1</v>
@@ -9531,7 +9414,7 @@
         <v>310</v>
       </c>
       <c r="B311" s="1" t="s">
-        <v>219</v>
+        <v>153</v>
       </c>
       <c r="C311" s="1">
         <v>1</v>
@@ -9542,7 +9425,7 @@
         <v>311</v>
       </c>
       <c r="B312" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C312" s="1">
         <v>1</v>
@@ -9553,7 +9436,7 @@
         <v>312</v>
       </c>
       <c r="B313" s="1" t="s">
-        <v>154</v>
+        <v>221</v>
       </c>
       <c r="C313" s="1">
         <v>1</v>
@@ -9564,7 +9447,7 @@
         <v>313</v>
       </c>
       <c r="B314" s="1" t="s">
-        <v>311</v>
+        <v>155</v>
       </c>
       <c r="C314" s="1">
         <v>1</v>
@@ -9575,51 +9458,43 @@
         <v>314</v>
       </c>
       <c r="B315" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="C315" s="1">
-        <v>1</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="C315" s="1"/>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A316" s="1">
         <v>315</v>
       </c>
       <c r="B316" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C316" s="1">
-        <v>1</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="C316" s="1"/>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A317" s="1">
         <v>316</v>
       </c>
       <c r="B317" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C317" s="1"/>
+        <v>158</v>
+      </c>
+      <c r="C317" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A318" s="1">
         <v>317</v>
       </c>
-      <c r="B318" s="1" t="s">
-        <v>157</v>
-      </c>
+      <c r="B318" s="1"/>
       <c r="C318" s="1"/>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A319" s="1">
         <v>318</v>
       </c>
-      <c r="B319" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C319" s="1">
-        <v>1</v>
-      </c>
+      <c r="B319" s="1"/>
+      <c r="C319" s="1"/>
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A320" s="1">
@@ -9820,7 +9695,7 @@
         <v>339</v>
       </c>
       <c r="B340" s="1" t="s">
-        <v>412</v>
+        <v>425</v>
       </c>
       <c r="C340" s="1">
         <v>1</v>
@@ -9904,18 +9779,16 @@
         <v>347</v>
       </c>
       <c r="B348" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="C348" s="1">
-        <v>1</v>
-      </c>
+        <v>423</v>
+      </c>
+      <c r="C348" s="1"/>
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A349" s="1">
         <v>348</v>
       </c>
       <c r="B349" s="1" t="s">
-        <v>334</v>
+        <v>176</v>
       </c>
       <c r="C349" s="1">
         <v>1</v>
@@ -9926,7 +9799,7 @@
         <v>349</v>
       </c>
       <c r="B350" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C350" s="1">
         <v>1</v>
@@ -9937,7 +9810,7 @@
         <v>350</v>
       </c>
       <c r="B351" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C351" s="1">
         <v>1</v>
@@ -9947,23 +9820,15 @@
       <c r="A352" s="1">
         <v>351</v>
       </c>
-      <c r="B352" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="C352" s="1">
-        <v>1</v>
-      </c>
+      <c r="B352" s="1"/>
+      <c r="C352" s="1"/>
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A353" s="1">
         <v>352</v>
       </c>
-      <c r="B353" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C353" s="1">
-        <v>1</v>
-      </c>
+      <c r="B353" s="1"/>
+      <c r="C353" s="1"/>
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A354" s="1">
@@ -10025,8 +9890,8 @@
       <c r="A362" s="1">
         <v>361</v>
       </c>
-      <c r="B362" s="2" t="s">
-        <v>338</v>
+      <c r="B362" s="1" t="s">
+        <v>179</v>
       </c>
       <c r="C362" s="1">
         <v>1</v>
@@ -10037,7 +9902,7 @@
         <v>362</v>
       </c>
       <c r="B363" s="1" t="s">
-        <v>258</v>
+        <v>180</v>
       </c>
       <c r="C363" s="1">
         <v>1</v>
@@ -10048,7 +9913,7 @@
         <v>363</v>
       </c>
       <c r="B364" s="1" t="s">
-        <v>259</v>
+        <v>396</v>
       </c>
       <c r="C364" s="1">
         <v>1</v>
@@ -10059,7 +9924,7 @@
         <v>364</v>
       </c>
       <c r="B365" s="1" t="s">
-        <v>228</v>
+        <v>181</v>
       </c>
       <c r="C365" s="1">
         <v>1</v>
@@ -10069,8 +9934,8 @@
       <c r="A366" s="1">
         <v>365</v>
       </c>
-      <c r="B366" s="1" t="s">
-        <v>286</v>
+      <c r="B366" s="2" t="s">
+        <v>220</v>
       </c>
       <c r="C366" s="1">
         <v>1</v>
@@ -10080,8 +9945,8 @@
       <c r="A367" s="1">
         <v>366</v>
       </c>
-      <c r="B367" s="2" t="s">
-        <v>224</v>
+      <c r="B367" s="1" t="s">
+        <v>268</v>
       </c>
       <c r="C367" s="1">
         <v>1</v>
@@ -10091,108 +9956,72 @@
       <c r="A368" s="1">
         <v>367</v>
       </c>
-      <c r="B368" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="C368" s="1">
-        <v>1</v>
-      </c>
+      <c r="B368" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C368" s="1"/>
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A369" s="1">
         <v>368</v>
       </c>
-      <c r="B369" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="C369" s="1">
-        <v>1</v>
-      </c>
+      <c r="B369" s="1"/>
+      <c r="C369" s="1"/>
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A370" s="1">
         <v>369</v>
       </c>
-      <c r="B370" s="1" t="s">
-        <v>396</v>
-      </c>
-      <c r="C370" s="1">
-        <v>1</v>
-      </c>
+      <c r="B370" s="1"/>
+      <c r="C370" s="1"/>
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A371" s="1">
         <v>370</v>
       </c>
-      <c r="B371" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="C371" s="1">
-        <v>1</v>
-      </c>
+      <c r="B371" s="1"/>
+      <c r="C371" s="1"/>
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A372" s="1">
         <v>371</v>
       </c>
-      <c r="B372" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="C372" s="1">
-        <v>1</v>
-      </c>
+      <c r="B372" s="1"/>
+      <c r="C372" s="1"/>
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A373" s="1">
         <v>372</v>
       </c>
-      <c r="B373" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="C373" s="1">
-        <v>1</v>
-      </c>
+      <c r="B373" s="1"/>
+      <c r="C373" s="1"/>
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A374" s="1">
         <v>373</v>
       </c>
-      <c r="B374" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="C374" s="1">
-        <v>1</v>
-      </c>
+      <c r="B374" s="1"/>
+      <c r="C374" s="1"/>
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A375" s="1">
         <v>374</v>
       </c>
-      <c r="B375" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="C375" s="1">
-        <v>1</v>
-      </c>
+      <c r="B375" s="1"/>
+      <c r="C375" s="1"/>
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A376" s="1">
         <v>375</v>
       </c>
-      <c r="B376" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="C376" s="1">
-        <v>1</v>
-      </c>
+      <c r="B376" s="1"/>
+      <c r="C376" s="1"/>
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A377" s="1">
         <v>376</v>
       </c>
-      <c r="B377" s="2" t="s">
-        <v>222</v>
-      </c>
+      <c r="B377" s="1"/>
       <c r="C377" s="1"/>
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.2">
@@ -10267,7 +10096,7 @@
         <v>386</v>
       </c>
       <c r="B387" s="1" t="s">
-        <v>342</v>
+        <v>183</v>
       </c>
       <c r="C387" s="1">
         <v>1</v>
@@ -10278,18 +10107,16 @@
         <v>387</v>
       </c>
       <c r="B388" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="C388" s="1">
-        <v>1</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="C388" s="1"/>
     </row>
     <row r="389" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A389" s="1">
         <v>388</v>
       </c>
       <c r="B389" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C389" s="1"/>
     </row>
@@ -10298,16 +10125,18 @@
         <v>389</v>
       </c>
       <c r="B390" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="C390" s="1"/>
+        <v>204</v>
+      </c>
+      <c r="C390" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="391" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A391" s="1">
         <v>390</v>
       </c>
       <c r="B391" s="1" t="s">
-        <v>204</v>
+        <v>186</v>
       </c>
       <c r="C391" s="1">
         <v>1</v>
@@ -10318,7 +10147,7 @@
         <v>391</v>
       </c>
       <c r="B392" s="1" t="s">
-        <v>343</v>
+        <v>187</v>
       </c>
       <c r="C392" s="1">
         <v>1</v>
@@ -10329,18 +10158,16 @@
         <v>392</v>
       </c>
       <c r="B393" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="C393" s="1">
-        <v>1</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="C393" s="1"/>
     </row>
     <row r="394" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A394" s="1">
         <v>393</v>
       </c>
       <c r="B394" s="1" t="s">
-        <v>345</v>
+        <v>189</v>
       </c>
       <c r="C394" s="1">
         <v>1</v>
@@ -10351,7 +10178,7 @@
         <v>394</v>
       </c>
       <c r="B395" s="1" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="C395" s="1">
         <v>1</v>
@@ -10362,7 +10189,7 @@
         <v>395</v>
       </c>
       <c r="B396" s="1" t="s">
-        <v>346</v>
+        <v>191</v>
       </c>
       <c r="C396" s="1">
         <v>1</v>
@@ -10373,18 +10200,16 @@
         <v>396</v>
       </c>
       <c r="B397" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="C397" s="1">
-        <v>1</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="C397" s="1"/>
     </row>
     <row r="398" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A398" s="1">
         <v>397</v>
       </c>
       <c r="B398" s="1" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="C398" s="1">
         <v>1</v>
@@ -10395,7 +10220,7 @@
         <v>398</v>
       </c>
       <c r="B399" s="1" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="C399" s="1"/>
     </row>
@@ -10404,7 +10229,7 @@
         <v>399</v>
       </c>
       <c r="B400" s="1" t="s">
-        <v>348</v>
+        <v>195</v>
       </c>
       <c r="C400" s="1">
         <v>1</v>
@@ -10415,18 +10240,16 @@
         <v>400</v>
       </c>
       <c r="B401" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="C401" s="1">
-        <v>1</v>
-      </c>
+        <v>196</v>
+      </c>
+      <c r="C401" s="1"/>
     </row>
     <row r="402" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A402" s="1">
         <v>401</v>
       </c>
       <c r="B402" s="1" t="s">
-        <v>349</v>
+        <v>197</v>
       </c>
       <c r="C402" s="1">
         <v>1</v>
@@ -10437,29 +10260,25 @@
         <v>402</v>
       </c>
       <c r="B403" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="C403" s="1">
-        <v>1</v>
-      </c>
+        <v>198</v>
+      </c>
+      <c r="C403" s="1"/>
     </row>
     <row r="404" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A404" s="1">
         <v>403</v>
       </c>
       <c r="B404" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="C404" s="1">
-        <v>1</v>
-      </c>
+        <v>199</v>
+      </c>
+      <c r="C404" s="1"/>
     </row>
     <row r="405" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A405" s="1">
         <v>404</v>
       </c>
       <c r="B405" s="1" t="s">
-        <v>351</v>
+        <v>200</v>
       </c>
       <c r="C405" s="1">
         <v>1</v>
@@ -10470,29 +10289,25 @@
         <v>405</v>
       </c>
       <c r="B406" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="C406" s="1">
-        <v>1</v>
-      </c>
+        <v>201</v>
+      </c>
+      <c r="C406" s="1"/>
     </row>
     <row r="407" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A407" s="1">
         <v>406</v>
       </c>
       <c r="B407" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="C407" s="1">
-        <v>1</v>
-      </c>
+        <v>202</v>
+      </c>
+      <c r="C407" s="1"/>
     </row>
     <row r="408" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A408" s="1">
         <v>407</v>
       </c>
       <c r="B408" s="1" t="s">
-        <v>353</v>
+        <v>203</v>
       </c>
       <c r="C408" s="1">
         <v>1</v>
@@ -10503,7 +10318,7 @@
         <v>408</v>
       </c>
       <c r="B409" s="1" t="s">
-        <v>192</v>
+        <v>205</v>
       </c>
       <c r="C409" s="1"/>
     </row>
@@ -10512,7 +10327,7 @@
         <v>409</v>
       </c>
       <c r="B410" s="1" t="s">
-        <v>193</v>
+        <v>206</v>
       </c>
       <c r="C410" s="1">
         <v>1</v>
@@ -10523,7 +10338,7 @@
         <v>410</v>
       </c>
       <c r="B411" s="1" t="s">
-        <v>236</v>
+        <v>207</v>
       </c>
       <c r="C411" s="1">
         <v>1</v>
@@ -10533,438 +10348,288 @@
       <c r="A412" s="1">
         <v>411</v>
       </c>
-      <c r="B412" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="C412" s="1">
-        <v>1</v>
-      </c>
+      <c r="B412" s="1"/>
+      <c r="C412" s="1"/>
     </row>
     <row r="413" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A413" s="1">
         <v>412</v>
       </c>
-      <c r="B413" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="C413" s="1">
-        <v>1</v>
-      </c>
+      <c r="B413" s="1"/>
+      <c r="C413" s="1"/>
     </row>
     <row r="414" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A414" s="1">
         <v>413</v>
       </c>
-      <c r="B414" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="C414" s="1">
-        <v>1</v>
-      </c>
+      <c r="B414" s="1"/>
+      <c r="C414" s="1"/>
     </row>
     <row r="415" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A415" s="1">
         <v>414</v>
       </c>
-      <c r="B415" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="C415" s="1">
-        <v>1</v>
-      </c>
+      <c r="B415" s="1"/>
+      <c r="C415" s="1"/>
     </row>
     <row r="416" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A416" s="1">
         <v>415</v>
       </c>
-      <c r="B416" s="1" t="s">
-        <v>194</v>
-      </c>
+      <c r="B416" s="1"/>
       <c r="C416" s="1"/>
     </row>
     <row r="417" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A417" s="1">
         <v>416</v>
       </c>
-      <c r="B417" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="C417" s="1">
-        <v>1</v>
-      </c>
+      <c r="B417" s="1"/>
+      <c r="C417" s="1"/>
     </row>
     <row r="418" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A418" s="1">
         <v>417</v>
       </c>
-      <c r="B418" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="C418" s="1">
-        <v>1</v>
-      </c>
+      <c r="B418" s="1"/>
+      <c r="C418" s="1"/>
     </row>
     <row r="419" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A419" s="1">
         <v>418</v>
       </c>
-      <c r="B419" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="C419" s="1">
-        <v>1</v>
-      </c>
+      <c r="B419" s="1"/>
+      <c r="C419" s="1"/>
     </row>
     <row r="420" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A420" s="1">
         <v>419</v>
       </c>
-      <c r="B420" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="C420" s="1">
-        <v>1</v>
-      </c>
+      <c r="B420" s="1"/>
+      <c r="C420" s="1"/>
     </row>
     <row r="421" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A421" s="1">
         <v>420</v>
       </c>
-      <c r="B421" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C421" s="1">
-        <v>1</v>
-      </c>
+      <c r="B421" s="1"/>
+      <c r="C421" s="1"/>
     </row>
     <row r="422" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A422" s="1">
         <v>421</v>
       </c>
-      <c r="B422" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="C422" s="1">
-        <v>1</v>
-      </c>
+      <c r="B422" s="1"/>
+      <c r="C422" s="1"/>
     </row>
     <row r="423" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A423" s="1">
         <v>422</v>
       </c>
-      <c r="B423" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="C423" s="1">
-        <v>1</v>
-      </c>
+      <c r="B423" s="1"/>
+      <c r="C423" s="1"/>
     </row>
     <row r="424" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A424" s="1">
         <v>423</v>
       </c>
-      <c r="B424" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="C424" s="1">
-        <v>1</v>
-      </c>
+      <c r="B424" s="1"/>
+      <c r="C424" s="1"/>
     </row>
     <row r="425" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A425" s="1">
         <v>424</v>
       </c>
-      <c r="B425" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="C425" s="1">
-        <v>1</v>
-      </c>
+      <c r="B425" s="1"/>
+      <c r="C425" s="1"/>
     </row>
     <row r="426" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A426" s="1">
         <v>425</v>
       </c>
-      <c r="B426" s="1" t="s">
-        <v>196</v>
-      </c>
+      <c r="B426" s="1"/>
       <c r="C426" s="1"/>
     </row>
     <row r="427" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A427" s="1">
         <v>426</v>
       </c>
-      <c r="B427" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="C427" s="1">
-        <v>1</v>
-      </c>
+      <c r="B427" s="1"/>
+      <c r="C427" s="1"/>
     </row>
     <row r="428" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A428" s="1">
         <v>427</v>
       </c>
-      <c r="B428" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="C428" s="1">
-        <v>1</v>
-      </c>
+      <c r="B428" s="1"/>
+      <c r="C428" s="1"/>
     </row>
     <row r="429" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A429" s="1">
         <v>428</v>
       </c>
-      <c r="B429" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="C429" s="1">
-        <v>1</v>
-      </c>
+      <c r="B429" s="1"/>
+      <c r="C429" s="1"/>
     </row>
     <row r="430" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A430" s="1">
         <v>429</v>
       </c>
-      <c r="B430" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="C430" s="1">
-        <v>1</v>
-      </c>
+      <c r="B430" s="1"/>
+      <c r="C430" s="1"/>
     </row>
     <row r="431" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A431" s="1">
         <v>430</v>
       </c>
-      <c r="B431" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="C431" s="1">
-        <v>1</v>
-      </c>
+      <c r="B431" s="1"/>
+      <c r="C431" s="1"/>
     </row>
     <row r="432" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A432" s="1">
         <v>431</v>
       </c>
-      <c r="B432" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C432" s="1">
-        <v>1</v>
-      </c>
+      <c r="B432" s="1"/>
+      <c r="C432" s="1"/>
     </row>
     <row r="433" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A433" s="1">
         <v>432</v>
       </c>
-      <c r="B433" s="1" t="s">
-        <v>198</v>
-      </c>
+      <c r="B433" s="1"/>
       <c r="C433" s="1"/>
     </row>
     <row r="434" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A434" s="1">
         <v>433</v>
       </c>
-      <c r="B434" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="C434" s="1">
-        <v>1</v>
-      </c>
+      <c r="B434" s="1"/>
+      <c r="C434" s="1"/>
     </row>
     <row r="435" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A435" s="1">
         <v>434</v>
       </c>
-      <c r="B435" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="C435" s="1">
-        <v>1</v>
-      </c>
+      <c r="B435" s="1"/>
+      <c r="C435" s="1"/>
     </row>
     <row r="436" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A436" s="1">
         <v>435</v>
       </c>
-      <c r="B436" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="C436" s="1">
-        <v>1</v>
-      </c>
+      <c r="B436" s="1"/>
+      <c r="C436" s="1"/>
     </row>
     <row r="437" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A437" s="1">
         <v>436</v>
       </c>
-      <c r="B437" s="1" t="s">
-        <v>199</v>
-      </c>
+      <c r="B437" s="1"/>
       <c r="C437" s="1"/>
     </row>
     <row r="438" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A438" s="1">
         <v>437</v>
       </c>
-      <c r="B438" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="C438" s="1">
-        <v>1</v>
-      </c>
+      <c r="B438" s="1"/>
+      <c r="C438" s="1"/>
     </row>
     <row r="439" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A439" s="1">
         <v>438</v>
       </c>
-      <c r="B439" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="C439" s="1">
-        <v>1</v>
-      </c>
+      <c r="B439" s="1"/>
+      <c r="C439" s="1"/>
     </row>
     <row r="440" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A440" s="1">
         <v>439</v>
       </c>
-      <c r="B440" s="1" t="s">
-        <v>201</v>
-      </c>
+      <c r="B440" s="1"/>
       <c r="C440" s="1"/>
     </row>
     <row r="441" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A441" s="1">
         <v>440</v>
       </c>
-      <c r="B441" s="1" t="s">
-        <v>202</v>
-      </c>
+      <c r="B441" s="1"/>
       <c r="C441" s="1"/>
     </row>
     <row r="442" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A442" s="1">
         <v>441</v>
       </c>
-      <c r="B442" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="C442" s="1">
-        <v>1</v>
-      </c>
+      <c r="B442" s="1"/>
+      <c r="C442" s="1"/>
     </row>
     <row r="443" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A443" s="1">
         <v>442</v>
       </c>
-      <c r="B443" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="C443" s="1">
-        <v>1</v>
-      </c>
+      <c r="B443" s="1"/>
+      <c r="C443" s="1"/>
     </row>
     <row r="444" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A444" s="1">
         <v>443</v>
       </c>
-      <c r="B444" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="C444" s="1">
-        <v>1</v>
-      </c>
+      <c r="B444" s="1"/>
+      <c r="C444" s="1"/>
     </row>
     <row r="445" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A445" s="1">
         <v>444</v>
       </c>
-      <c r="B445" s="1" t="s">
-        <v>205</v>
-      </c>
+      <c r="B445" s="1"/>
       <c r="C445" s="1"/>
     </row>
     <row r="446" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A446" s="1">
         <v>445</v>
       </c>
-      <c r="B446" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="C446" s="1">
-        <v>1</v>
-      </c>
+      <c r="B446" s="1"/>
+      <c r="C446" s="1"/>
     </row>
     <row r="447" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A447" s="1">
         <v>446</v>
       </c>
-      <c r="B447" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="C447" s="1">
-        <v>1</v>
-      </c>
+      <c r="B447" s="1"/>
+      <c r="C447" s="1"/>
     </row>
     <row r="448" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A448" s="1">
         <v>447</v>
       </c>
-      <c r="B448" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="C448" s="1">
-        <v>1</v>
-      </c>
+      <c r="B448" s="1"/>
+      <c r="C448" s="1"/>
     </row>
     <row r="449" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A449" s="1">
         <v>448</v>
       </c>
-      <c r="B449" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="C449" s="1">
-        <v>1</v>
-      </c>
+      <c r="B449" s="1"/>
+      <c r="C449" s="1"/>
     </row>
     <row r="450" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A450" s="1">
         <v>449</v>
       </c>
-      <c r="B450" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="C450" s="1">
-        <v>1</v>
-      </c>
+      <c r="B450" s="1"/>
+      <c r="C450" s="1"/>
     </row>
     <row r="451" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A451" s="1">
         <v>450</v>
       </c>
-      <c r="B451" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="C451" s="1">
-        <v>1</v>
-      </c>
+      <c r="B451" s="1"/>
+      <c r="C451" s="1"/>
     </row>
     <row r="452" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A452" s="1">
         <v>451</v>
       </c>
-      <c r="B452" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="C452" s="1">
-        <v>1</v>
-      </c>
+      <c r="B452" s="1"/>
+      <c r="C452" s="1"/>
     </row>
     <row r="453" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A453" s="1">
@@ -11028,7 +10693,7 @@
         <v>459</v>
       </c>
       <c r="B460" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C460" s="1">
         <v>1</v>
@@ -11050,7 +10715,7 @@
         <v>461</v>
       </c>
       <c r="B462" s="1" t="s">
-        <v>414</v>
+        <v>210</v>
       </c>
       <c r="C462" s="1">
         <v>1</v>
@@ -11061,7 +10726,7 @@
         <v>462</v>
       </c>
       <c r="B463" s="1" t="s">
-        <v>210</v>
+        <v>313</v>
       </c>
       <c r="C463" s="1">
         <v>1</v>
@@ -11072,7 +10737,7 @@
         <v>463</v>
       </c>
       <c r="B464" s="1" t="s">
-        <v>313</v>
+        <v>413</v>
       </c>
       <c r="C464" s="1">
         <v>1</v>
@@ -11105,7 +10770,7 @@
         <v>466</v>
       </c>
       <c r="B467" s="1" t="s">
-        <v>213</v>
+        <v>414</v>
       </c>
       <c r="C467" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
Read any csv as Binder
</commit_message>
<xml_diff>
--- a/data/binder/Binder.xlsx
+++ b/data/binder/Binder.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Dados/MTG/EDH-DeckHelper/data/binder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22936C48-9DF7-134B-BB3F-E9A2E2B78B36}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBEE5188-08B5-5540-9337-B014338478BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="12680" windowHeight="15540" activeTab="1" xr2:uid="{7ABBCC85-5F92-6F41-92E4-65212D317CF6}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="436">
   <si>
     <t>Slot</t>
   </si>
@@ -1304,6 +1304,36 @@
   </si>
   <si>
     <t>Command the Dreadhorde</t>
+  </si>
+  <si>
+    <t>Cabal Coffers</t>
+  </si>
+  <si>
+    <t>Mindcrank</t>
+  </si>
+  <si>
+    <t>Whip of Erebos</t>
+  </si>
+  <si>
+    <t>Whispersilk Cloak</t>
+  </si>
+  <si>
+    <t>Phyrexian Reclamation</t>
+  </si>
+  <si>
+    <t>Vilis, Broker of Blood</t>
+  </si>
+  <si>
+    <t>Temur Battle Rage</t>
+  </si>
+  <si>
+    <t>Fling</t>
+  </si>
+  <si>
+    <t>Chaos Warp</t>
+  </si>
+  <si>
+    <t>Chandra's Ignition</t>
   </si>
 </sst>
 </file>
@@ -6350,8 +6380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5953B7FC-4B75-B146-8A26-6CA09B5F3C99}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A445" workbookViewId="0">
-      <selection activeCell="B470" sqref="B470:C470"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C407" sqref="C407"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6899,7 +6929,9 @@
       <c r="B52" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="C52" s="1"/>
+      <c r="C52" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
@@ -6908,7 +6940,9 @@
       <c r="B53" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="C53" s="1"/>
+      <c r="C53" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
@@ -7583,18 +7617,16 @@
         <v>121</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>415</v>
-      </c>
-      <c r="C122" s="1">
-        <v>1</v>
-      </c>
+        <v>426</v>
+      </c>
+      <c r="C122" s="1"/>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
         <v>122</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>288</v>
+        <v>415</v>
       </c>
       <c r="C123" s="1">
         <v>1</v>
@@ -7604,8 +7636,8 @@
       <c r="A124" s="1">
         <v>123</v>
       </c>
-      <c r="B124" s="2" t="s">
-        <v>69</v>
+      <c r="B124" s="1" t="s">
+        <v>288</v>
       </c>
       <c r="C124" s="1">
         <v>1</v>
@@ -7615,8 +7647,8 @@
       <c r="A125" s="1">
         <v>124</v>
       </c>
-      <c r="B125" s="1" t="s">
-        <v>256</v>
+      <c r="B125" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="C125" s="1">
         <v>1</v>
@@ -7626,8 +7658,8 @@
       <c r="A126" s="1">
         <v>125</v>
       </c>
-      <c r="B126" s="2" t="s">
-        <v>65</v>
+      <c r="B126" s="1" t="s">
+        <v>256</v>
       </c>
       <c r="C126" s="1">
         <v>1</v>
@@ -7638,7 +7670,7 @@
         <v>126</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C127" s="1">
         <v>1</v>
@@ -7649,7 +7681,7 @@
         <v>127</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>397</v>
+        <v>67</v>
       </c>
       <c r="C128" s="1">
         <v>1</v>
@@ -7660,7 +7692,7 @@
         <v>128</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>336</v>
+        <v>397</v>
       </c>
       <c r="C129" s="1">
         <v>1</v>
@@ -7670,8 +7702,8 @@
       <c r="A130" s="1">
         <v>129</v>
       </c>
-      <c r="B130" s="1" t="s">
-        <v>291</v>
+      <c r="B130" s="2" t="s">
+        <v>336</v>
       </c>
       <c r="C130" s="1">
         <v>1</v>
@@ -7682,7 +7714,7 @@
         <v>130</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>70</v>
+        <v>291</v>
       </c>
       <c r="C131" s="1">
         <v>1</v>
@@ -7692,28 +7724,28 @@
       <c r="A132" s="1">
         <v>131</v>
       </c>
-      <c r="B132" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C132" s="1"/>
+      <c r="B132" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C132" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
         <v>132</v>
       </c>
-      <c r="B133" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="C133" s="1">
-        <v>1</v>
-      </c>
+      <c r="B133" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C133" s="1"/>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
         <v>133</v>
       </c>
-      <c r="B134" s="2" t="s">
-        <v>64</v>
+      <c r="B134" s="1" t="s">
+        <v>312</v>
       </c>
       <c r="C134" s="1">
         <v>1</v>
@@ -7724,7 +7756,7 @@
         <v>134</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C135" s="1">
         <v>1</v>
@@ -7734,16 +7766,20 @@
       <c r="A136" s="1">
         <v>135</v>
       </c>
-      <c r="B136" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="C136" s="1"/>
+      <c r="B136" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C136" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
         <v>136</v>
       </c>
-      <c r="B137" s="1"/>
+      <c r="B137" s="1" t="s">
+        <v>250</v>
+      </c>
       <c r="C137" s="1"/>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
@@ -8129,7 +8165,7 @@
         <v>179</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>91</v>
+        <v>427</v>
       </c>
       <c r="C180" s="1">
         <v>1</v>
@@ -8140,7 +8176,7 @@
         <v>180</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C181" s="1">
         <v>1</v>
@@ -8151,7 +8187,7 @@
         <v>181</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C182" s="1">
         <v>1</v>
@@ -8162,7 +8198,7 @@
         <v>182</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>387</v>
+        <v>93</v>
       </c>
       <c r="C183" s="1">
         <v>1</v>
@@ -8173,7 +8209,7 @@
         <v>183</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>416</v>
+        <v>387</v>
       </c>
       <c r="C184" s="1">
         <v>1</v>
@@ -8184,27 +8220,27 @@
         <v>184</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C185" s="1"/>
+        <v>416</v>
+      </c>
+      <c r="C185" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A186" s="1">
         <v>185</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C186" s="1">
-        <v>1</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="C186" s="1"/>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A187" s="1">
         <v>186</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="C187" s="1">
         <v>1</v>
@@ -8215,7 +8251,7 @@
         <v>187</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C188" s="1">
         <v>1</v>
@@ -8226,7 +8262,7 @@
         <v>188</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>388</v>
+        <v>105</v>
       </c>
       <c r="C189" s="1">
         <v>1</v>
@@ -8237,7 +8273,7 @@
         <v>189</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>249</v>
+        <v>388</v>
       </c>
       <c r="C190" s="1">
         <v>1</v>
@@ -8248,7 +8284,7 @@
         <v>190</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>112</v>
+        <v>249</v>
       </c>
       <c r="C191" s="1">
         <v>1</v>
@@ -8259,7 +8295,7 @@
         <v>191</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="C192" s="1">
         <v>1</v>
@@ -8270,7 +8306,7 @@
         <v>192</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C193" s="1">
         <v>1</v>
@@ -8281,7 +8317,7 @@
         <v>193</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="C194" s="1">
         <v>1</v>
@@ -8292,7 +8328,7 @@
         <v>194</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C195" s="1">
         <v>1</v>
@@ -8302,10 +8338,10 @@
       <c r="A196" s="1">
         <v>195</v>
       </c>
-      <c r="B196" s="3" t="s">
-        <v>389</v>
-      </c>
-      <c r="C196" s="3">
+      <c r="B196" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C196" s="1">
         <v>1</v>
       </c>
     </row>
@@ -8313,10 +8349,10 @@
       <c r="A197" s="1">
         <v>196</v>
       </c>
-      <c r="B197" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="C197" s="1">
+      <c r="B197" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="C197" s="3">
         <v>1</v>
       </c>
     </row>
@@ -8325,7 +8361,7 @@
         <v>197</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C198" s="1">
         <v>1</v>
@@ -8336,7 +8372,7 @@
         <v>198</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C199" s="1">
         <v>1</v>
@@ -8347,7 +8383,7 @@
         <v>199</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>99</v>
+        <v>380</v>
       </c>
       <c r="C200" s="1">
         <v>1</v>
@@ -8358,7 +8394,7 @@
         <v>200</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>381</v>
+        <v>99</v>
       </c>
       <c r="C201" s="1">
         <v>1</v>
@@ -8369,7 +8405,7 @@
         <v>201</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>113</v>
+        <v>381</v>
       </c>
       <c r="C202" s="1">
         <v>1</v>
@@ -8380,7 +8416,7 @@
         <v>202</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="C203" s="1">
         <v>1</v>
@@ -8391,7 +8427,7 @@
         <v>203</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="C204" s="1">
         <v>1</v>
@@ -8402,7 +8438,7 @@
         <v>204</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>382</v>
+        <v>114</v>
       </c>
       <c r="C205" s="1">
         <v>1</v>
@@ -8413,7 +8449,7 @@
         <v>205</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>115</v>
+        <v>382</v>
       </c>
       <c r="C206" s="1">
         <v>1</v>
@@ -8424,7 +8460,7 @@
         <v>206</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>285</v>
+        <v>115</v>
       </c>
       <c r="C207" s="1">
         <v>1</v>
@@ -8435,7 +8471,7 @@
         <v>207</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>390</v>
+        <v>285</v>
       </c>
       <c r="C208" s="1">
         <v>1</v>
@@ -8446,7 +8482,7 @@
         <v>208</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C209" s="1">
         <v>1</v>
@@ -8457,7 +8493,7 @@
         <v>209</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C210" s="1">
         <v>1</v>
@@ -8468,7 +8504,7 @@
         <v>210</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>101</v>
+        <v>393</v>
       </c>
       <c r="C211" s="1">
         <v>1</v>
@@ -8479,7 +8515,7 @@
         <v>211</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C212" s="1">
         <v>1</v>
@@ -8490,7 +8526,7 @@
         <v>212</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C213" s="1">
         <v>1</v>
@@ -8500,22 +8536,34 @@
       <c r="A214" s="1">
         <v>213</v>
       </c>
-      <c r="B214" s="1"/>
-      <c r="C214" s="1"/>
+      <c r="B214" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="C214" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A215" s="1">
         <v>214</v>
       </c>
-      <c r="B215" s="1"/>
-      <c r="C215" s="1"/>
+      <c r="B215" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="C215" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A216" s="1">
         <v>215</v>
       </c>
-      <c r="B216" s="1"/>
-      <c r="C216" s="1"/>
+      <c r="B216" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C216" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A217" s="1">
@@ -9554,18 +9602,16 @@
         <v>326</v>
       </c>
       <c r="B327" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="C327" s="1">
-        <v>1</v>
-      </c>
+        <v>431</v>
+      </c>
+      <c r="C327" s="1"/>
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A328" s="1">
         <v>327</v>
       </c>
       <c r="B328" s="1" t="s">
-        <v>245</v>
+        <v>160</v>
       </c>
       <c r="C328" s="1">
         <v>1</v>
@@ -9576,7 +9622,7 @@
         <v>328</v>
       </c>
       <c r="B329" s="1" t="s">
-        <v>161</v>
+        <v>245</v>
       </c>
       <c r="C329" s="1">
         <v>1</v>
@@ -9587,7 +9633,7 @@
         <v>329</v>
       </c>
       <c r="B330" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C330" s="1">
         <v>1</v>
@@ -9598,7 +9644,7 @@
         <v>330</v>
       </c>
       <c r="B331" s="1" t="s">
-        <v>315</v>
+        <v>162</v>
       </c>
       <c r="C331" s="1">
         <v>1</v>
@@ -9609,7 +9655,7 @@
         <v>331</v>
       </c>
       <c r="B332" s="1" t="s">
-        <v>163</v>
+        <v>315</v>
       </c>
       <c r="C332" s="1">
         <v>1</v>
@@ -9620,7 +9666,7 @@
         <v>332</v>
       </c>
       <c r="B333" s="1" t="s">
-        <v>164</v>
+        <v>430</v>
       </c>
       <c r="C333" s="1">
         <v>1</v>
@@ -9631,7 +9677,7 @@
         <v>333</v>
       </c>
       <c r="B334" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C334" s="1">
         <v>1</v>
@@ -9642,16 +9688,18 @@
         <v>334</v>
       </c>
       <c r="B335" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="C335" s="1"/>
+        <v>164</v>
+      </c>
+      <c r="C335" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A336" s="1">
         <v>335</v>
       </c>
       <c r="B336" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C336" s="1">
         <v>1</v>
@@ -9662,18 +9710,16 @@
         <v>336</v>
       </c>
       <c r="B337" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="C337" s="1">
-        <v>1</v>
-      </c>
+        <v>408</v>
+      </c>
+      <c r="C337" s="1"/>
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A338" s="1">
         <v>337</v>
       </c>
       <c r="B338" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C338" s="1">
         <v>1</v>
@@ -9684,7 +9730,7 @@
         <v>338</v>
       </c>
       <c r="B339" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C339" s="1">
         <v>1</v>
@@ -9695,7 +9741,7 @@
         <v>339</v>
       </c>
       <c r="B340" s="1" t="s">
-        <v>425</v>
+        <v>168</v>
       </c>
       <c r="C340" s="1">
         <v>1</v>
@@ -9706,7 +9752,7 @@
         <v>340</v>
       </c>
       <c r="B341" s="1" t="s">
-        <v>314</v>
+        <v>169</v>
       </c>
       <c r="C341" s="1">
         <v>1</v>
@@ -9717,7 +9763,7 @@
         <v>341</v>
       </c>
       <c r="B342" s="1" t="s">
-        <v>170</v>
+        <v>425</v>
       </c>
       <c r="C342" s="1">
         <v>1</v>
@@ -9728,7 +9774,7 @@
         <v>342</v>
       </c>
       <c r="B343" s="1" t="s">
-        <v>171</v>
+        <v>314</v>
       </c>
       <c r="C343" s="1">
         <v>1</v>
@@ -9739,7 +9785,7 @@
         <v>343</v>
       </c>
       <c r="B344" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C344" s="1">
         <v>1</v>
@@ -9750,7 +9796,7 @@
         <v>344</v>
       </c>
       <c r="B345" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C345" s="1">
         <v>1</v>
@@ -9761,25 +9807,29 @@
         <v>345</v>
       </c>
       <c r="B346" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="C346" s="1"/>
+        <v>172</v>
+      </c>
+      <c r="C346" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A347" s="1">
         <v>346</v>
       </c>
       <c r="B347" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="C347" s="1"/>
+        <v>173</v>
+      </c>
+      <c r="C347" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A348" s="1">
         <v>347</v>
       </c>
       <c r="B348" s="1" t="s">
-        <v>423</v>
+        <v>174</v>
       </c>
       <c r="C348" s="1"/>
     </row>
@@ -9788,29 +9838,25 @@
         <v>348</v>
       </c>
       <c r="B349" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C349" s="1">
-        <v>1</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="C349" s="1"/>
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A350" s="1">
         <v>349</v>
       </c>
       <c r="B350" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="C350" s="1">
-        <v>1</v>
-      </c>
+        <v>423</v>
+      </c>
+      <c r="C350" s="1"/>
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A351" s="1">
         <v>350</v>
       </c>
       <c r="B351" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C351" s="1">
         <v>1</v>
@@ -9820,15 +9866,23 @@
       <c r="A352" s="1">
         <v>351</v>
       </c>
-      <c r="B352" s="1"/>
-      <c r="C352" s="1"/>
+      <c r="B352" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C352" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A353" s="1">
         <v>352</v>
       </c>
-      <c r="B353" s="1"/>
-      <c r="C353" s="1"/>
+      <c r="B353" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C353" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A354" s="1">
@@ -9891,7 +9945,7 @@
         <v>361</v>
       </c>
       <c r="B362" s="1" t="s">
-        <v>179</v>
+        <v>434</v>
       </c>
       <c r="C362" s="1">
         <v>1</v>
@@ -9902,7 +9956,7 @@
         <v>362</v>
       </c>
       <c r="B363" s="1" t="s">
-        <v>180</v>
+        <v>433</v>
       </c>
       <c r="C363" s="1">
         <v>1</v>
@@ -9913,7 +9967,7 @@
         <v>363</v>
       </c>
       <c r="B364" s="1" t="s">
-        <v>396</v>
+        <v>179</v>
       </c>
       <c r="C364" s="1">
         <v>1</v>
@@ -9924,7 +9978,7 @@
         <v>364</v>
       </c>
       <c r="B365" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C365" s="1">
         <v>1</v>
@@ -9934,8 +9988,8 @@
       <c r="A366" s="1">
         <v>365</v>
       </c>
-      <c r="B366" s="2" t="s">
-        <v>220</v>
+      <c r="B366" s="1" t="s">
+        <v>432</v>
       </c>
       <c r="C366" s="1">
         <v>1</v>
@@ -9946,7 +10000,7 @@
         <v>366</v>
       </c>
       <c r="B367" s="1" t="s">
-        <v>268</v>
+        <v>396</v>
       </c>
       <c r="C367" s="1">
         <v>1</v>
@@ -9956,37 +10010,53 @@
       <c r="A368" s="1">
         <v>367</v>
       </c>
-      <c r="B368" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="C368" s="1"/>
+      <c r="B368" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="C368" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A369" s="1">
         <v>368</v>
       </c>
-      <c r="B369" s="1"/>
-      <c r="C369" s="1"/>
+      <c r="B369" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C369" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A370" s="1">
         <v>369</v>
       </c>
-      <c r="B370" s="1"/>
-      <c r="C370" s="1"/>
+      <c r="B370" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C370" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A371" s="1">
         <v>370</v>
       </c>
-      <c r="B371" s="1"/>
-      <c r="C371" s="1"/>
+      <c r="B371" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C371" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A372" s="1">
         <v>371</v>
       </c>
-      <c r="B372" s="1"/>
+      <c r="B372" s="2" t="s">
+        <v>222</v>
+      </c>
       <c r="C372" s="1"/>
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.2">
@@ -10291,7 +10361,9 @@
       <c r="B406" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="C406" s="1"/>
+      <c r="C406" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="407" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A407" s="1">

</xml_diff>

<commit_message>
Updating with new decks
</commit_message>
<xml_diff>
--- a/data/binder/Binder.xlsx
+++ b/data/binder/Binder.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Dados/MTG/EDH-DeckHelper/data/binder/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Dados/MTG/EDH DeckHelper/EDH-DeckHelper/data/binder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBEE5188-08B5-5540-9337-B014338478BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF64532-A1A1-7E40-A955-191847BB4317}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="12680" windowHeight="15540" activeTab="1" xr2:uid="{7ABBCC85-5F92-6F41-92E4-65212D317CF6}"/>
   </bookViews>
@@ -6380,8 +6380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5953B7FC-4B75-B146-8A26-6CA09B5F3C99}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C407" sqref="C407"/>
+    <sheetView tabSelected="1" topLeftCell="A451" workbookViewId="0">
+      <selection activeCell="D406" sqref="D406"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7193,7 +7193,9 @@
       <c r="B82" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="C82" s="1"/>
+      <c r="C82" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
@@ -8006,7 +8008,9 @@
       <c r="B165" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="C165" s="1"/>
+      <c r="C165" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
@@ -10341,7 +10345,9 @@
       <c r="B404" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="C404" s="1"/>
+      <c r="C404" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="405" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A405" s="1">

</xml_diff>

<commit_message>
Updated binder and decks
</commit_message>
<xml_diff>
--- a/data/binder/Binder.xlsx
+++ b/data/binder/Binder.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Dados/MTG/EDH DeckHelper/EDH-DeckHelper/data/binder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF64532-A1A1-7E40-A955-191847BB4317}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D35318-3CE3-0E4F-97AA-CD4A77EBB764}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="12680" windowHeight="15540" activeTab="1" xr2:uid="{7ABBCC85-5F92-6F41-92E4-65212D317CF6}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="493">
   <si>
     <t>Slot</t>
   </si>
@@ -1261,96 +1261,260 @@
     <t>Have</t>
   </si>
   <si>
-    <t>Jace, Vryn's Prodigy // Jace, Telepath Unbound</t>
+    <t>Dovin's Veto</t>
+  </si>
+  <si>
+    <t>Lim-Dûl's Vault</t>
+  </si>
+  <si>
+    <t>Cephalid Coliseum</t>
+  </si>
+  <si>
+    <t>Gilded Drake</t>
+  </si>
+  <si>
+    <t>Spellseeker</t>
+  </si>
+  <si>
+    <t>Jace, Wielder of Mysteries</t>
+  </si>
+  <si>
+    <t>Copy Artifact</t>
+  </si>
+  <si>
+    <t>Narset's Reversal</t>
+  </si>
+  <si>
+    <t>Plunge into Darkness</t>
+  </si>
+  <si>
+    <t>Ketria Triome</t>
+  </si>
+  <si>
+    <t>Zagoth Triome</t>
+  </si>
+  <si>
+    <t>Raugrin Triome</t>
+  </si>
+  <si>
+    <t>Indatha Tiome</t>
+  </si>
+  <si>
+    <t>Savai Triome</t>
+  </si>
+  <si>
+    <t>Fabled Passage</t>
+  </si>
+  <si>
+    <t>Emergence Zone</t>
+  </si>
+  <si>
+    <t>Arcane Signet</t>
+  </si>
+  <si>
+    <t>Drannith Magistrate</t>
+  </si>
+  <si>
+    <t>Rest in Peace</t>
+  </si>
+  <si>
+    <t>Consecrated Sphinx</t>
+  </si>
+  <si>
+    <t>Thassa's Oracle</t>
+  </si>
+  <si>
+    <t>Narset, Parter of Veils</t>
+  </si>
+  <si>
+    <t>Fierce Guardianship</t>
+  </si>
+  <si>
+    <t>Force of Negation</t>
+  </si>
+  <si>
+    <t>Winds of Rebuke</t>
+  </si>
+  <si>
+    <t>Razaketh, the Foulblooded</t>
+  </si>
+  <si>
+    <t>Culling the Weak</t>
+  </si>
+  <si>
+    <t>Rain of Filth</t>
+  </si>
+  <si>
+    <t>Dockside Extortionist</t>
+  </si>
+  <si>
+    <t>Underworld Breach</t>
+  </si>
+  <si>
+    <t>Collector Ouphe</t>
+  </si>
+  <si>
+    <t>Oakhame Adversary</t>
+  </si>
+  <si>
+    <t>Runic Armasaur</t>
+  </si>
+  <si>
+    <t>Seedborn Muse</t>
+  </si>
+  <si>
+    <t>Force of Vigor</t>
+  </si>
+  <si>
+    <t>Veil of Summer</t>
+  </si>
+  <si>
+    <t>Finale of Devastation</t>
+  </si>
+  <si>
+    <t>Vexing Shusher</t>
+  </si>
+  <si>
+    <t>Assassin's Trophy</t>
+  </si>
+  <si>
+    <t>Drown in the Loch</t>
+  </si>
+  <si>
+    <t>Neoform</t>
+  </si>
+  <si>
+    <t>Commander's Sphere</t>
+  </si>
+  <si>
+    <t>Elixir of Immortality</t>
+  </si>
+  <si>
+    <t>Mindcrank</t>
+  </si>
+  <si>
+    <t>Skullclamp</t>
+  </si>
+  <si>
+    <t>Urza's Bauble</t>
+  </si>
+  <si>
+    <t>Vanquisher's Banner</t>
+  </si>
+  <si>
+    <t>Whispersilk Cloak</t>
+  </si>
+  <si>
+    <t>Akroma's Memorial</t>
+  </si>
+  <si>
+    <t>Generous Gift</t>
+  </si>
+  <si>
+    <t>Fact or Fiction</t>
+  </si>
+  <si>
+    <t>Mystic Confluence</t>
+  </si>
+  <si>
+    <t>Pull from Tomorrow</t>
+  </si>
+  <si>
+    <t>Doom Whisperer</t>
+  </si>
+  <si>
+    <t>Vilis, Broker of Blood</t>
+  </si>
+  <si>
+    <t>Whip of Erebos</t>
+  </si>
+  <si>
+    <t>Command the Dreadhorde</t>
+  </si>
+  <si>
+    <t>Living Death</t>
+  </si>
+  <si>
+    <t>Glint-Horn Buccaneer</t>
+  </si>
+  <si>
+    <t>Aggravated Assault</t>
+  </si>
+  <si>
+    <t>Chaos Warp</t>
+  </si>
+  <si>
+    <t>Fling</t>
+  </si>
+  <si>
+    <t>Savage Beating</t>
+  </si>
+  <si>
+    <t>Temur Battle Rage</t>
+  </si>
+  <si>
+    <t>Chandra's Ignition</t>
+  </si>
+  <si>
+    <t>Heroic Intervention</t>
+  </si>
+  <si>
+    <t>Garna, the Bloodflame</t>
+  </si>
+  <si>
+    <t>Mirari's Wake</t>
   </si>
   <si>
     <t>Ashiok, Dream Render</t>
   </si>
   <si>
-    <t>Dovin's Veto</t>
-  </si>
-  <si>
-    <t>Lim-Dûl's Vault</t>
-  </si>
-  <si>
-    <t>Cephalid Coliseum</t>
-  </si>
-  <si>
-    <t>Nihil Spellbomb</t>
-  </si>
-  <si>
-    <t>Gilded Drake</t>
-  </si>
-  <si>
-    <t>Sai, Master Thopterist</t>
-  </si>
-  <si>
-    <t>Spellseeker</t>
-  </si>
-  <si>
-    <t>Jace, Wielder of Mysteries</t>
-  </si>
-  <si>
-    <t>Copy Artifact</t>
-  </si>
-  <si>
-    <t>Narset's Reversal</t>
-  </si>
-  <si>
-    <t>Plunge into Darkness</t>
-  </si>
-  <si>
-    <t>Fact or Fiction</t>
-  </si>
-  <si>
-    <t>Command the Dreadhorde</t>
+    <t>Boros Charm</t>
+  </si>
+  <si>
+    <t>Counterflux</t>
+  </si>
+  <si>
+    <t>Rakdos Charm</t>
+  </si>
+  <si>
+    <t>Terminate</t>
+  </si>
+  <si>
+    <t>Mythos of Snapdax</t>
   </si>
   <si>
     <t>Cabal Coffers</t>
   </si>
   <si>
-    <t>Mindcrank</t>
-  </si>
-  <si>
-    <t>Whip of Erebos</t>
-  </si>
-  <si>
-    <t>Whispersilk Cloak</t>
+    <t>Hanweir Battlements</t>
+  </si>
+  <si>
+    <t>Homeward Path</t>
+  </si>
+  <si>
+    <t>Hall of Heliod's Generosity</t>
+  </si>
+  <si>
+    <t>Geier Reach Sanitarium</t>
+  </si>
+  <si>
+    <t>Rogue's Passage</t>
+  </si>
+  <si>
+    <t>Tolaria West</t>
   </si>
   <si>
     <t>Phyrexian Reclamation</t>
-  </si>
-  <si>
-    <t>Vilis, Broker of Blood</t>
-  </si>
-  <si>
-    <t>Temur Battle Rage</t>
-  </si>
-  <si>
-    <t>Fling</t>
-  </si>
-  <si>
-    <t>Chaos Warp</t>
-  </si>
-  <si>
-    <t>Chandra's Ignition</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1402,12 +1566,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1742,10 +1905,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="5"/>
+      <c r="B1" s="4"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1">
         <v>44</v>
@@ -6380,8 +6543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5953B7FC-4B75-B146-8A26-6CA09B5F3C99}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A451" workbookViewId="0">
-      <selection activeCell="D406" sqref="D406"/>
+    <sheetView tabSelected="1" topLeftCell="A445" zoomScale="91" workbookViewId="0">
+      <selection activeCell="D466" sqref="D466"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6451,7 +6614,7 @@
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="1"/>
@@ -6460,7 +6623,7 @@
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="1"/>
@@ -6469,7 +6632,7 @@
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="1"/>
@@ -6478,7 +6641,7 @@
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="1"/>
@@ -6487,7 +6650,7 @@
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="1"/>
@@ -6496,7 +6659,7 @@
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="1">
@@ -6507,7 +6670,7 @@
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="1">
@@ -6518,7 +6681,7 @@
       <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="1">
@@ -6529,7 +6692,7 @@
       <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C15" s="1">
@@ -6540,7 +6703,7 @@
       <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C16" s="1">
@@ -6551,7 +6714,7 @@
       <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C17" s="1">
@@ -6562,7 +6725,7 @@
       <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C18" s="1">
@@ -6573,7 +6736,7 @@
       <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="1">
@@ -6584,7 +6747,7 @@
       <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C20" s="1">
@@ -6595,7 +6758,7 @@
       <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="1">
@@ -6606,7 +6769,7 @@
       <c r="A22" s="1">
         <v>21</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C22" s="1">
@@ -6617,7 +6780,7 @@
       <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C23" s="1">
@@ -6628,7 +6791,7 @@
       <c r="A24" s="1">
         <v>23</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C24" s="1"/>
@@ -6637,7 +6800,7 @@
       <c r="A25" s="1">
         <v>24</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C25" s="1">
@@ -6648,7 +6811,7 @@
       <c r="A26" s="1">
         <v>25</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C26" s="1"/>
@@ -6657,7 +6820,7 @@
       <c r="A27" s="1">
         <v>26</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C27" s="1">
@@ -6668,7 +6831,7 @@
       <c r="A28" s="1">
         <v>27</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C28" s="1">
@@ -6679,7 +6842,7 @@
       <c r="A29" s="1">
         <v>28</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C29" s="1"/>
@@ -6688,7 +6851,7 @@
       <c r="A30" s="1">
         <v>29</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C30" s="1"/>
@@ -6697,7 +6860,7 @@
       <c r="A31" s="1">
         <v>30</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C31" s="1">
@@ -6708,7 +6871,7 @@
       <c r="A32" s="1">
         <v>31</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C32" s="1">
@@ -6719,7 +6882,7 @@
       <c r="A33" s="1">
         <v>32</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C33" s="1">
@@ -6730,7 +6893,7 @@
       <c r="A34" s="1">
         <v>33</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C34" s="1">
@@ -6741,7 +6904,7 @@
       <c r="A35" s="1">
         <v>34</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C35" s="1">
@@ -6752,7 +6915,7 @@
       <c r="A36" s="1">
         <v>35</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C36" s="1">
@@ -6763,7 +6926,7 @@
       <c r="A37" s="1">
         <v>36</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C37" s="1">
@@ -6774,7 +6937,7 @@
       <c r="A38" s="1">
         <v>37</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C38" s="1">
@@ -6785,7 +6948,7 @@
       <c r="A39" s="1">
         <v>38</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C39" s="1"/>
@@ -6794,7 +6957,7 @@
       <c r="A40" s="1">
         <v>39</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C40" s="1">
@@ -6805,7 +6968,7 @@
       <c r="A41" s="1">
         <v>40</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C41" s="1">
@@ -6816,7 +6979,7 @@
       <c r="A42" s="1">
         <v>41</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C42" s="1">
@@ -6827,7 +6990,7 @@
       <c r="A43" s="1">
         <v>42</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C43" s="1">
@@ -6838,7 +7001,7 @@
       <c r="A44" s="1">
         <v>43</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C44" s="1">
@@ -6849,7 +7012,7 @@
       <c r="A45" s="1">
         <v>44</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C45" s="1">
@@ -6860,7 +7023,7 @@
       <c r="A46" s="1">
         <v>45</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C46" s="1">
@@ -6871,7 +7034,7 @@
       <c r="A47" s="1">
         <v>46</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C47" s="1">
@@ -6882,7 +7045,7 @@
       <c r="A48" s="1">
         <v>47</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C48" s="1">
@@ -6893,7 +7056,7 @@
       <c r="A49" s="1">
         <v>48</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C49" s="1">
@@ -6904,7 +7067,7 @@
       <c r="A50" s="1">
         <v>49</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B50" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C50" s="1">
@@ -6915,7 +7078,7 @@
       <c r="A51" s="1">
         <v>50</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C51" s="1">
@@ -6926,7 +7089,7 @@
       <c r="A52" s="1">
         <v>51</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B52" s="1" t="s">
         <v>370</v>
       </c>
       <c r="C52" s="1">
@@ -6937,7 +7100,7 @@
       <c r="A53" s="1">
         <v>52</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B53" s="1" t="s">
         <v>371</v>
       </c>
       <c r="C53" s="1">
@@ -6948,7 +7111,7 @@
       <c r="A54" s="1">
         <v>53</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B54" s="1" t="s">
         <v>372</v>
       </c>
       <c r="C54" s="1"/>
@@ -6957,7 +7120,7 @@
       <c r="A55" s="1">
         <v>54</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B55" s="1" t="s">
         <v>373</v>
       </c>
       <c r="C55" s="1"/>
@@ -6977,42 +7140,42 @@
       <c r="A57" s="1">
         <v>56</v>
       </c>
-      <c r="B57" s="2"/>
+      <c r="B57" s="1"/>
       <c r="C57" s="1"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>57</v>
       </c>
-      <c r="B58" s="2"/>
+      <c r="B58" s="1"/>
       <c r="C58" s="1"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>58</v>
       </c>
-      <c r="B59" s="2"/>
+      <c r="B59" s="1"/>
       <c r="C59" s="1"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>59</v>
       </c>
-      <c r="B60" s="2"/>
+      <c r="B60" s="1"/>
       <c r="C60" s="1"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>60</v>
       </c>
-      <c r="B61" s="2"/>
+      <c r="B61" s="1"/>
       <c r="C61" s="1"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>61</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B62" s="1" t="s">
         <v>53</v>
       </c>
       <c r="C62" s="1"/>
@@ -7021,7 +7184,7 @@
       <c r="A63" s="1">
         <v>62</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B63" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C63" s="1">
@@ -7032,7 +7195,7 @@
       <c r="A64" s="1">
         <v>63</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B64" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C64" s="1">
@@ -7043,7 +7206,7 @@
       <c r="A65" s="1">
         <v>64</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B65" s="1" t="s">
         <v>56</v>
       </c>
       <c r="C65" s="1">
@@ -7054,7 +7217,7 @@
       <c r="A66" s="1">
         <v>65</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B66" s="1" t="s">
         <v>57</v>
       </c>
       <c r="C66" s="1">
@@ -7190,7 +7353,7 @@
       <c r="A82" s="1">
         <v>81</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="B82" s="1" t="s">
         <v>324</v>
       </c>
       <c r="C82" s="1">
@@ -7204,7 +7367,9 @@
       <c r="B83" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="C83" s="1"/>
+      <c r="C83" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
@@ -7213,7 +7378,9 @@
       <c r="B84" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="C84" s="1"/>
+      <c r="C84" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
@@ -7266,7 +7433,9 @@
       <c r="B89" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="C89" s="1"/>
+      <c r="C89" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
@@ -7294,116 +7463,88 @@
       <c r="A92" s="1">
         <v>91</v>
       </c>
-      <c r="B92" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C92" s="1">
-        <v>1</v>
-      </c>
+      <c r="B92" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="C92" s="1"/>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>92</v>
       </c>
-      <c r="B93" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C93" s="1">
-        <v>1</v>
-      </c>
+      <c r="B93" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="C93" s="1"/>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>93</v>
       </c>
-      <c r="B94" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C94" s="1">
-        <v>1</v>
-      </c>
+      <c r="B94" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="C94" s="1"/>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>94</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C95" s="1">
-        <v>1</v>
-      </c>
+        <v>424</v>
+      </c>
+      <c r="C95" s="1"/>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>95</v>
       </c>
-      <c r="B96" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C96" s="1">
-        <v>1</v>
-      </c>
+      <c r="B96" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="C96" s="1"/>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>96</v>
       </c>
-      <c r="B97" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C97" s="1">
-        <v>1</v>
-      </c>
+      <c r="B97" s="1"/>
+      <c r="C97" s="1"/>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>97</v>
       </c>
-      <c r="B98" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C98" s="1">
-        <v>1</v>
-      </c>
+      <c r="B98" s="1"/>
+      <c r="C98" s="1"/>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>98</v>
       </c>
-      <c r="B99" s="2" t="s">
-        <v>78</v>
-      </c>
+      <c r="B99" s="1"/>
       <c r="C99" s="1"/>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>99</v>
       </c>
-      <c r="B100" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="C100" s="1">
-        <v>1</v>
-      </c>
+      <c r="B100" s="1"/>
+      <c r="C100" s="1"/>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>100</v>
       </c>
-      <c r="B101" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="C101" s="1">
-        <v>1</v>
-      </c>
+      <c r="B101" s="1"/>
+      <c r="C101" s="1"/>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>101</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>298</v>
+        <v>73</v>
       </c>
       <c r="C102" s="1">
         <v>1</v>
@@ -7414,7 +7555,7 @@
         <v>102</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>299</v>
+        <v>74</v>
       </c>
       <c r="C103" s="1">
         <v>1</v>
@@ -7425,7 +7566,7 @@
         <v>103</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>301</v>
+        <v>75</v>
       </c>
       <c r="C104" s="1">
         <v>1</v>
@@ -7436,7 +7577,7 @@
         <v>104</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>300</v>
+        <v>79</v>
       </c>
       <c r="C105" s="1">
         <v>1</v>
@@ -7447,7 +7588,7 @@
         <v>105</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>302</v>
+        <v>76</v>
       </c>
       <c r="C106" s="1">
         <v>1</v>
@@ -7458,7 +7599,7 @@
         <v>106</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>303</v>
+        <v>77</v>
       </c>
       <c r="C107" s="1">
         <v>1</v>
@@ -7469,7 +7610,7 @@
         <v>107</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>304</v>
+        <v>80</v>
       </c>
       <c r="C108" s="1">
         <v>1</v>
@@ -7480,27 +7621,27 @@
         <v>108</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="C109" s="1">
-        <v>1</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="C109" s="1"/>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>109</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>402</v>
-      </c>
-      <c r="C110" s="1"/>
+        <v>296</v>
+      </c>
+      <c r="C110" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>110</v>
       </c>
-      <c r="B111" s="2" t="s">
-        <v>322</v>
+      <c r="B111" s="1" t="s">
+        <v>297</v>
       </c>
       <c r="C111" s="1">
         <v>1</v>
@@ -7510,8 +7651,8 @@
       <c r="A112" s="1">
         <v>111</v>
       </c>
-      <c r="B112" s="2" t="s">
-        <v>406</v>
+      <c r="B112" s="1" t="s">
+        <v>298</v>
       </c>
       <c r="C112" s="1">
         <v>1</v>
@@ -7521,8 +7662,8 @@
       <c r="A113" s="1">
         <v>112</v>
       </c>
-      <c r="B113" s="2" t="s">
-        <v>320</v>
+      <c r="B113" s="1" t="s">
+        <v>299</v>
       </c>
       <c r="C113" s="1">
         <v>1</v>
@@ -7532,8 +7673,8 @@
       <c r="A114" s="1">
         <v>113</v>
       </c>
-      <c r="B114" s="2" t="s">
-        <v>59</v>
+      <c r="B114" s="1" t="s">
+        <v>301</v>
       </c>
       <c r="C114" s="1">
         <v>1</v>
@@ -7543,8 +7684,8 @@
       <c r="A115" s="1">
         <v>114</v>
       </c>
-      <c r="B115" s="2" t="s">
-        <v>58</v>
+      <c r="B115" s="1" t="s">
+        <v>300</v>
       </c>
       <c r="C115" s="1">
         <v>1</v>
@@ -7554,8 +7695,8 @@
       <c r="A116" s="1">
         <v>115</v>
       </c>
-      <c r="B116" s="2" t="s">
-        <v>60</v>
+      <c r="B116" s="1" t="s">
+        <v>302</v>
       </c>
       <c r="C116" s="1">
         <v>1</v>
@@ -7565,8 +7706,8 @@
       <c r="A117" s="1">
         <v>116</v>
       </c>
-      <c r="B117" s="2" t="s">
-        <v>61</v>
+      <c r="B117" s="1" t="s">
+        <v>303</v>
       </c>
       <c r="C117" s="1">
         <v>1</v>
@@ -7576,8 +7717,8 @@
       <c r="A118" s="1">
         <v>117</v>
       </c>
-      <c r="B118" s="2" t="s">
-        <v>63</v>
+      <c r="B118" s="1" t="s">
+        <v>304</v>
       </c>
       <c r="C118" s="1">
         <v>1</v>
@@ -7587,8 +7728,8 @@
       <c r="A119" s="1">
         <v>118</v>
       </c>
-      <c r="B119" s="2" t="s">
-        <v>62</v>
+      <c r="B119" s="1" t="s">
+        <v>305</v>
       </c>
       <c r="C119" s="1">
         <v>1</v>
@@ -7598,19 +7739,17 @@
       <c r="A120" s="1">
         <v>119</v>
       </c>
-      <c r="B120" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C120" s="1">
-        <v>1</v>
-      </c>
+      <c r="B120" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="C120" s="1"/>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
         <v>120</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>278</v>
+        <v>402</v>
       </c>
       <c r="C121" s="1"/>
     </row>
@@ -7619,16 +7758,18 @@
         <v>121</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>426</v>
-      </c>
-      <c r="C122" s="1"/>
+        <v>322</v>
+      </c>
+      <c r="C122" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
         <v>122</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
       <c r="C123" s="1">
         <v>1</v>
@@ -7639,7 +7780,7 @@
         <v>123</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>288</v>
+        <v>320</v>
       </c>
       <c r="C124" s="1">
         <v>1</v>
@@ -7649,8 +7790,8 @@
       <c r="A125" s="1">
         <v>124</v>
       </c>
-      <c r="B125" s="2" t="s">
-        <v>69</v>
+      <c r="B125" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="C125" s="1">
         <v>1</v>
@@ -7661,7 +7802,7 @@
         <v>125</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>256</v>
+        <v>58</v>
       </c>
       <c r="C126" s="1">
         <v>1</v>
@@ -7671,8 +7812,8 @@
       <c r="A127" s="1">
         <v>126</v>
       </c>
-      <c r="B127" s="2" t="s">
-        <v>65</v>
+      <c r="B127" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="C127" s="1">
         <v>1</v>
@@ -7682,8 +7823,8 @@
       <c r="A128" s="1">
         <v>127</v>
       </c>
-      <c r="B128" s="2" t="s">
-        <v>67</v>
+      <c r="B128" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="C128" s="1">
         <v>1</v>
@@ -7693,8 +7834,8 @@
       <c r="A129" s="1">
         <v>128</v>
       </c>
-      <c r="B129" s="2" t="s">
-        <v>397</v>
+      <c r="B129" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="C129" s="1">
         <v>1</v>
@@ -7704,8 +7845,8 @@
       <c r="A130" s="1">
         <v>129</v>
       </c>
-      <c r="B130" s="2" t="s">
-        <v>336</v>
+      <c r="B130" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="C130" s="1">
         <v>1</v>
@@ -7716,18 +7857,16 @@
         <v>130</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="C131" s="1">
-        <v>1</v>
-      </c>
+        <v>278</v>
+      </c>
+      <c r="C131" s="1"/>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
         <v>131</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C132" s="1">
         <v>1</v>
@@ -7737,28 +7876,28 @@
       <c r="A133" s="1">
         <v>132</v>
       </c>
-      <c r="B133" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C133" s="1"/>
+      <c r="B133" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C133" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
         <v>133</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="C134" s="1">
-        <v>1</v>
-      </c>
+        <v>485</v>
+      </c>
+      <c r="C134" s="1"/>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
         <v>134</v>
       </c>
-      <c r="B135" s="2" t="s">
-        <v>64</v>
+      <c r="B135" s="1" t="s">
+        <v>413</v>
       </c>
       <c r="C135" s="1">
         <v>1</v>
@@ -7768,8 +7907,8 @@
       <c r="A136" s="1">
         <v>135</v>
       </c>
-      <c r="B136" s="2" t="s">
-        <v>66</v>
+      <c r="B136" s="1" t="s">
+        <v>288</v>
       </c>
       <c r="C136" s="1">
         <v>1</v>
@@ -7780,121 +7919,187 @@
         <v>136</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="C137" s="1"/>
+        <v>426</v>
+      </c>
+      <c r="C137" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
         <v>137</v>
       </c>
-      <c r="B138" s="1"/>
-      <c r="C138" s="1"/>
+      <c r="B138" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C138" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
         <v>138</v>
       </c>
-      <c r="B139" s="1"/>
-      <c r="C139" s="1"/>
+      <c r="B139" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C139" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" s="1">
         <v>139</v>
       </c>
-      <c r="B140" s="1"/>
-      <c r="C140" s="1"/>
+      <c r="B140" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="C140" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
         <v>140</v>
       </c>
-      <c r="B141" s="1"/>
-      <c r="C141" s="1"/>
+      <c r="B141" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C141" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
         <v>141</v>
       </c>
-      <c r="B142" s="1"/>
-      <c r="C142" s="1"/>
+      <c r="B142" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="C142" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
         <v>142</v>
       </c>
-      <c r="B143" s="1"/>
-      <c r="C143" s="1"/>
+      <c r="B143" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="C143" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
         <v>143</v>
       </c>
-      <c r="B144" s="1"/>
-      <c r="C144" s="1"/>
+      <c r="B144" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="C144" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
         <v>144</v>
       </c>
-      <c r="B145" s="1"/>
-      <c r="C145" s="1"/>
+      <c r="B145" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="C145" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
         <v>145</v>
       </c>
-      <c r="B146" s="1"/>
-      <c r="C146" s="1"/>
+      <c r="B146" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C146" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
         <v>146</v>
       </c>
-      <c r="B147" s="1"/>
-      <c r="C147" s="1"/>
+      <c r="B147" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="C147" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
         <v>147</v>
       </c>
-      <c r="B148" s="1"/>
-      <c r="C148" s="1"/>
+      <c r="B148" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C148" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
         <v>148</v>
       </c>
-      <c r="B149" s="1"/>
-      <c r="C149" s="1"/>
+      <c r="B149" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C149" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" s="1">
         <v>149</v>
       </c>
-      <c r="B150" s="1"/>
-      <c r="C150" s="1"/>
+      <c r="B150" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="C150" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" s="1">
         <v>150</v>
       </c>
-      <c r="B151" s="1"/>
-      <c r="C151" s="1"/>
+      <c r="B151" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C151" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" s="1">
         <v>151</v>
       </c>
-      <c r="B152" s="1"/>
-      <c r="C152" s="1"/>
+      <c r="B152" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="C152" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" s="1">
         <v>152</v>
       </c>
-      <c r="B153" s="1"/>
-      <c r="C153" s="1"/>
+      <c r="B153" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C153" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" s="1">
@@ -7929,7 +8134,7 @@
         <v>157</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>81</v>
+        <v>459</v>
       </c>
       <c r="C158" s="1">
         <v>1</v>
@@ -7940,7 +8145,7 @@
         <v>158</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>107</v>
+        <v>427</v>
       </c>
       <c r="C159" s="1">
         <v>1</v>
@@ -7951,7 +8156,7 @@
         <v>159</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C160" s="1">
         <v>1</v>
@@ -7962,7 +8167,7 @@
         <v>160</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>374</v>
+        <v>104</v>
       </c>
       <c r="C161" s="1">
         <v>1</v>
@@ -7973,7 +8178,7 @@
         <v>161</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>82</v>
+        <v>374</v>
       </c>
       <c r="C162" s="1">
         <v>1</v>
@@ -7984,7 +8189,7 @@
         <v>162</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>225</v>
+        <v>82</v>
       </c>
       <c r="C163" s="1">
         <v>1</v>
@@ -7995,7 +8200,7 @@
         <v>163</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>83</v>
+        <v>452</v>
       </c>
       <c r="C164" s="1">
         <v>1</v>
@@ -8006,7 +8211,7 @@
         <v>164</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>280</v>
+        <v>225</v>
       </c>
       <c r="C165" s="1">
         <v>1</v>
@@ -8017,7 +8222,7 @@
         <v>165</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C166" s="1">
         <v>1</v>
@@ -8028,7 +8233,7 @@
         <v>166</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>376</v>
+        <v>453</v>
       </c>
       <c r="C167" s="1">
         <v>1</v>
@@ -8039,7 +8244,7 @@
         <v>167</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>108</v>
+        <v>280</v>
       </c>
       <c r="C168" s="1">
         <v>1</v>
@@ -8050,7 +8255,7 @@
         <v>168</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>227</v>
+        <v>84</v>
       </c>
       <c r="C169" s="1">
         <v>1</v>
@@ -8061,7 +8266,7 @@
         <v>169</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>85</v>
+        <v>376</v>
       </c>
       <c r="C170" s="1">
         <v>1</v>
@@ -8072,7 +8277,7 @@
         <v>170</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C171" s="1">
         <v>1</v>
@@ -8083,7 +8288,7 @@
         <v>171</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>384</v>
+        <v>227</v>
       </c>
       <c r="C172" s="1">
         <v>1</v>
@@ -8094,7 +8299,7 @@
         <v>172</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C173" s="1">
         <v>1</v>
@@ -8105,7 +8310,7 @@
         <v>173</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C174" s="1">
         <v>1</v>
@@ -8116,7 +8321,7 @@
         <v>174</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C175" s="1">
         <v>1</v>
@@ -8127,16 +8332,18 @@
         <v>175</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C176" s="1"/>
+        <v>86</v>
+      </c>
+      <c r="C176" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
         <v>176</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>88</v>
+        <v>110</v>
       </c>
       <c r="C177" s="1">
         <v>1</v>
@@ -8147,7 +8354,7 @@
         <v>177</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>89</v>
+        <v>385</v>
       </c>
       <c r="C178" s="1">
         <v>1</v>
@@ -8158,18 +8365,16 @@
         <v>178</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C179" s="1">
-        <v>1</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="C179" s="1"/>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A180" s="1">
         <v>179</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>427</v>
+        <v>88</v>
       </c>
       <c r="C180" s="1">
         <v>1</v>
@@ -8180,7 +8385,7 @@
         <v>180</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C181" s="1">
         <v>1</v>
@@ -8191,7 +8396,7 @@
         <v>181</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C182" s="1">
         <v>1</v>
@@ -8202,7 +8407,7 @@
         <v>182</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C183" s="1">
         <v>1</v>
@@ -8213,7 +8418,7 @@
         <v>183</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>387</v>
+        <v>454</v>
       </c>
       <c r="C184" s="1">
         <v>1</v>
@@ -8224,7 +8429,7 @@
         <v>184</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>416</v>
+        <v>92</v>
       </c>
       <c r="C185" s="1">
         <v>1</v>
@@ -8235,16 +8440,18 @@
         <v>185</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C186" s="1"/>
+        <v>93</v>
+      </c>
+      <c r="C186" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A187" s="1">
         <v>186</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>111</v>
+        <v>387</v>
       </c>
       <c r="C187" s="1">
         <v>1</v>
@@ -8255,7 +8462,7 @@
         <v>187</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="C188" s="1">
         <v>1</v>
@@ -8332,7 +8539,7 @@
         <v>194</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>97</v>
+        <v>455</v>
       </c>
       <c r="C195" s="1">
         <v>1</v>
@@ -8343,7 +8550,7 @@
         <v>195</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C196" s="1">
         <v>1</v>
@@ -8353,10 +8560,10 @@
       <c r="A197" s="1">
         <v>196</v>
       </c>
-      <c r="B197" s="3" t="s">
+      <c r="B197" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="C197" s="3">
+      <c r="C197" s="1">
         <v>1</v>
       </c>
     </row>
@@ -8519,18 +8726,16 @@
         <v>211</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C212" s="1">
-        <v>1</v>
-      </c>
+        <v>456</v>
+      </c>
+      <c r="C212" s="1"/>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A213" s="1">
         <v>212</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>102</v>
+        <v>457</v>
       </c>
       <c r="C213" s="1">
         <v>1</v>
@@ -8541,7 +8746,7 @@
         <v>213</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>428</v>
+        <v>101</v>
       </c>
       <c r="C214" s="1">
         <v>1</v>
@@ -8552,7 +8757,7 @@
         <v>214</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>429</v>
+        <v>458</v>
       </c>
       <c r="C215" s="1">
         <v>1</v>
@@ -8563,7 +8768,7 @@
         <v>215</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C216" s="1">
         <v>1</v>
@@ -8573,8 +8778,12 @@
       <c r="A217" s="1">
         <v>216</v>
       </c>
-      <c r="B217" s="1"/>
-      <c r="C217" s="1"/>
+      <c r="B217" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C217" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A218" s="1">
@@ -8657,7 +8866,7 @@
       <c r="A229" s="1">
         <v>228</v>
       </c>
-      <c r="B229" s="2"/>
+      <c r="B229" s="1"/>
       <c r="C229" s="1"/>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.2">
@@ -8676,18 +8885,16 @@
         <v>230</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C231" s="1">
-        <v>1</v>
-      </c>
+        <v>428</v>
+      </c>
+      <c r="C231" s="1"/>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A232" s="1">
         <v>231</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>272</v>
+        <v>116</v>
       </c>
       <c r="C232" s="1">
         <v>1</v>
@@ -8698,7 +8905,7 @@
         <v>232</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="C233" s="1">
         <v>1</v>
@@ -8709,7 +8916,7 @@
         <v>233</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>261</v>
+        <v>272</v>
       </c>
       <c r="C234" s="1">
         <v>1</v>
@@ -8720,7 +8927,7 @@
         <v>234</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>340</v>
+        <v>260</v>
       </c>
       <c r="C235" s="1">
         <v>1</v>
@@ -8731,7 +8938,7 @@
         <v>235</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>289</v>
+        <v>261</v>
       </c>
       <c r="C236" s="1">
         <v>1</v>
@@ -8742,7 +8949,7 @@
         <v>236</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>248</v>
+        <v>262</v>
       </c>
       <c r="C237" s="1">
         <v>1</v>
@@ -8753,7 +8960,7 @@
         <v>237</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>405</v>
+        <v>265</v>
       </c>
       <c r="C238" s="1">
         <v>1</v>
@@ -8764,7 +8971,7 @@
         <v>238</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>310</v>
+        <v>340</v>
       </c>
       <c r="C239" s="1">
         <v>1</v>
@@ -8775,7 +8982,7 @@
         <v>239</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>118</v>
+        <v>289</v>
       </c>
       <c r="C240" s="1">
         <v>1</v>
@@ -8786,7 +8993,7 @@
         <v>240</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>119</v>
+        <v>248</v>
       </c>
       <c r="C241" s="1">
         <v>1</v>
@@ -8797,7 +9004,7 @@
         <v>241</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>120</v>
+        <v>429</v>
       </c>
       <c r="C242" s="1">
         <v>1</v>
@@ -8808,7 +9015,7 @@
         <v>242</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>252</v>
+        <v>405</v>
       </c>
       <c r="C243" s="1">
         <v>1</v>
@@ -8819,7 +9026,7 @@
         <v>243</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>251</v>
+        <v>310</v>
       </c>
       <c r="C244" s="1">
         <v>1</v>
@@ -8829,43 +9036,67 @@
       <c r="A245" s="1">
         <v>244</v>
       </c>
-      <c r="B245" s="1"/>
-      <c r="C245" s="1"/>
+      <c r="B245" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C245" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A246" s="1">
         <v>245</v>
       </c>
-      <c r="B246" s="1"/>
-      <c r="C246" s="1"/>
+      <c r="B246" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="C246" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A247" s="1">
         <v>246</v>
       </c>
-      <c r="B247" s="1"/>
-      <c r="C247" s="1"/>
+      <c r="B247" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C247" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A248" s="1">
         <v>247</v>
       </c>
-      <c r="B248" s="1"/>
-      <c r="C248" s="1"/>
+      <c r="B248" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C248" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A249" s="1">
         <v>248</v>
       </c>
-      <c r="B249" s="1"/>
-      <c r="C249" s="1"/>
+      <c r="B249" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C249" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A250" s="1">
         <v>249</v>
       </c>
-      <c r="B250" s="1"/>
-      <c r="C250" s="1"/>
+      <c r="B250" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C250" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A251" s="1">
@@ -8977,7 +9208,7 @@
         <v>265</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="C266" s="1">
         <v>1</v>
@@ -8988,16 +9219,18 @@
         <v>266</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>417</v>
-      </c>
-      <c r="C267" s="1"/>
+        <v>430</v>
+      </c>
+      <c r="C267" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A268" s="1">
         <v>267</v>
       </c>
       <c r="B268" s="1" t="s">
-        <v>411</v>
+        <v>226</v>
       </c>
       <c r="C268" s="1">
         <v>1</v>
@@ -9008,20 +9241,20 @@
         <v>268</v>
       </c>
       <c r="B269" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C269" s="1">
-        <v>1</v>
-      </c>
+        <v>414</v>
+      </c>
+      <c r="C269" s="1"/>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A270" s="1">
         <v>269</v>
       </c>
-      <c r="B270" s="4" t="s">
-        <v>418</v>
-      </c>
-      <c r="C270" s="1"/>
+      <c r="B270" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C270" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A271" s="1">
@@ -9039,7 +9272,7 @@
         <v>271</v>
       </c>
       <c r="B272" s="1" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="C272" s="1">
         <v>1</v>
@@ -9050,7 +9283,7 @@
         <v>272</v>
       </c>
       <c r="B273" s="1" t="s">
-        <v>123</v>
+        <v>431</v>
       </c>
       <c r="C273" s="1">
         <v>1</v>
@@ -9061,7 +9294,7 @@
         <v>273</v>
       </c>
       <c r="B274" s="1" t="s">
-        <v>420</v>
+        <v>123</v>
       </c>
       <c r="C274" s="1">
         <v>1</v>
@@ -9072,7 +9305,7 @@
         <v>274</v>
       </c>
       <c r="B275" s="1" t="s">
-        <v>284</v>
+        <v>416</v>
       </c>
       <c r="C275" s="1">
         <v>1</v>
@@ -9083,18 +9316,16 @@
         <v>275</v>
       </c>
       <c r="B276" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="C276" s="1">
-        <v>1</v>
-      </c>
+        <v>432</v>
+      </c>
+      <c r="C276" s="1"/>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A277" s="1">
         <v>276</v>
       </c>
       <c r="B277" s="1" t="s">
-        <v>124</v>
+        <v>284</v>
       </c>
       <c r="C277" s="1">
         <v>1</v>
@@ -9105,7 +9336,7 @@
         <v>277</v>
       </c>
       <c r="B278" s="1" t="s">
-        <v>283</v>
+        <v>223</v>
       </c>
       <c r="C278" s="1">
         <v>1</v>
@@ -9116,18 +9347,16 @@
         <v>278</v>
       </c>
       <c r="B279" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="C279" s="1">
-        <v>1</v>
-      </c>
+        <v>417</v>
+      </c>
+      <c r="C279" s="1"/>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A280" s="1">
         <v>279</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C280" s="1">
         <v>1</v>
@@ -9138,7 +9367,7 @@
         <v>280</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>126</v>
+        <v>283</v>
       </c>
       <c r="C281" s="1">
         <v>1</v>
@@ -9149,7 +9378,7 @@
         <v>281</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>127</v>
+        <v>394</v>
       </c>
       <c r="C282" s="1">
         <v>1</v>
@@ -9160,7 +9389,7 @@
         <v>282</v>
       </c>
       <c r="B283" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C283" s="1">
         <v>1</v>
@@ -9171,7 +9400,7 @@
         <v>283</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C284" s="1">
         <v>1</v>
@@ -9182,7 +9411,7 @@
         <v>284</v>
       </c>
       <c r="B285" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C285" s="1">
         <v>1</v>
@@ -9193,7 +9422,7 @@
         <v>285</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C286" s="1">
         <v>1</v>
@@ -9204,7 +9433,7 @@
         <v>286</v>
       </c>
       <c r="B287" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C287" s="1">
         <v>1</v>
@@ -9215,7 +9444,7 @@
         <v>287</v>
       </c>
       <c r="B288" s="1" t="s">
-        <v>424</v>
+        <v>130</v>
       </c>
       <c r="C288" s="1">
         <v>1</v>
@@ -9226,7 +9455,7 @@
         <v>288</v>
       </c>
       <c r="B289" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C289" s="1">
         <v>1</v>
@@ -9237,7 +9466,7 @@
         <v>289</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C290" s="1">
         <v>1</v>
@@ -9248,7 +9477,7 @@
         <v>290</v>
       </c>
       <c r="B291" s="1" t="s">
-        <v>135</v>
+        <v>461</v>
       </c>
       <c r="C291" s="1">
         <v>1</v>
@@ -9259,18 +9488,16 @@
         <v>291</v>
       </c>
       <c r="B292" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C292" s="1">
-        <v>1</v>
-      </c>
+        <v>433</v>
+      </c>
+      <c r="C292" s="1"/>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A293" s="1">
         <v>292</v>
       </c>
       <c r="B293" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C293" s="1">
         <v>1</v>
@@ -9281,18 +9508,16 @@
         <v>293</v>
       </c>
       <c r="B294" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C294" s="1">
-        <v>1</v>
-      </c>
+        <v>434</v>
+      </c>
+      <c r="C294" s="1"/>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A295" s="1">
         <v>294</v>
       </c>
       <c r="B295" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C295" s="1">
         <v>1</v>
@@ -9303,7 +9528,7 @@
         <v>295</v>
       </c>
       <c r="B296" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C296" s="1">
         <v>1</v>
@@ -9314,7 +9539,7 @@
         <v>296</v>
       </c>
       <c r="B297" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C297" s="1">
         <v>1</v>
@@ -9325,7 +9550,7 @@
         <v>297</v>
       </c>
       <c r="B298" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C298" s="1">
         <v>1</v>
@@ -9336,7 +9561,7 @@
         <v>298</v>
       </c>
       <c r="B299" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C299" s="1">
         <v>1</v>
@@ -9347,7 +9572,7 @@
         <v>299</v>
       </c>
       <c r="B300" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C300" s="1">
         <v>1</v>
@@ -9358,7 +9583,7 @@
         <v>300</v>
       </c>
       <c r="B301" s="1" t="s">
-        <v>422</v>
+        <v>142</v>
       </c>
       <c r="C301" s="1">
         <v>1</v>
@@ -9369,7 +9594,7 @@
         <v>301</v>
       </c>
       <c r="B302" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C302" s="1">
         <v>1</v>
@@ -9380,7 +9605,7 @@
         <v>302</v>
       </c>
       <c r="B303" s="1" t="s">
-        <v>306</v>
+        <v>462</v>
       </c>
       <c r="C303" s="1">
         <v>1</v>
@@ -9391,7 +9616,7 @@
         <v>303</v>
       </c>
       <c r="B304" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C304" s="1">
         <v>1</v>
@@ -9402,7 +9627,7 @@
         <v>304</v>
       </c>
       <c r="B305" s="1" t="s">
-        <v>147</v>
+        <v>418</v>
       </c>
       <c r="C305" s="1">
         <v>1</v>
@@ -9413,7 +9638,7 @@
         <v>305</v>
       </c>
       <c r="B306" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C306" s="1">
         <v>1</v>
@@ -9424,16 +9649,18 @@
         <v>306</v>
       </c>
       <c r="B307" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="C307" s="1"/>
+        <v>306</v>
+      </c>
+      <c r="C307" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A308" s="1">
         <v>307</v>
       </c>
       <c r="B308" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C308" s="1">
         <v>1</v>
@@ -9444,7 +9671,7 @@
         <v>308</v>
       </c>
       <c r="B309" s="1" t="s">
-        <v>151</v>
+        <v>463</v>
       </c>
       <c r="C309" s="1">
         <v>1</v>
@@ -9455,7 +9682,7 @@
         <v>309</v>
       </c>
       <c r="B310" s="1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C310" s="1">
         <v>1</v>
@@ -9466,7 +9693,7 @@
         <v>310</v>
       </c>
       <c r="B311" s="1" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C311" s="1">
         <v>1</v>
@@ -9477,7 +9704,7 @@
         <v>311</v>
       </c>
       <c r="B312" s="1" t="s">
-        <v>154</v>
+        <v>287</v>
       </c>
       <c r="C312" s="1">
         <v>1</v>
@@ -9488,7 +9715,7 @@
         <v>312</v>
       </c>
       <c r="B313" s="1" t="s">
-        <v>221</v>
+        <v>435</v>
       </c>
       <c r="C313" s="1">
         <v>1</v>
@@ -9499,7 +9726,7 @@
         <v>313</v>
       </c>
       <c r="B314" s="1" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C314" s="1">
         <v>1</v>
@@ -9510,25 +9737,29 @@
         <v>314</v>
       </c>
       <c r="B315" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C315" s="1"/>
+        <v>151</v>
+      </c>
+      <c r="C315" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A316" s="1">
         <v>315</v>
       </c>
       <c r="B316" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C316" s="1"/>
+        <v>152</v>
+      </c>
+      <c r="C316" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A317" s="1">
         <v>316</v>
       </c>
       <c r="B317" s="1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C317" s="1">
         <v>1</v>
@@ -9538,43 +9769,63 @@
       <c r="A318" s="1">
         <v>317</v>
       </c>
-      <c r="B318" s="1"/>
-      <c r="C318" s="1"/>
+      <c r="B318" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C318" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A319" s="1">
         <v>318</v>
       </c>
-      <c r="B319" s="1"/>
-      <c r="C319" s="1"/>
+      <c r="B319" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C319" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A320" s="1">
         <v>319</v>
       </c>
-      <c r="B320" s="1"/>
-      <c r="C320" s="1"/>
+      <c r="B320" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C320" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A321" s="1">
         <v>320</v>
       </c>
-      <c r="B321" s="1"/>
+      <c r="B321" s="1" t="s">
+        <v>156</v>
+      </c>
       <c r="C321" s="1"/>
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A322" s="1">
         <v>321</v>
       </c>
-      <c r="B322" s="1"/>
+      <c r="B322" s="1" t="s">
+        <v>157</v>
+      </c>
       <c r="C322" s="1"/>
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A323" s="1">
         <v>322</v>
       </c>
-      <c r="B323" s="1"/>
-      <c r="C323" s="1"/>
+      <c r="B323" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C323" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A324" s="1">
@@ -9594,128 +9845,84 @@
       <c r="A326" s="1">
         <v>325</v>
       </c>
-      <c r="B326" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="C326" s="1">
-        <v>1</v>
-      </c>
+      <c r="B326" s="1"/>
+      <c r="C326" s="1"/>
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A327" s="1">
         <v>326</v>
       </c>
-      <c r="B327" s="1" t="s">
-        <v>431</v>
-      </c>
+      <c r="B327" s="1"/>
       <c r="C327" s="1"/>
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A328" s="1">
         <v>327</v>
       </c>
-      <c r="B328" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="C328" s="1">
-        <v>1</v>
-      </c>
+      <c r="B328" s="1"/>
+      <c r="C328" s="1"/>
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A329" s="1">
         <v>328</v>
       </c>
-      <c r="B329" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="C329" s="1">
-        <v>1</v>
-      </c>
+      <c r="B329" s="1"/>
+      <c r="C329" s="1"/>
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A330" s="1">
         <v>329</v>
       </c>
-      <c r="B330" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="C330" s="1">
-        <v>1</v>
-      </c>
+      <c r="B330" s="1"/>
+      <c r="C330" s="1"/>
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A331" s="1">
         <v>330</v>
       </c>
-      <c r="B331" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C331" s="1">
-        <v>1</v>
-      </c>
+      <c r="B331" s="1"/>
+      <c r="C331" s="1"/>
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A332" s="1">
         <v>331</v>
       </c>
-      <c r="B332" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="C332" s="1">
-        <v>1</v>
-      </c>
+      <c r="B332" s="1"/>
+      <c r="C332" s="1"/>
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A333" s="1">
         <v>332</v>
       </c>
-      <c r="B333" s="1" t="s">
-        <v>430</v>
-      </c>
-      <c r="C333" s="1">
-        <v>1</v>
-      </c>
+      <c r="B333" s="1"/>
+      <c r="C333" s="1"/>
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A334" s="1">
         <v>333</v>
       </c>
-      <c r="B334" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C334" s="1">
-        <v>1</v>
-      </c>
+      <c r="B334" s="1"/>
+      <c r="C334" s="1"/>
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A335" s="1">
         <v>334</v>
       </c>
-      <c r="B335" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C335" s="1">
-        <v>1</v>
-      </c>
+      <c r="B335" s="1"/>
+      <c r="C335" s="1"/>
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A336" s="1">
         <v>335</v>
       </c>
-      <c r="B336" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C336" s="1">
-        <v>1</v>
-      </c>
+      <c r="B336" s="1"/>
+      <c r="C336" s="1"/>
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A337" s="1">
         <v>336</v>
       </c>
-      <c r="B337" s="1" t="s">
-        <v>408</v>
-      </c>
+      <c r="B337" s="1"/>
       <c r="C337" s="1"/>
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.2">
@@ -9723,7 +9930,7 @@
         <v>337</v>
       </c>
       <c r="B338" s="1" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="C338" s="1">
         <v>1</v>
@@ -9734,7 +9941,7 @@
         <v>338</v>
       </c>
       <c r="B339" s="1" t="s">
-        <v>167</v>
+        <v>464</v>
       </c>
       <c r="C339" s="1">
         <v>1</v>
@@ -9745,7 +9952,7 @@
         <v>339</v>
       </c>
       <c r="B340" s="1" t="s">
-        <v>168</v>
+        <v>436</v>
       </c>
       <c r="C340" s="1">
         <v>1</v>
@@ -9756,18 +9963,16 @@
         <v>340</v>
       </c>
       <c r="B341" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="C341" s="1">
-        <v>1</v>
-      </c>
+        <v>465</v>
+      </c>
+      <c r="C341" s="1"/>
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A342" s="1">
         <v>341</v>
       </c>
       <c r="B342" s="1" t="s">
-        <v>425</v>
+        <v>160</v>
       </c>
       <c r="C342" s="1">
         <v>1</v>
@@ -9778,7 +9983,7 @@
         <v>342</v>
       </c>
       <c r="B343" s="1" t="s">
-        <v>314</v>
+        <v>245</v>
       </c>
       <c r="C343" s="1">
         <v>1</v>
@@ -9789,7 +9994,7 @@
         <v>343</v>
       </c>
       <c r="B344" s="1" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="C344" s="1">
         <v>1</v>
@@ -9800,7 +10005,7 @@
         <v>344</v>
       </c>
       <c r="B345" s="1" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="C345" s="1">
         <v>1</v>
@@ -9810,10 +10015,10 @@
       <c r="A346" s="1">
         <v>345</v>
       </c>
-      <c r="B346" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="C346" s="1">
+      <c r="B346" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="C346" s="3">
         <v>1</v>
       </c>
     </row>
@@ -9822,7 +10027,7 @@
         <v>346</v>
       </c>
       <c r="B347" s="1" t="s">
-        <v>173</v>
+        <v>466</v>
       </c>
       <c r="C347" s="1">
         <v>1</v>
@@ -9833,25 +10038,29 @@
         <v>347</v>
       </c>
       <c r="B348" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="C348" s="1"/>
+        <v>163</v>
+      </c>
+      <c r="C348" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A349" s="1">
         <v>348</v>
       </c>
       <c r="B349" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="C349" s="1"/>
+        <v>164</v>
+      </c>
+      <c r="C349" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A350" s="1">
         <v>349</v>
       </c>
       <c r="B350" s="1" t="s">
-        <v>423</v>
+        <v>437</v>
       </c>
       <c r="C350" s="1"/>
     </row>
@@ -9860,7 +10069,7 @@
         <v>350</v>
       </c>
       <c r="B351" s="1" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="C351" s="1">
         <v>1</v>
@@ -9871,18 +10080,16 @@
         <v>351</v>
       </c>
       <c r="B352" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="C352" s="1">
-        <v>1</v>
-      </c>
+        <v>408</v>
+      </c>
+      <c r="C352" s="1"/>
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A353" s="1">
         <v>352</v>
       </c>
       <c r="B353" s="1" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="C353" s="1">
         <v>1</v>
@@ -9892,64 +10099,94 @@
       <c r="A354" s="1">
         <v>353</v>
       </c>
-      <c r="B354" s="1"/>
+      <c r="B354" s="1" t="s">
+        <v>419</v>
+      </c>
       <c r="C354" s="1"/>
     </row>
     <row r="355" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A355" s="1">
         <v>354</v>
       </c>
-      <c r="B355" s="1"/>
-      <c r="C355" s="1"/>
+      <c r="B355" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="C355" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="356" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A356" s="1">
         <v>355</v>
       </c>
-      <c r="B356" s="1"/>
-      <c r="C356" s="1"/>
+      <c r="B356" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C356" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="357" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A357" s="1">
         <v>356</v>
       </c>
-      <c r="B357" s="1"/>
-      <c r="C357" s="1"/>
+      <c r="B357" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C357" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="358" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A358" s="1">
         <v>357</v>
       </c>
-      <c r="B358" s="1"/>
-      <c r="C358" s="1"/>
+      <c r="B358" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C358" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="359" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A359" s="1">
         <v>358</v>
       </c>
-      <c r="B359" s="1"/>
-      <c r="C359" s="1"/>
+      <c r="B359" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="C359" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A360" s="1">
         <v>359</v>
       </c>
-      <c r="B360" s="1"/>
-      <c r="C360" s="1"/>
+      <c r="B360" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C360" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="361" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A361" s="1">
         <v>360</v>
       </c>
-      <c r="B361" s="1"/>
-      <c r="C361" s="1"/>
+      <c r="B361" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C361" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="362" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A362" s="1">
         <v>361</v>
       </c>
       <c r="B362" s="1" t="s">
-        <v>434</v>
+        <v>171</v>
       </c>
       <c r="C362" s="1">
         <v>1</v>
@@ -9960,7 +10197,7 @@
         <v>362</v>
       </c>
       <c r="B363" s="1" t="s">
-        <v>433</v>
+        <v>172</v>
       </c>
       <c r="C363" s="1">
         <v>1</v>
@@ -9971,18 +10208,16 @@
         <v>363</v>
       </c>
       <c r="B364" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="C364" s="1">
-        <v>1</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="C364" s="1"/>
     </row>
     <row r="365" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A365" s="1">
         <v>364</v>
       </c>
       <c r="B365" s="1" t="s">
-        <v>180</v>
+        <v>468</v>
       </c>
       <c r="C365" s="1">
         <v>1</v>
@@ -9993,7 +10228,7 @@
         <v>365</v>
       </c>
       <c r="B366" s="1" t="s">
-        <v>432</v>
+        <v>334</v>
       </c>
       <c r="C366" s="1">
         <v>1</v>
@@ -10004,7 +10239,7 @@
         <v>366</v>
       </c>
       <c r="B367" s="1" t="s">
-        <v>396</v>
+        <v>176</v>
       </c>
       <c r="C367" s="1">
         <v>1</v>
@@ -10015,7 +10250,7 @@
         <v>367</v>
       </c>
       <c r="B368" s="1" t="s">
-        <v>435</v>
+        <v>177</v>
       </c>
       <c r="C368" s="1">
         <v>1</v>
@@ -10026,7 +10261,7 @@
         <v>368</v>
       </c>
       <c r="B369" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C369" s="1">
         <v>1</v>
@@ -10036,31 +10271,21 @@
       <c r="A370" s="1">
         <v>369</v>
       </c>
-      <c r="B370" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="C370" s="1">
-        <v>1</v>
-      </c>
+      <c r="B370" s="1"/>
+      <c r="C370" s="1"/>
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A371" s="1">
         <v>370</v>
       </c>
-      <c r="B371" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="C371" s="1">
-        <v>1</v>
-      </c>
+      <c r="B371" s="1"/>
+      <c r="C371" s="1"/>
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A372" s="1">
         <v>371</v>
       </c>
-      <c r="B372" s="2" t="s">
-        <v>222</v>
-      </c>
+      <c r="B372" s="1"/>
       <c r="C372" s="1"/>
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.2">
@@ -10074,92 +10299,136 @@
       <c r="A374" s="1">
         <v>373</v>
       </c>
-      <c r="B374" s="1"/>
+      <c r="B374" s="1" t="s">
+        <v>439</v>
+      </c>
       <c r="C374" s="1"/>
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A375" s="1">
         <v>374</v>
       </c>
-      <c r="B375" s="1"/>
-      <c r="C375" s="1"/>
+      <c r="B375" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="C375" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A376" s="1">
         <v>375</v>
       </c>
-      <c r="B376" s="1"/>
-      <c r="C376" s="1"/>
+      <c r="B376" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C376" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A377" s="1">
         <v>376</v>
       </c>
-      <c r="B377" s="1"/>
-      <c r="C377" s="1"/>
+      <c r="B377" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="C377" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A378" s="1">
         <v>377</v>
       </c>
-      <c r="B378" s="1"/>
-      <c r="C378" s="1"/>
+      <c r="B378" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C378" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A379" s="1">
         <v>378</v>
       </c>
-      <c r="B379" s="1"/>
+      <c r="B379" s="1" t="s">
+        <v>440</v>
+      </c>
       <c r="C379" s="1"/>
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A380" s="1">
         <v>379</v>
       </c>
-      <c r="B380" s="1"/>
-      <c r="C380" s="1"/>
+      <c r="B380" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="C380" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A381" s="1">
         <v>380</v>
       </c>
-      <c r="B381" s="1"/>
-      <c r="C381" s="1"/>
+      <c r="B381" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="C381" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A382" s="1">
         <v>381</v>
       </c>
-      <c r="B382" s="1"/>
-      <c r="C382" s="1"/>
+      <c r="B382" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C382" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A383" s="1">
         <v>382</v>
       </c>
-      <c r="B383" s="1"/>
-      <c r="C383" s="1"/>
+      <c r="B383" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C383" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="384" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A384" s="1">
         <v>383</v>
       </c>
-      <c r="B384" s="1"/>
-      <c r="C384" s="1"/>
+      <c r="B384" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="C384" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="385" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A385" s="1">
         <v>384</v>
       </c>
-      <c r="B385" s="1"/>
-      <c r="C385" s="1"/>
+      <c r="B385" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="C385" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="386" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A386" s="1">
         <v>385</v>
       </c>
       <c r="B386" s="1" t="s">
-        <v>182</v>
+        <v>396</v>
       </c>
       <c r="C386" s="1">
         <v>1</v>
@@ -10170,7 +10439,7 @@
         <v>386</v>
       </c>
       <c r="B387" s="1" t="s">
-        <v>183</v>
+        <v>218</v>
       </c>
       <c r="C387" s="1">
         <v>1</v>
@@ -10181,25 +10450,29 @@
         <v>387</v>
       </c>
       <c r="B388" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C388" s="1"/>
+        <v>475</v>
+      </c>
+      <c r="C388" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="389" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A389" s="1">
         <v>388</v>
       </c>
       <c r="B389" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="C389" s="1"/>
+        <v>339</v>
+      </c>
+      <c r="C389" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="390" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A390" s="1">
         <v>389</v>
       </c>
       <c r="B390" s="1" t="s">
-        <v>204</v>
+        <v>181</v>
       </c>
       <c r="C390" s="1">
         <v>1</v>
@@ -10210,7 +10483,7 @@
         <v>390</v>
       </c>
       <c r="B391" s="1" t="s">
-        <v>186</v>
+        <v>220</v>
       </c>
       <c r="C391" s="1">
         <v>1</v>
@@ -10221,7 +10494,7 @@
         <v>391</v>
       </c>
       <c r="B392" s="1" t="s">
-        <v>187</v>
+        <v>268</v>
       </c>
       <c r="C392" s="1">
         <v>1</v>
@@ -10232,7 +10505,7 @@
         <v>392</v>
       </c>
       <c r="B393" s="1" t="s">
-        <v>188</v>
+        <v>222</v>
       </c>
       <c r="C393" s="1"/>
     </row>
@@ -10240,164 +10513,112 @@
       <c r="A394" s="1">
         <v>393</v>
       </c>
-      <c r="B394" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="C394" s="1">
-        <v>1</v>
-      </c>
+      <c r="B394" s="1"/>
+      <c r="C394" s="1"/>
     </row>
     <row r="395" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A395" s="1">
         <v>394</v>
       </c>
-      <c r="B395" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="C395" s="1">
-        <v>1</v>
-      </c>
+      <c r="B395" s="1"/>
+      <c r="C395" s="1"/>
     </row>
     <row r="396" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A396" s="1">
         <v>395</v>
       </c>
-      <c r="B396" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="C396" s="1">
-        <v>1</v>
-      </c>
+      <c r="B396" s="1"/>
+      <c r="C396" s="1"/>
     </row>
     <row r="397" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A397" s="1">
         <v>396</v>
       </c>
-      <c r="B397" s="1" t="s">
-        <v>192</v>
-      </c>
+      <c r="B397" s="1"/>
       <c r="C397" s="1"/>
     </row>
     <row r="398" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A398" s="1">
         <v>397</v>
       </c>
-      <c r="B398" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="C398" s="1">
-        <v>1</v>
-      </c>
+      <c r="B398" s="1"/>
+      <c r="C398" s="1"/>
     </row>
     <row r="399" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A399" s="1">
         <v>398</v>
       </c>
-      <c r="B399" s="1" t="s">
-        <v>194</v>
-      </c>
+      <c r="B399" s="1"/>
       <c r="C399" s="1"/>
     </row>
     <row r="400" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A400" s="1">
         <v>399</v>
       </c>
-      <c r="B400" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C400" s="1">
-        <v>1</v>
-      </c>
+      <c r="B400" s="1"/>
+      <c r="C400" s="1"/>
     </row>
     <row r="401" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A401" s="1">
         <v>400</v>
       </c>
-      <c r="B401" s="1" t="s">
-        <v>196</v>
-      </c>
+      <c r="B401" s="1"/>
       <c r="C401" s="1"/>
     </row>
     <row r="402" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A402" s="1">
         <v>401</v>
       </c>
-      <c r="B402" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C402" s="1">
-        <v>1</v>
-      </c>
+      <c r="B402" s="1"/>
+      <c r="C402" s="1"/>
     </row>
     <row r="403" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A403" s="1">
         <v>402</v>
       </c>
-      <c r="B403" s="1" t="s">
-        <v>198</v>
-      </c>
+      <c r="B403" s="1"/>
       <c r="C403" s="1"/>
     </row>
     <row r="404" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A404" s="1">
         <v>403</v>
       </c>
-      <c r="B404" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="C404" s="1">
-        <v>1</v>
-      </c>
+      <c r="B404" s="1"/>
+      <c r="C404" s="1"/>
     </row>
     <row r="405" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A405" s="1">
         <v>404</v>
       </c>
-      <c r="B405" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="C405" s="1">
-        <v>1</v>
-      </c>
+      <c r="B405" s="1"/>
+      <c r="C405" s="1"/>
     </row>
     <row r="406" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A406" s="1">
         <v>405</v>
       </c>
-      <c r="B406" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C406" s="1">
-        <v>1</v>
-      </c>
+      <c r="B406" s="1"/>
+      <c r="C406" s="1"/>
     </row>
     <row r="407" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A407" s="1">
         <v>406</v>
       </c>
-      <c r="B407" s="1" t="s">
-        <v>202</v>
-      </c>
+      <c r="B407" s="1"/>
       <c r="C407" s="1"/>
     </row>
     <row r="408" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A408" s="1">
         <v>407</v>
       </c>
-      <c r="B408" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="C408" s="1">
-        <v>1</v>
-      </c>
+      <c r="B408" s="1"/>
+      <c r="C408" s="1"/>
     </row>
     <row r="409" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A409" s="1">
         <v>408</v>
       </c>
-      <c r="B409" s="1" t="s">
-        <v>205</v>
-      </c>
+      <c r="B409" s="1"/>
       <c r="C409" s="1"/>
     </row>
     <row r="410" spans="1:3" x14ac:dyDescent="0.2">
@@ -10405,7 +10626,7 @@
         <v>409</v>
       </c>
       <c r="B410" s="1" t="s">
-        <v>206</v>
+        <v>182</v>
       </c>
       <c r="C410" s="1">
         <v>1</v>
@@ -10416,7 +10637,7 @@
         <v>410</v>
       </c>
       <c r="B411" s="1" t="s">
-        <v>207</v>
+        <v>183</v>
       </c>
       <c r="C411" s="1">
         <v>1</v>
@@ -10426,246 +10647,362 @@
       <c r="A412" s="1">
         <v>411</v>
       </c>
-      <c r="B412" s="1"/>
+      <c r="B412" s="1" t="s">
+        <v>184</v>
+      </c>
       <c r="C412" s="1"/>
     </row>
     <row r="413" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A413" s="1">
         <v>412</v>
       </c>
-      <c r="B413" s="1"/>
+      <c r="B413" s="1" t="s">
+        <v>185</v>
+      </c>
       <c r="C413" s="1"/>
     </row>
     <row r="414" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A414" s="1">
         <v>413</v>
       </c>
-      <c r="B414" s="1"/>
-      <c r="C414" s="1"/>
+      <c r="B414" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C414" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="415" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A415" s="1">
         <v>414</v>
       </c>
-      <c r="B415" s="1"/>
-      <c r="C415" s="1"/>
+      <c r="B415" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="C415" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="416" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A416" s="1">
         <v>415</v>
       </c>
-      <c r="B416" s="1"/>
-      <c r="C416" s="1"/>
+      <c r="B416" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C416" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="417" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A417" s="1">
         <v>416</v>
       </c>
-      <c r="B417" s="1"/>
-      <c r="C417" s="1"/>
+      <c r="B417" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C417" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="418" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A418" s="1">
         <v>417</v>
       </c>
-      <c r="B418" s="1"/>
-      <c r="C418" s="1"/>
+      <c r="B418" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C418" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="419" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A419" s="1">
         <v>418</v>
       </c>
-      <c r="B419" s="1"/>
-      <c r="C419" s="1"/>
+      <c r="B419" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C419" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="420" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A420" s="1">
         <v>419</v>
       </c>
-      <c r="B420" s="1"/>
-      <c r="C420" s="1"/>
+      <c r="B420" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C420" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="421" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A421" s="1">
         <v>420</v>
       </c>
-      <c r="B421" s="1"/>
+      <c r="B421" s="1" t="s">
+        <v>192</v>
+      </c>
       <c r="C421" s="1"/>
     </row>
     <row r="422" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A422" s="1">
         <v>421</v>
       </c>
-      <c r="B422" s="1"/>
+      <c r="B422" s="1" t="s">
+        <v>442</v>
+      </c>
       <c r="C422" s="1"/>
     </row>
     <row r="423" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A423" s="1">
         <v>422</v>
       </c>
-      <c r="B423" s="1"/>
-      <c r="C423" s="1"/>
+      <c r="B423" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C423" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="424" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A424" s="1">
         <v>423</v>
       </c>
-      <c r="B424" s="1"/>
-      <c r="C424" s="1"/>
+      <c r="B424" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C424" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="425" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A425" s="1">
         <v>424</v>
       </c>
-      <c r="B425" s="1"/>
-      <c r="C425" s="1"/>
+      <c r="B425" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C425" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="426" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A426" s="1">
         <v>425</v>
       </c>
-      <c r="B426" s="1"/>
+      <c r="B426" s="1" t="s">
+        <v>443</v>
+      </c>
       <c r="C426" s="1"/>
     </row>
     <row r="427" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A427" s="1">
         <v>426</v>
       </c>
-      <c r="B427" s="1"/>
-      <c r="C427" s="1"/>
+      <c r="B427" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="C427" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="428" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A428" s="1">
         <v>427</v>
       </c>
-      <c r="B428" s="1"/>
+      <c r="B428" s="1" t="s">
+        <v>196</v>
+      </c>
       <c r="C428" s="1"/>
     </row>
     <row r="429" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A429" s="1">
         <v>428</v>
       </c>
-      <c r="B429" s="1"/>
-      <c r="C429" s="1"/>
+      <c r="B429" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C429" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="430" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A430" s="1">
         <v>429</v>
       </c>
-      <c r="B430" s="1"/>
+      <c r="B430" s="1" t="s">
+        <v>198</v>
+      </c>
       <c r="C430" s="1"/>
     </row>
     <row r="431" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A431" s="1">
         <v>430</v>
       </c>
-      <c r="B431" s="1"/>
-      <c r="C431" s="1"/>
+      <c r="B431" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="C431" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="432" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A432" s="1">
         <v>431</v>
       </c>
-      <c r="B432" s="1"/>
-      <c r="C432" s="1"/>
+      <c r="B432" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="C432" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="433" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A433" s="1">
         <v>432</v>
       </c>
-      <c r="B433" s="1"/>
-      <c r="C433" s="1"/>
+      <c r="B433" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C433" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="434" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A434" s="1">
         <v>433</v>
       </c>
-      <c r="B434" s="1"/>
-      <c r="C434" s="1"/>
+      <c r="B434" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C434" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="435" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A435" s="1">
         <v>434</v>
       </c>
-      <c r="B435" s="1"/>
-      <c r="C435" s="1"/>
+      <c r="B435" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C435" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="436" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A436" s="1">
         <v>435</v>
       </c>
-      <c r="B436" s="1"/>
+      <c r="B436" s="1" t="s">
+        <v>445</v>
+      </c>
       <c r="C436" s="1"/>
     </row>
     <row r="437" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A437" s="1">
         <v>436</v>
       </c>
-      <c r="B437" s="1"/>
-      <c r="C437" s="1"/>
+      <c r="B437" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="C437" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="438" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A438" s="1">
         <v>437</v>
       </c>
-      <c r="B438" s="1"/>
-      <c r="C438" s="1"/>
+      <c r="B438" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C438" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="439" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A439" s="1">
         <v>438</v>
       </c>
-      <c r="B439" s="1"/>
+      <c r="B439" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="C439" s="1"/>
     </row>
     <row r="440" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A440" s="1">
         <v>439</v>
       </c>
-      <c r="B440" s="1"/>
-      <c r="C440" s="1"/>
+      <c r="B440" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C440" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="441" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A441" s="1">
         <v>440</v>
       </c>
-      <c r="B441" s="1"/>
+      <c r="B441" s="1" t="s">
+        <v>446</v>
+      </c>
       <c r="C441" s="1"/>
     </row>
     <row r="442" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A442" s="1">
         <v>441</v>
       </c>
-      <c r="B442" s="1"/>
-      <c r="C442" s="1"/>
+      <c r="B442" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C442" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="443" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A443" s="1">
         <v>442</v>
       </c>
-      <c r="B443" s="1"/>
+      <c r="B443" s="1" t="s">
+        <v>205</v>
+      </c>
       <c r="C443" s="1"/>
     </row>
     <row r="444" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A444" s="1">
         <v>443</v>
       </c>
-      <c r="B444" s="1"/>
+      <c r="B444" s="1" t="s">
+        <v>447</v>
+      </c>
       <c r="C444" s="1"/>
     </row>
     <row r="445" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A445" s="1">
         <v>444</v>
       </c>
-      <c r="B445" s="1"/>
-      <c r="C445" s="1"/>
+      <c r="B445" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C445" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="446" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A446" s="1">
         <v>445</v>
       </c>
-      <c r="B446" s="1"/>
-      <c r="C446" s="1"/>
+      <c r="B446" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C446" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="447" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A447" s="1">
@@ -10760,7 +11097,7 @@
         <v>458</v>
       </c>
       <c r="B459" s="1" t="s">
-        <v>209</v>
+        <v>477</v>
       </c>
       <c r="C459" s="1">
         <v>1</v>
@@ -10771,7 +11108,7 @@
         <v>459</v>
       </c>
       <c r="B460" s="1" t="s">
-        <v>412</v>
+        <v>209</v>
       </c>
       <c r="C460" s="1">
         <v>1</v>
@@ -10782,18 +11119,16 @@
         <v>460</v>
       </c>
       <c r="B461" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="C461" s="1">
-        <v>1</v>
-      </c>
+        <v>448</v>
+      </c>
+      <c r="C461" s="1"/>
     </row>
     <row r="462" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A462" s="1">
         <v>461</v>
       </c>
       <c r="B462" s="1" t="s">
-        <v>210</v>
+        <v>479</v>
       </c>
       <c r="C462" s="1">
         <v>1</v>
@@ -10804,7 +11139,7 @@
         <v>462</v>
       </c>
       <c r="B463" s="1" t="s">
-        <v>313</v>
+        <v>279</v>
       </c>
       <c r="C463" s="1">
         <v>1</v>
@@ -10815,18 +11150,16 @@
         <v>463</v>
       </c>
       <c r="B464" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="C464" s="1">
-        <v>1</v>
-      </c>
+        <v>478</v>
+      </c>
+      <c r="C464" s="1"/>
     </row>
     <row r="465" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A465" s="1">
         <v>464</v>
       </c>
       <c r="B465" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C465" s="1">
         <v>1</v>
@@ -10836,10 +11169,10 @@
       <c r="A466" s="1">
         <v>465</v>
       </c>
-      <c r="B466" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="C466" s="1">
+      <c r="B466" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="C466" s="3">
         <v>1</v>
       </c>
     </row>
@@ -10848,18 +11181,16 @@
         <v>466</v>
       </c>
       <c r="B467" s="1" t="s">
-        <v>414</v>
-      </c>
-      <c r="C467" s="1">
-        <v>1</v>
-      </c>
+        <v>449</v>
+      </c>
+      <c r="C467" s="1"/>
     </row>
     <row r="468" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A468" s="1">
         <v>467</v>
       </c>
       <c r="B468" s="1" t="s">
-        <v>247</v>
+        <v>480</v>
       </c>
       <c r="C468" s="1">
         <v>1</v>
@@ -10870,7 +11201,7 @@
         <v>468</v>
       </c>
       <c r="B469" s="1" t="s">
-        <v>292</v>
+        <v>481</v>
       </c>
       <c r="C469" s="1">
         <v>1</v>
@@ -10880,78 +11211,116 @@
       <c r="A470" s="1">
         <v>469</v>
       </c>
-      <c r="B470" s="1"/>
-      <c r="C470" s="1"/>
+      <c r="B470" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="C470" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="471" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A471" s="1">
         <v>470</v>
       </c>
-      <c r="B471" s="1"/>
+      <c r="B471" s="1" t="s">
+        <v>450</v>
+      </c>
       <c r="C471" s="1"/>
     </row>
     <row r="472" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A472" s="1">
         <v>471</v>
       </c>
-      <c r="B472" s="1"/>
-      <c r="C472" s="1"/>
+      <c r="B472" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C472" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="473" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A473" s="1">
         <v>472</v>
       </c>
-      <c r="B473" s="1"/>
-      <c r="C473" s="1"/>
+      <c r="B473" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C473" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="474" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A474" s="1">
         <v>473</v>
       </c>
-      <c r="B474" s="1"/>
-      <c r="C474" s="1"/>
+      <c r="B474" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="C474" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="475" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A475" s="1">
         <v>474</v>
       </c>
-      <c r="B475" s="1"/>
-      <c r="C475" s="1"/>
+      <c r="B475" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="C475" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="476" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A476" s="1">
         <v>475</v>
       </c>
-      <c r="B476" s="1"/>
-      <c r="C476" s="1"/>
+      <c r="B476" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="C476" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="477" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A477" s="1">
         <v>476</v>
       </c>
-      <c r="B477" s="1"/>
-      <c r="C477" s="1"/>
+      <c r="B477" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C477" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="478" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A478" s="1">
         <v>477</v>
       </c>
-      <c r="B478" s="1"/>
+      <c r="B478" s="1" t="s">
+        <v>484</v>
+      </c>
       <c r="C478" s="1"/>
     </row>
     <row r="479" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A479" s="1">
         <v>478</v>
       </c>
-      <c r="B479" s="1"/>
+      <c r="B479" s="1" t="s">
+        <v>451</v>
+      </c>
       <c r="C479" s="1"/>
     </row>
     <row r="480" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A480" s="1">
         <v>479</v>
       </c>
-      <c r="B480" s="1"/>
-      <c r="C480" s="1"/>
+      <c r="B480" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C480" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="481" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A481" s="1">

</xml_diff>

<commit_message>
Updated binder and lists
</commit_message>
<xml_diff>
--- a/data/binder/Binder.xlsx
+++ b/data/binder/Binder.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Dados/MTG/EDH DeckHelper/EDH-DeckHelper/data/binder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D35318-3CE3-0E4F-97AA-CD4A77EBB764}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2B86FA7-ADB5-5645-BA82-B2EF12696D52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="12680" windowHeight="15540" activeTab="1" xr2:uid="{7ABBCC85-5F92-6F41-92E4-65212D317CF6}"/>
   </bookViews>
@@ -6543,8 +6543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5953B7FC-4B75-B146-8A26-6CA09B5F3C99}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A445" zoomScale="91" workbookViewId="0">
-      <selection activeCell="D466" sqref="D466"/>
+    <sheetView tabSelected="1" topLeftCell="A396" zoomScale="91" workbookViewId="0">
+      <selection activeCell="B480" sqref="B480:C480"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7114,7 +7114,9 @@
       <c r="B54" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="C54" s="1"/>
+      <c r="C54" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
@@ -7123,7 +7125,9 @@
       <c r="B55" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="C55" s="1"/>
+      <c r="C55" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
@@ -7493,7 +7497,9 @@
       <c r="B95" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="C95" s="1"/>
+      <c r="C95" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
@@ -7502,7 +7508,9 @@
       <c r="B96" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="C96" s="1"/>
+      <c r="C96" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
@@ -8728,7 +8736,9 @@
       <c r="B212" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="C212" s="1"/>
+      <c r="C212" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A213" s="1">
@@ -8887,7 +8897,9 @@
       <c r="B231" s="1" t="s">
         <v>428</v>
       </c>
-      <c r="C231" s="1"/>
+      <c r="C231" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A232" s="1">
@@ -9092,7 +9104,7 @@
         <v>249</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>251</v>
+        <v>484</v>
       </c>
       <c r="C250" s="1">
         <v>1</v>
@@ -9102,8 +9114,12 @@
       <c r="A251" s="1">
         <v>250</v>
       </c>
-      <c r="B251" s="1"/>
-      <c r="C251" s="1"/>
+      <c r="B251" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C251" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A252" s="1">
@@ -9490,7 +9506,9 @@
       <c r="B292" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="C292" s="1"/>
+      <c r="C292" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A293" s="1">
@@ -9965,7 +9983,9 @@
       <c r="B341" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="C341" s="1"/>
+      <c r="C341" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A342" s="1">
@@ -10650,7 +10670,9 @@
       <c r="B412" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="C412" s="1"/>
+      <c r="C412" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="413" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A413" s="1">
@@ -10816,7 +10838,9 @@
       <c r="B428" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="C428" s="1"/>
+      <c r="C428" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="429" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A429" s="1">
@@ -10971,7 +10995,9 @@
       <c r="B443" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="C443" s="1"/>
+      <c r="C443" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="444" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A444" s="1">
@@ -11152,7 +11178,9 @@
       <c r="B464" s="1" t="s">
         <v>478</v>
       </c>
-      <c r="C464" s="1"/>
+      <c r="C464" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="465" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A465" s="1">
@@ -11298,7 +11326,7 @@
         <v>477</v>
       </c>
       <c r="B478" s="1" t="s">
-        <v>484</v>
+        <v>451</v>
       </c>
       <c r="C478" s="1"/>
     </row>
@@ -11307,20 +11335,18 @@
         <v>478</v>
       </c>
       <c r="B479" s="1" t="s">
-        <v>451</v>
-      </c>
-      <c r="C479" s="1"/>
+        <v>292</v>
+      </c>
+      <c r="C479" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="480" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A480" s="1">
         <v>479</v>
       </c>
-      <c r="B480" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="C480" s="1">
-        <v>1</v>
-      </c>
+      <c r="B480" s="1"/>
+      <c r="C480" s="1"/>
     </row>
     <row r="481" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A481" s="1">

</xml_diff>

<commit_message>
Function '0' now adds cards that are in core but not in binder
</commit_message>
<xml_diff>
--- a/data/binder/Binder.xlsx
+++ b/data/binder/Binder.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Dados/MTG/EDH DeckHelper/EDH-DeckHelper/data/binder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2B86FA7-ADB5-5645-BA82-B2EF12696D52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF631B81-8AA6-E346-9F2A-B4792229CDF7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="12680" windowHeight="15540" activeTab="1" xr2:uid="{7ABBCC85-5F92-6F41-92E4-65212D317CF6}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="486">
   <si>
     <t>Slot</t>
   </si>
@@ -1318,9 +1318,6 @@
     <t>Rest in Peace</t>
   </si>
   <si>
-    <t>Consecrated Sphinx</t>
-  </si>
-  <si>
     <t>Thassa's Oracle</t>
   </si>
   <si>
@@ -1336,9 +1333,6 @@
     <t>Winds of Rebuke</t>
   </si>
   <si>
-    <t>Razaketh, the Foulblooded</t>
-  </si>
-  <si>
     <t>Culling the Weak</t>
   </si>
   <si>
@@ -1354,15 +1348,6 @@
     <t>Collector Ouphe</t>
   </si>
   <si>
-    <t>Oakhame Adversary</t>
-  </si>
-  <si>
-    <t>Runic Armasaur</t>
-  </si>
-  <si>
-    <t>Seedborn Muse</t>
-  </si>
-  <si>
     <t>Force of Vigor</t>
   </si>
   <si>
@@ -1372,13 +1357,7 @@
     <t>Finale of Devastation</t>
   </si>
   <si>
-    <t>Vexing Shusher</t>
-  </si>
-  <si>
     <t>Assassin's Trophy</t>
-  </si>
-  <si>
-    <t>Drown in the Loch</t>
   </si>
   <si>
     <t>Neoform</t>
@@ -6543,8 +6522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5953B7FC-4B75-B146-8A26-6CA09B5F3C99}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A396" zoomScale="91" workbookViewId="0">
-      <selection activeCell="B480" sqref="B480:C480"/>
+    <sheetView tabSelected="1" topLeftCell="A416" zoomScale="91" workbookViewId="0">
+      <selection activeCell="B427" sqref="B427:C427"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7896,7 +7875,7 @@
         <v>133</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>485</v>
+        <v>478</v>
       </c>
       <c r="C134" s="1"/>
     </row>
@@ -7960,7 +7939,7 @@
         <v>139</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>489</v>
+        <v>482</v>
       </c>
       <c r="C140" s="1">
         <v>1</v>
@@ -7982,7 +7961,7 @@
         <v>141</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>488</v>
+        <v>481</v>
       </c>
       <c r="C142" s="1">
         <v>1</v>
@@ -8004,7 +7983,7 @@
         <v>143</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>486</v>
+        <v>479</v>
       </c>
       <c r="C144" s="1">
         <v>1</v>
@@ -8015,7 +7994,7 @@
         <v>144</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>487</v>
+        <v>480</v>
       </c>
       <c r="C145" s="1">
         <v>1</v>
@@ -8070,7 +8049,7 @@
         <v>149</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>490</v>
+        <v>483</v>
       </c>
       <c r="C150" s="1">
         <v>1</v>
@@ -8092,7 +8071,7 @@
         <v>151</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>491</v>
+        <v>484</v>
       </c>
       <c r="C152" s="1">
         <v>1</v>
@@ -8142,7 +8121,7 @@
         <v>157</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>459</v>
+        <v>452</v>
       </c>
       <c r="C158" s="1">
         <v>1</v>
@@ -8208,7 +8187,7 @@
         <v>163</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>452</v>
+        <v>445</v>
       </c>
       <c r="C164" s="1">
         <v>1</v>
@@ -8241,7 +8220,7 @@
         <v>166</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
       <c r="C167" s="1">
         <v>1</v>
@@ -8426,7 +8405,7 @@
         <v>183</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
       <c r="C184" s="1">
         <v>1</v>
@@ -8547,7 +8526,7 @@
         <v>194</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>455</v>
+        <v>448</v>
       </c>
       <c r="C195" s="1">
         <v>1</v>
@@ -8734,7 +8713,7 @@
         <v>211</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="C212" s="1">
         <v>1</v>
@@ -8745,7 +8724,7 @@
         <v>212</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="C213" s="1">
         <v>1</v>
@@ -8767,7 +8746,7 @@
         <v>214</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>458</v>
+        <v>451</v>
       </c>
       <c r="C215" s="1">
         <v>1</v>
@@ -8788,12 +8767,8 @@
       <c r="A217" s="1">
         <v>216</v>
       </c>
-      <c r="B217" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="C217" s="1">
-        <v>1</v>
-      </c>
+      <c r="B217" s="1"/>
+      <c r="C217" s="1"/>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A218" s="1">
@@ -9060,7 +9035,7 @@
         <v>245</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>460</v>
+        <v>453</v>
       </c>
       <c r="C246" s="1">
         <v>1</v>
@@ -9104,7 +9079,7 @@
         <v>249</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>484</v>
+        <v>477</v>
       </c>
       <c r="C250" s="1">
         <v>1</v>
@@ -9223,23 +9198,15 @@
       <c r="A266" s="1">
         <v>265</v>
       </c>
-      <c r="B266" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="C266" s="1">
-        <v>1</v>
-      </c>
+      <c r="B266" s="1"/>
+      <c r="C266" s="1"/>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A267" s="1">
         <v>266</v>
       </c>
-      <c r="B267" s="1" t="s">
-        <v>430</v>
-      </c>
-      <c r="C267" s="1">
-        <v>1</v>
-      </c>
+      <c r="B267" s="1"/>
+      <c r="C267" s="1"/>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A268" s="1">
@@ -9299,7 +9266,7 @@
         <v>272</v>
       </c>
       <c r="B273" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C273" s="1">
         <v>1</v>
@@ -9332,7 +9299,7 @@
         <v>275</v>
       </c>
       <c r="B276" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C276" s="1"/>
     </row>
@@ -9351,12 +9318,8 @@
       <c r="A278" s="1">
         <v>277</v>
       </c>
-      <c r="B278" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="C278" s="1">
-        <v>1</v>
-      </c>
+      <c r="B278" s="1"/>
+      <c r="C278" s="1"/>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A279" s="1">
@@ -9493,7 +9456,7 @@
         <v>290</v>
       </c>
       <c r="B291" s="1" t="s">
-        <v>461</v>
+        <v>454</v>
       </c>
       <c r="C291" s="1">
         <v>1</v>
@@ -9504,7 +9467,7 @@
         <v>291</v>
       </c>
       <c r="B292" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C292" s="1">
         <v>1</v>
@@ -9526,7 +9489,7 @@
         <v>293</v>
       </c>
       <c r="B294" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C294" s="1"/>
     </row>
@@ -9623,7 +9586,7 @@
         <v>302</v>
       </c>
       <c r="B303" s="1" t="s">
-        <v>462</v>
+        <v>455</v>
       </c>
       <c r="C303" s="1">
         <v>1</v>
@@ -9689,7 +9652,7 @@
         <v>308</v>
       </c>
       <c r="B309" s="1" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
       <c r="C309" s="1">
         <v>1</v>
@@ -9733,7 +9696,7 @@
         <v>312</v>
       </c>
       <c r="B313" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C313" s="1">
         <v>1</v>
@@ -9959,7 +9922,7 @@
         <v>338</v>
       </c>
       <c r="B339" s="1" t="s">
-        <v>464</v>
+        <v>457</v>
       </c>
       <c r="C339" s="1">
         <v>1</v>
@@ -9969,19 +9932,15 @@
       <c r="A340" s="1">
         <v>339</v>
       </c>
-      <c r="B340" s="1" t="s">
-        <v>436</v>
-      </c>
-      <c r="C340" s="1">
-        <v>1</v>
-      </c>
+      <c r="B340" s="1"/>
+      <c r="C340" s="1"/>
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A341" s="1">
         <v>340</v>
       </c>
       <c r="B341" s="1" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="C341" s="1">
         <v>1</v>
@@ -10036,7 +9995,7 @@
         <v>345</v>
       </c>
       <c r="B346" s="3" t="s">
-        <v>492</v>
+        <v>485</v>
       </c>
       <c r="C346" s="3">
         <v>1</v>
@@ -10047,7 +10006,7 @@
         <v>346</v>
       </c>
       <c r="B347" s="1" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="C347" s="1">
         <v>1</v>
@@ -10080,7 +10039,7 @@
         <v>349</v>
       </c>
       <c r="B350" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C350" s="1"/>
     </row>
@@ -10129,7 +10088,7 @@
         <v>354</v>
       </c>
       <c r="B355" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C355" s="1">
         <v>1</v>
@@ -10173,7 +10132,7 @@
         <v>358</v>
       </c>
       <c r="B359" s="1" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="C359" s="1">
         <v>1</v>
@@ -10237,7 +10196,7 @@
         <v>364</v>
       </c>
       <c r="B365" s="1" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="C365" s="1">
         <v>1</v>
@@ -10320,7 +10279,7 @@
         <v>373</v>
       </c>
       <c r="B374" s="1" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C374" s="1"/>
     </row>
@@ -10329,7 +10288,7 @@
         <v>374</v>
       </c>
       <c r="B375" s="1" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="C375" s="1">
         <v>1</v>
@@ -10351,7 +10310,7 @@
         <v>376</v>
       </c>
       <c r="B377" s="1" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="C377" s="1">
         <v>1</v>
@@ -10373,7 +10332,7 @@
         <v>378</v>
       </c>
       <c r="B379" s="1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C379" s="1"/>
     </row>
@@ -10382,7 +10341,7 @@
         <v>379</v>
       </c>
       <c r="B380" s="1" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="C380" s="1">
         <v>1</v>
@@ -10393,7 +10352,7 @@
         <v>380</v>
       </c>
       <c r="B381" s="1" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="C381" s="1">
         <v>1</v>
@@ -10426,7 +10385,7 @@
         <v>383</v>
       </c>
       <c r="B384" s="1" t="s">
-        <v>473</v>
+        <v>466</v>
       </c>
       <c r="C384" s="1">
         <v>1</v>
@@ -10437,7 +10396,7 @@
         <v>384</v>
       </c>
       <c r="B385" s="1" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
       <c r="C385" s="1">
         <v>1</v>
@@ -10470,7 +10429,7 @@
         <v>387</v>
       </c>
       <c r="B388" s="1" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="C388" s="1">
         <v>1</v>
@@ -10687,19 +10646,15 @@
       <c r="A414" s="1">
         <v>413</v>
       </c>
-      <c r="B414" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="C414" s="1">
-        <v>1</v>
-      </c>
+      <c r="B414" s="1"/>
+      <c r="C414" s="1"/>
     </row>
     <row r="415" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A415" s="1">
         <v>414</v>
       </c>
       <c r="B415" s="1" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C415" s="1">
         <v>1</v>
@@ -10773,9 +10728,7 @@
       <c r="A422" s="1">
         <v>421</v>
       </c>
-      <c r="B422" s="1" t="s">
-        <v>442</v>
-      </c>
+      <c r="B422" s="1"/>
       <c r="C422" s="1"/>
     </row>
     <row r="423" spans="1:3" x14ac:dyDescent="0.2">
@@ -10793,43 +10746,29 @@
       <c r="A424" s="1">
         <v>423</v>
       </c>
-      <c r="B424" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="C424" s="1">
-        <v>1</v>
-      </c>
+      <c r="B424" s="1"/>
+      <c r="C424" s="1"/>
     </row>
     <row r="425" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A425" s="1">
         <v>424</v>
       </c>
-      <c r="B425" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="C425" s="1">
-        <v>1</v>
-      </c>
+      <c r="B425" s="1"/>
+      <c r="C425" s="1"/>
     </row>
     <row r="426" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A426" s="1">
         <v>425</v>
       </c>
-      <c r="B426" s="1" t="s">
-        <v>443</v>
-      </c>
+      <c r="B426" s="1"/>
       <c r="C426" s="1"/>
     </row>
     <row r="427" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A427" s="1">
         <v>426</v>
       </c>
-      <c r="B427" s="1" t="s">
-        <v>444</v>
-      </c>
-      <c r="C427" s="1">
-        <v>1</v>
-      </c>
+      <c r="B427" s="1"/>
+      <c r="C427" s="1"/>
     </row>
     <row r="428" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A428" s="1">
@@ -10922,7 +10861,7 @@
         <v>435</v>
       </c>
       <c r="B436" s="1" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="C436" s="1"/>
     </row>
@@ -10931,7 +10870,7 @@
         <v>436</v>
       </c>
       <c r="B437" s="1" t="s">
-        <v>476</v>
+        <v>469</v>
       </c>
       <c r="C437" s="1">
         <v>1</v>
@@ -10961,19 +10900,15 @@
       <c r="A440" s="1">
         <v>439</v>
       </c>
-      <c r="B440" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="C440" s="1">
-        <v>1</v>
-      </c>
+      <c r="B440" s="1"/>
+      <c r="C440" s="1"/>
     </row>
     <row r="441" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A441" s="1">
         <v>440</v>
       </c>
       <c r="B441" s="1" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="C441" s="1"/>
     </row>
@@ -11004,7 +10939,7 @@
         <v>443</v>
       </c>
       <c r="B444" s="1" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="C444" s="1"/>
     </row>
@@ -11123,7 +11058,7 @@
         <v>458</v>
       </c>
       <c r="B459" s="1" t="s">
-        <v>477</v>
+        <v>470</v>
       </c>
       <c r="C459" s="1">
         <v>1</v>
@@ -11144,9 +11079,7 @@
       <c r="A461" s="1">
         <v>460</v>
       </c>
-      <c r="B461" s="1" t="s">
-        <v>448</v>
-      </c>
+      <c r="B461" s="1"/>
       <c r="C461" s="1"/>
     </row>
     <row r="462" spans="1:3" x14ac:dyDescent="0.2">
@@ -11154,7 +11087,7 @@
         <v>461</v>
       </c>
       <c r="B462" s="1" t="s">
-        <v>479</v>
+        <v>472</v>
       </c>
       <c r="C462" s="1">
         <v>1</v>
@@ -11176,7 +11109,7 @@
         <v>463</v>
       </c>
       <c r="B464" s="1" t="s">
-        <v>478</v>
+        <v>471</v>
       </c>
       <c r="C464" s="1">
         <v>1</v>
@@ -11209,7 +11142,7 @@
         <v>466</v>
       </c>
       <c r="B467" s="1" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="C467" s="1"/>
     </row>
@@ -11218,7 +11151,7 @@
         <v>467</v>
       </c>
       <c r="B468" s="1" t="s">
-        <v>480</v>
+        <v>473</v>
       </c>
       <c r="C468" s="1">
         <v>1</v>
@@ -11229,7 +11162,7 @@
         <v>468</v>
       </c>
       <c r="B469" s="1" t="s">
-        <v>481</v>
+        <v>474</v>
       </c>
       <c r="C469" s="1">
         <v>1</v>
@@ -11250,9 +11183,7 @@
       <c r="A471" s="1">
         <v>470</v>
       </c>
-      <c r="B471" s="1" t="s">
-        <v>450</v>
-      </c>
+      <c r="B471" s="1"/>
       <c r="C471" s="1"/>
     </row>
     <row r="472" spans="1:3" x14ac:dyDescent="0.2">
@@ -11293,7 +11224,7 @@
         <v>474</v>
       </c>
       <c r="B475" s="1" t="s">
-        <v>482</v>
+        <v>475</v>
       </c>
       <c r="C475" s="1">
         <v>1</v>
@@ -11304,7 +11235,7 @@
         <v>475</v>
       </c>
       <c r="B476" s="1" t="s">
-        <v>483</v>
+        <v>476</v>
       </c>
       <c r="C476" s="1">
         <v>1</v>
@@ -11326,7 +11257,7 @@
         <v>477</v>
       </c>
       <c r="B478" s="1" t="s">
-        <v>451</v>
+        <v>444</v>
       </c>
       <c r="C478" s="1"/>
     </row>

</xml_diff>

<commit_message>
Updated decks and collection
</commit_message>
<xml_diff>
--- a/data/binder/Binder.xlsx
+++ b/data/binder/Binder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Dados/MTG/EDH DeckHelper/EDH-DeckHelper/data/binder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF631B81-8AA6-E346-9F2A-B4792229CDF7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{664478B3-944D-7840-B791-F95E8A0E1F95}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="12680" windowHeight="15540" activeTab="1" xr2:uid="{7ABBCC85-5F92-6F41-92E4-65212D317CF6}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="15500" windowHeight="15540" activeTab="1" xr2:uid="{7ABBCC85-5F92-6F41-92E4-65212D317CF6}"/>
   </bookViews>
   <sheets>
     <sheet name="Dual" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="533">
   <si>
     <t>Slot</t>
   </si>
@@ -1484,6 +1484,147 @@
   </si>
   <si>
     <t>Phyrexian Reclamation</t>
+  </si>
+  <si>
+    <t>Barkchannel Pathway // Tidechannel Pathway</t>
+  </si>
+  <si>
+    <t>Blightstep Pathway // Searstep Pathway</t>
+  </si>
+  <si>
+    <t>Branchloft Pathway // Boulderloft Pathway</t>
+  </si>
+  <si>
+    <t>Brightclimb Pathway // Grimclimb Pathway</t>
+  </si>
+  <si>
+    <t>Clearwater Pathway // Murkwater Pathway</t>
+  </si>
+  <si>
+    <t>Cragcrown Pathway // Timbercrown Pathway</t>
+  </si>
+  <si>
+    <t>Darkbore Pathway // Slitherbore Pathway</t>
+  </si>
+  <si>
+    <t>Hengegate Pathway // Mistgate Pathway</t>
+  </si>
+  <si>
+    <t>Needleverge Pathway // Pillarverge Pathway</t>
+  </si>
+  <si>
+    <t>Riverglide Pathway // Lavaglide Pathway</t>
+  </si>
+  <si>
+    <t>Rejuvenating Springs</t>
+  </si>
+  <si>
+    <t>Spectator Seating</t>
+  </si>
+  <si>
+    <t>Training Center</t>
+  </si>
+  <si>
+    <t>Undergrowth Stadium</t>
+  </si>
+  <si>
+    <t>Vault of Champions</t>
+  </si>
+  <si>
+    <t>Spire of Industry</t>
+  </si>
+  <si>
+    <t>Bag of Holding</t>
+  </si>
+  <si>
+    <t>Mox Amber</t>
+  </si>
+  <si>
+    <t>Idyllic Tutor</t>
+  </si>
+  <si>
+    <t>Ranger-Captain of Eos</t>
+  </si>
+  <si>
+    <t>Sevinne's Reclamation</t>
+  </si>
+  <si>
+    <t>Decree of Silence</t>
+  </si>
+  <si>
+    <t>Future Sight</t>
+  </si>
+  <si>
+    <t>Recurring Insight</t>
+  </si>
+  <si>
+    <t>Verity Circle</t>
+  </si>
+  <si>
+    <t>Brain Freeze</t>
+  </si>
+  <si>
+    <t>Hullbreacher</t>
+  </si>
+  <si>
+    <t>Miscast</t>
+  </si>
+  <si>
+    <t>Phantasmal Image</t>
+  </si>
+  <si>
+    <t>Teferi, Master of Time</t>
+  </si>
+  <si>
+    <t>Opposition Agent</t>
+  </si>
+  <si>
+    <t>Peer into the Abyss</t>
+  </si>
+  <si>
+    <t>Wishclaw Talisman</t>
+  </si>
+  <si>
+    <t>Abrade</t>
+  </si>
+  <si>
+    <t>Deflecting Swat</t>
+  </si>
+  <si>
+    <t>Jeska's Will</t>
+  </si>
+  <si>
+    <t>Rite of Flame</t>
+  </si>
+  <si>
+    <t>Simian Spirit Guide</t>
+  </si>
+  <si>
+    <t>Wheel of Misfortune</t>
+  </si>
+  <si>
+    <t>Beast Whisperer</t>
+  </si>
+  <si>
+    <t>Cultivate</t>
+  </si>
+  <si>
+    <t>Kodama's Reach</t>
+  </si>
+  <si>
+    <t>Vivien Reid</t>
+  </si>
+  <si>
+    <t>Thrasios, Triton Hero</t>
+  </si>
+  <si>
+    <t>Tymna the Weaver</t>
+  </si>
+  <si>
+    <t>Jeweled Lotus</t>
+  </si>
+  <si>
+    <t>Karn's Bastion</t>
   </si>
 </sst>
 </file>
@@ -6522,8 +6663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5953B7FC-4B75-B146-8A26-6CA09B5F3C99}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A416" zoomScale="91" workbookViewId="0">
-      <selection activeCell="B427" sqref="B427:C427"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6549,7 +6690,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>486</v>
       </c>
       <c r="C2" s="1"/>
     </row>
@@ -6558,7 +6699,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>487</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -6567,25 +6708,29 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="1"/>
+        <v>488</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="1"/>
+        <v>489</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>490</v>
       </c>
       <c r="C6" s="1"/>
     </row>
@@ -6594,7 +6739,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>8</v>
+        <v>491</v>
       </c>
       <c r="C7" s="1"/>
     </row>
@@ -6603,7 +6748,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>492</v>
       </c>
       <c r="C8" s="1"/>
     </row>
@@ -6612,7 +6757,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>10</v>
+        <v>493</v>
       </c>
       <c r="C9" s="1"/>
     </row>
@@ -6621,7 +6766,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>11</v>
+        <v>494</v>
       </c>
       <c r="C10" s="1"/>
     </row>
@@ -6630,9 +6775,11 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="1"/>
+        <v>495</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
@@ -6773,7 +6920,9 @@
       <c r="B24" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="1"/>
+      <c r="C24" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
@@ -7190,18 +7339,16 @@
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C65" s="1">
-        <v>1</v>
-      </c>
+        <v>496</v>
+      </c>
+      <c r="C65" s="1"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C66" s="1">
         <v>1</v>
@@ -7211,35 +7358,51 @@
       <c r="A67" s="1">
         <v>66</v>
       </c>
-      <c r="B67" s="1"/>
-      <c r="C67" s="1"/>
+      <c r="B67" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="C67" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>67</v>
       </c>
-      <c r="B68" s="1"/>
-      <c r="C68" s="1"/>
+      <c r="B68" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C68" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>68</v>
       </c>
-      <c r="B69" s="1"/>
-      <c r="C69" s="1"/>
+      <c r="B69" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="C69" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>69</v>
       </c>
-      <c r="B70" s="1"/>
+      <c r="B70" s="1" t="s">
+        <v>499</v>
+      </c>
       <c r="C70" s="1"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>70</v>
       </c>
-      <c r="B71" s="1"/>
+      <c r="B71" s="1" t="s">
+        <v>500</v>
+      </c>
       <c r="C71" s="1"/>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -7449,7 +7612,9 @@
       <c r="B92" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="C92" s="1"/>
+      <c r="C92" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
@@ -7729,7 +7894,9 @@
       <c r="B120" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="C120" s="1"/>
+      <c r="C120" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
@@ -7846,7 +8013,9 @@
       <c r="B131" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="C131" s="1"/>
+      <c r="C131" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
@@ -8016,7 +8185,7 @@
         <v>146</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>291</v>
+        <v>532</v>
       </c>
       <c r="C147" s="1">
         <v>1</v>
@@ -8027,7 +8196,7 @@
         <v>147</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>70</v>
+        <v>291</v>
       </c>
       <c r="C148" s="1">
         <v>1</v>
@@ -8038,7 +8207,7 @@
         <v>148</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>312</v>
+        <v>70</v>
       </c>
       <c r="C149" s="1">
         <v>1</v>
@@ -8048,19 +8217,17 @@
       <c r="A150" s="1">
         <v>149</v>
       </c>
-      <c r="B150" s="1" t="s">
-        <v>483</v>
-      </c>
-      <c r="C150" s="1">
-        <v>1</v>
-      </c>
+      <c r="B150" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C150" s="1"/>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" s="1">
         <v>150</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>64</v>
+        <v>312</v>
       </c>
       <c r="C151" s="1">
         <v>1</v>
@@ -8071,7 +8238,7 @@
         <v>151</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C152" s="1">
         <v>1</v>
@@ -8081,8 +8248,8 @@
       <c r="A153" s="1">
         <v>152</v>
       </c>
-      <c r="B153" s="1" t="s">
-        <v>66</v>
+      <c r="B153" s="3" t="s">
+        <v>501</v>
       </c>
       <c r="C153" s="1">
         <v>1</v>
@@ -8092,22 +8259,34 @@
       <c r="A154" s="1">
         <v>153</v>
       </c>
-      <c r="B154" s="1"/>
-      <c r="C154" s="1"/>
+      <c r="B154" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C154" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
         <v>154</v>
       </c>
-      <c r="B155" s="1"/>
-      <c r="C155" s="1"/>
+      <c r="B155" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="C155" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
         <v>155</v>
       </c>
-      <c r="B156" s="1"/>
-      <c r="C156" s="1"/>
+      <c r="B156" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C156" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
@@ -8154,7 +8333,7 @@
         <v>160</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>104</v>
+        <v>502</v>
       </c>
       <c r="C161" s="1">
         <v>1</v>
@@ -8165,7 +8344,7 @@
         <v>161</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>374</v>
+        <v>104</v>
       </c>
       <c r="C162" s="1">
         <v>1</v>
@@ -8176,7 +8355,7 @@
         <v>162</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>82</v>
+        <v>374</v>
       </c>
       <c r="C163" s="1">
         <v>1</v>
@@ -8187,7 +8366,7 @@
         <v>163</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>445</v>
+        <v>82</v>
       </c>
       <c r="C164" s="1">
         <v>1</v>
@@ -8198,7 +8377,7 @@
         <v>164</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>225</v>
+        <v>445</v>
       </c>
       <c r="C165" s="1">
         <v>1</v>
@@ -8209,7 +8388,7 @@
         <v>165</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>83</v>
+        <v>225</v>
       </c>
       <c r="C166" s="1">
         <v>1</v>
@@ -8220,7 +8399,7 @@
         <v>166</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>446</v>
+        <v>83</v>
       </c>
       <c r="C167" s="1">
         <v>1</v>
@@ -8231,7 +8410,7 @@
         <v>167</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>280</v>
+        <v>446</v>
       </c>
       <c r="C168" s="1">
         <v>1</v>
@@ -8242,7 +8421,7 @@
         <v>168</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>84</v>
+        <v>280</v>
       </c>
       <c r="C169" s="1">
         <v>1</v>
@@ -8253,7 +8432,7 @@
         <v>169</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>376</v>
+        <v>84</v>
       </c>
       <c r="C170" s="1">
         <v>1</v>
@@ -8264,7 +8443,7 @@
         <v>170</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>108</v>
+        <v>376</v>
       </c>
       <c r="C171" s="1">
         <v>1</v>
@@ -8275,7 +8454,7 @@
         <v>171</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>227</v>
+        <v>108</v>
       </c>
       <c r="C172" s="1">
         <v>1</v>
@@ -8286,7 +8465,7 @@
         <v>172</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>85</v>
+        <v>227</v>
       </c>
       <c r="C173" s="1">
         <v>1</v>
@@ -8297,7 +8476,7 @@
         <v>173</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
       <c r="C174" s="1">
         <v>1</v>
@@ -8308,7 +8487,7 @@
         <v>174</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>384</v>
+        <v>109</v>
       </c>
       <c r="C175" s="1">
         <v>1</v>
@@ -8319,7 +8498,7 @@
         <v>175</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>86</v>
+        <v>384</v>
       </c>
       <c r="C176" s="1">
         <v>1</v>
@@ -8330,7 +8509,7 @@
         <v>176</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>110</v>
+        <v>86</v>
       </c>
       <c r="C177" s="1">
         <v>1</v>
@@ -8341,7 +8520,7 @@
         <v>177</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>385</v>
+        <v>110</v>
       </c>
       <c r="C178" s="1">
         <v>1</v>
@@ -8352,7 +8531,7 @@
         <v>178</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>87</v>
+        <v>531</v>
       </c>
       <c r="C179" s="1"/>
     </row>
@@ -8361,7 +8540,7 @@
         <v>179</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>88</v>
+        <v>385</v>
       </c>
       <c r="C180" s="1">
         <v>1</v>
@@ -8372,18 +8551,16 @@
         <v>180</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C181" s="1">
-        <v>1</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="C181" s="1"/>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A182" s="1">
         <v>181</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C182" s="1">
         <v>1</v>
@@ -8394,7 +8571,7 @@
         <v>182</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C183" s="1">
         <v>1</v>
@@ -8405,7 +8582,7 @@
         <v>183</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>447</v>
+        <v>90</v>
       </c>
       <c r="C184" s="1">
         <v>1</v>
@@ -8416,7 +8593,7 @@
         <v>184</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C185" s="1">
         <v>1</v>
@@ -8427,7 +8604,7 @@
         <v>185</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>93</v>
+        <v>447</v>
       </c>
       <c r="C186" s="1">
         <v>1</v>
@@ -8438,18 +8615,16 @@
         <v>186</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="C187" s="1">
-        <v>1</v>
-      </c>
+        <v>503</v>
+      </c>
+      <c r="C187" s="1"/>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A188" s="1">
         <v>187</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="C188" s="1">
         <v>1</v>
@@ -8460,7 +8635,7 @@
         <v>188</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="C189" s="1">
         <v>1</v>
@@ -8471,7 +8646,7 @@
         <v>189</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C190" s="1">
         <v>1</v>
@@ -8482,7 +8657,7 @@
         <v>190</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>249</v>
+        <v>111</v>
       </c>
       <c r="C191" s="1">
         <v>1</v>
@@ -8493,7 +8668,7 @@
         <v>191</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="C192" s="1">
         <v>1</v>
@@ -8504,7 +8679,7 @@
         <v>192</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>96</v>
+        <v>388</v>
       </c>
       <c r="C193" s="1">
         <v>1</v>
@@ -8515,7 +8690,7 @@
         <v>193</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>106</v>
+        <v>249</v>
       </c>
       <c r="C194" s="1">
         <v>1</v>
@@ -8526,7 +8701,7 @@
         <v>194</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>448</v>
+        <v>112</v>
       </c>
       <c r="C195" s="1">
         <v>1</v>
@@ -8537,7 +8712,7 @@
         <v>195</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C196" s="1">
         <v>1</v>
@@ -8548,7 +8723,7 @@
         <v>196</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>389</v>
+        <v>106</v>
       </c>
       <c r="C197" s="1">
         <v>1</v>
@@ -8559,7 +8734,7 @@
         <v>197</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>378</v>
+        <v>448</v>
       </c>
       <c r="C198" s="1">
         <v>1</v>
@@ -8570,7 +8745,7 @@
         <v>198</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>379</v>
+        <v>97</v>
       </c>
       <c r="C199" s="1">
         <v>1</v>
@@ -8581,7 +8756,7 @@
         <v>199</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>380</v>
+        <v>389</v>
       </c>
       <c r="C200" s="1">
         <v>1</v>
@@ -8592,7 +8767,7 @@
         <v>200</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>99</v>
+        <v>378</v>
       </c>
       <c r="C201" s="1">
         <v>1</v>
@@ -8603,7 +8778,7 @@
         <v>201</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C202" s="1">
         <v>1</v>
@@ -8614,7 +8789,7 @@
         <v>202</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>113</v>
+        <v>380</v>
       </c>
       <c r="C203" s="1">
         <v>1</v>
@@ -8625,7 +8800,7 @@
         <v>203</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C204" s="1">
         <v>1</v>
@@ -8636,7 +8811,7 @@
         <v>204</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>114</v>
+        <v>381</v>
       </c>
       <c r="C205" s="1">
         <v>1</v>
@@ -8647,7 +8822,7 @@
         <v>205</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>382</v>
+        <v>113</v>
       </c>
       <c r="C206" s="1">
         <v>1</v>
@@ -8658,7 +8833,7 @@
         <v>206</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="C207" s="1">
         <v>1</v>
@@ -8669,7 +8844,7 @@
         <v>207</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>285</v>
+        <v>114</v>
       </c>
       <c r="C208" s="1">
         <v>1</v>
@@ -8680,7 +8855,7 @@
         <v>208</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="C209" s="1">
         <v>1</v>
@@ -8691,7 +8866,7 @@
         <v>209</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>391</v>
+        <v>115</v>
       </c>
       <c r="C210" s="1">
         <v>1</v>
@@ -8702,7 +8877,7 @@
         <v>210</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>393</v>
+        <v>285</v>
       </c>
       <c r="C211" s="1">
         <v>1</v>
@@ -8713,7 +8888,7 @@
         <v>211</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>449</v>
+        <v>390</v>
       </c>
       <c r="C212" s="1">
         <v>1</v>
@@ -8724,7 +8899,7 @@
         <v>212</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>450</v>
+        <v>391</v>
       </c>
       <c r="C213" s="1">
         <v>1</v>
@@ -8735,7 +8910,7 @@
         <v>213</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>101</v>
+        <v>393</v>
       </c>
       <c r="C214" s="1">
         <v>1</v>
@@ -8746,7 +8921,7 @@
         <v>214</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="C215" s="1">
         <v>1</v>
@@ -8757,7 +8932,7 @@
         <v>215</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>102</v>
+        <v>450</v>
       </c>
       <c r="C216" s="1">
         <v>1</v>
@@ -8767,22 +8942,34 @@
       <c r="A217" s="1">
         <v>216</v>
       </c>
-      <c r="B217" s="1"/>
-      <c r="C217" s="1"/>
+      <c r="B217" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C217" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A218" s="1">
         <v>217</v>
       </c>
-      <c r="B218" s="1"/>
-      <c r="C218" s="1"/>
+      <c r="B218" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="C218" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A219" s="1">
         <v>218</v>
       </c>
-      <c r="B219" s="1"/>
-      <c r="C219" s="1"/>
+      <c r="B219" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C219" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A220" s="1">
@@ -8870,7 +9057,7 @@
         <v>230</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>428</v>
+        <v>253</v>
       </c>
       <c r="C231" s="1">
         <v>1</v>
@@ -8881,7 +9068,7 @@
         <v>231</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>116</v>
+        <v>428</v>
       </c>
       <c r="C232" s="1">
         <v>1</v>
@@ -8892,7 +9079,7 @@
         <v>232</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>246</v>
+        <v>116</v>
       </c>
       <c r="C233" s="1">
         <v>1</v>
@@ -8903,7 +9090,7 @@
         <v>233</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>272</v>
+        <v>246</v>
       </c>
       <c r="C234" s="1">
         <v>1</v>
@@ -8914,7 +9101,7 @@
         <v>234</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>260</v>
+        <v>272</v>
       </c>
       <c r="C235" s="1">
         <v>1</v>
@@ -8925,7 +9112,7 @@
         <v>235</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C236" s="1">
         <v>1</v>
@@ -8936,7 +9123,7 @@
         <v>236</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C237" s="1">
         <v>1</v>
@@ -8947,7 +9134,7 @@
         <v>237</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>265</v>
+        <v>505</v>
       </c>
       <c r="C238" s="1">
         <v>1</v>
@@ -8958,7 +9145,7 @@
         <v>238</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>340</v>
+        <v>262</v>
       </c>
       <c r="C239" s="1">
         <v>1</v>
@@ -8969,7 +9156,7 @@
         <v>239</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>289</v>
+        <v>265</v>
       </c>
       <c r="C240" s="1">
         <v>1</v>
@@ -8980,7 +9167,7 @@
         <v>240</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>248</v>
+        <v>340</v>
       </c>
       <c r="C241" s="1">
         <v>1</v>
@@ -8991,7 +9178,7 @@
         <v>241</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>429</v>
+        <v>289</v>
       </c>
       <c r="C242" s="1">
         <v>1</v>
@@ -9002,7 +9189,7 @@
         <v>242</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>405</v>
+        <v>248</v>
       </c>
       <c r="C243" s="1">
         <v>1</v>
@@ -9013,7 +9200,7 @@
         <v>243</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>310</v>
+        <v>429</v>
       </c>
       <c r="C244" s="1">
         <v>1</v>
@@ -9024,7 +9211,7 @@
         <v>244</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>118</v>
+        <v>405</v>
       </c>
       <c r="C245" s="1">
         <v>1</v>
@@ -9035,7 +9222,7 @@
         <v>245</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>453</v>
+        <v>310</v>
       </c>
       <c r="C246" s="1">
         <v>1</v>
@@ -9046,7 +9233,7 @@
         <v>246</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C247" s="1">
         <v>1</v>
@@ -9057,7 +9244,7 @@
         <v>247</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>120</v>
+        <v>453</v>
       </c>
       <c r="C248" s="1">
         <v>1</v>
@@ -9068,7 +9255,7 @@
         <v>248</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>252</v>
+        <v>119</v>
       </c>
       <c r="C249" s="1">
         <v>1</v>
@@ -9079,7 +9266,7 @@
         <v>249</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>477</v>
+        <v>120</v>
       </c>
       <c r="C250" s="1">
         <v>1</v>
@@ -9090,7 +9277,7 @@
         <v>250</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C251" s="1">
         <v>1</v>
@@ -9100,29 +9287,43 @@
       <c r="A252" s="1">
         <v>251</v>
       </c>
-      <c r="B252" s="1"/>
-      <c r="C252" s="1"/>
+      <c r="B252" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="C252" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A253" s="1">
         <v>252</v>
       </c>
-      <c r="B253" s="1"/>
-      <c r="C253" s="1"/>
+      <c r="B253" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="C253" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A254" s="1">
         <v>253</v>
       </c>
-      <c r="B254" s="1"/>
+      <c r="B254" s="1" t="s">
+        <v>506</v>
+      </c>
       <c r="C254" s="1"/>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A255" s="1">
         <v>254</v>
       </c>
-      <c r="B255" s="1"/>
-      <c r="C255" s="1"/>
+      <c r="B255" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C255" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A256" s="1">
@@ -9198,14 +9399,20 @@
       <c r="A266" s="1">
         <v>265</v>
       </c>
-      <c r="B266" s="1"/>
-      <c r="C266" s="1"/>
+      <c r="B266" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C266" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A267" s="1">
         <v>266</v>
       </c>
-      <c r="B267" s="1"/>
+      <c r="B267" s="1" t="s">
+        <v>414</v>
+      </c>
       <c r="C267" s="1"/>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.2">
@@ -9213,31 +9420,29 @@
         <v>267</v>
       </c>
       <c r="B268" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="C268" s="1">
-        <v>1</v>
-      </c>
+        <v>512</v>
+      </c>
+      <c r="C268" s="1"/>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A269" s="1">
         <v>268</v>
       </c>
       <c r="B269" s="1" t="s">
-        <v>414</v>
-      </c>
-      <c r="C269" s="1"/>
+        <v>121</v>
+      </c>
+      <c r="C269" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A270" s="1">
         <v>269</v>
       </c>
       <c r="B270" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C270" s="1">
-        <v>1</v>
-      </c>
+        <v>514</v>
+      </c>
+      <c r="C270" s="1"/>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A271" s="1">
@@ -9308,18 +9513,20 @@
         <v>276</v>
       </c>
       <c r="B277" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="C277" s="1">
-        <v>1</v>
-      </c>
+        <v>515</v>
+      </c>
+      <c r="C277" s="1"/>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A278" s="1">
         <v>277</v>
       </c>
-      <c r="B278" s="1"/>
-      <c r="C278" s="1"/>
+      <c r="B278" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="C278" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A279" s="1">
@@ -9335,7 +9542,7 @@
         <v>279</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>124</v>
+        <v>507</v>
       </c>
       <c r="C280" s="1">
         <v>1</v>
@@ -9346,7 +9553,7 @@
         <v>280</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>283</v>
+        <v>508</v>
       </c>
       <c r="C281" s="1">
         <v>1</v>
@@ -9357,7 +9564,7 @@
         <v>281</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>394</v>
+        <v>124</v>
       </c>
       <c r="C282" s="1">
         <v>1</v>
@@ -9368,7 +9575,7 @@
         <v>282</v>
       </c>
       <c r="B283" s="1" t="s">
-        <v>125</v>
+        <v>283</v>
       </c>
       <c r="C283" s="1">
         <v>1</v>
@@ -9379,7 +9586,7 @@
         <v>283</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>126</v>
+        <v>510</v>
       </c>
       <c r="C284" s="1">
         <v>1</v>
@@ -9390,7 +9597,7 @@
         <v>284</v>
       </c>
       <c r="B285" s="1" t="s">
-        <v>127</v>
+        <v>394</v>
       </c>
       <c r="C285" s="1">
         <v>1</v>
@@ -9401,7 +9608,7 @@
         <v>285</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>128</v>
+        <v>511</v>
       </c>
       <c r="C286" s="1">
         <v>1</v>
@@ -9412,7 +9619,7 @@
         <v>286</v>
       </c>
       <c r="B287" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C287" s="1">
         <v>1</v>
@@ -9423,7 +9630,7 @@
         <v>287</v>
       </c>
       <c r="B288" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C288" s="1">
         <v>1</v>
@@ -9434,7 +9641,7 @@
         <v>288</v>
       </c>
       <c r="B289" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C289" s="1">
         <v>1</v>
@@ -9445,7 +9652,7 @@
         <v>289</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C290" s="1">
         <v>1</v>
@@ -9456,7 +9663,7 @@
         <v>290</v>
       </c>
       <c r="B291" s="1" t="s">
-        <v>454</v>
+        <v>129</v>
       </c>
       <c r="C291" s="1">
         <v>1</v>
@@ -9467,7 +9674,7 @@
         <v>291</v>
       </c>
       <c r="B292" s="1" t="s">
-        <v>432</v>
+        <v>130</v>
       </c>
       <c r="C292" s="1">
         <v>1</v>
@@ -9478,7 +9685,7 @@
         <v>292</v>
       </c>
       <c r="B293" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C293" s="1">
         <v>1</v>
@@ -9489,16 +9696,18 @@
         <v>293</v>
       </c>
       <c r="B294" s="1" t="s">
-        <v>433</v>
-      </c>
-      <c r="C294" s="1"/>
+        <v>132</v>
+      </c>
+      <c r="C294" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A295" s="1">
         <v>294</v>
       </c>
       <c r="B295" s="1" t="s">
-        <v>134</v>
+        <v>454</v>
       </c>
       <c r="C295" s="1">
         <v>1</v>
@@ -9509,7 +9718,7 @@
         <v>295</v>
       </c>
       <c r="B296" s="1" t="s">
-        <v>135</v>
+        <v>432</v>
       </c>
       <c r="C296" s="1">
         <v>1</v>
@@ -9520,7 +9729,7 @@
         <v>296</v>
       </c>
       <c r="B297" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C297" s="1">
         <v>1</v>
@@ -9531,18 +9740,16 @@
         <v>297</v>
       </c>
       <c r="B298" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C298" s="1">
-        <v>1</v>
-      </c>
+        <v>433</v>
+      </c>
+      <c r="C298" s="1"/>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A299" s="1">
         <v>298</v>
       </c>
       <c r="B299" s="1" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C299" s="1">
         <v>1</v>
@@ -9553,7 +9760,7 @@
         <v>299</v>
       </c>
       <c r="B300" s="1" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C300" s="1">
         <v>1</v>
@@ -9564,7 +9771,7 @@
         <v>300</v>
       </c>
       <c r="B301" s="1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C301" s="1">
         <v>1</v>
@@ -9575,7 +9782,7 @@
         <v>301</v>
       </c>
       <c r="B302" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C302" s="1">
         <v>1</v>
@@ -9586,7 +9793,7 @@
         <v>302</v>
       </c>
       <c r="B303" s="1" t="s">
-        <v>455</v>
+        <v>140</v>
       </c>
       <c r="C303" s="1">
         <v>1</v>
@@ -9597,7 +9804,7 @@
         <v>303</v>
       </c>
       <c r="B304" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C304" s="1">
         <v>1</v>
@@ -9608,7 +9815,7 @@
         <v>304</v>
       </c>
       <c r="B305" s="1" t="s">
-        <v>418</v>
+        <v>142</v>
       </c>
       <c r="C305" s="1">
         <v>1</v>
@@ -9619,7 +9826,7 @@
         <v>305</v>
       </c>
       <c r="B306" s="1" t="s">
-        <v>145</v>
+        <v>513</v>
       </c>
       <c r="C306" s="1">
         <v>1</v>
@@ -9630,7 +9837,7 @@
         <v>306</v>
       </c>
       <c r="B307" s="1" t="s">
-        <v>306</v>
+        <v>143</v>
       </c>
       <c r="C307" s="1">
         <v>1</v>
@@ -9641,7 +9848,7 @@
         <v>307</v>
       </c>
       <c r="B308" s="1" t="s">
-        <v>146</v>
+        <v>455</v>
       </c>
       <c r="C308" s="1">
         <v>1</v>
@@ -9652,7 +9859,7 @@
         <v>308</v>
       </c>
       <c r="B309" s="1" t="s">
-        <v>456</v>
+        <v>144</v>
       </c>
       <c r="C309" s="1">
         <v>1</v>
@@ -9663,7 +9870,7 @@
         <v>309</v>
       </c>
       <c r="B310" s="1" t="s">
-        <v>147</v>
+        <v>418</v>
       </c>
       <c r="C310" s="1">
         <v>1</v>
@@ -9674,7 +9881,7 @@
         <v>310</v>
       </c>
       <c r="B311" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C311" s="1">
         <v>1</v>
@@ -9685,7 +9892,7 @@
         <v>311</v>
       </c>
       <c r="B312" s="1" t="s">
-        <v>287</v>
+        <v>306</v>
       </c>
       <c r="C312" s="1">
         <v>1</v>
@@ -9696,7 +9903,7 @@
         <v>312</v>
       </c>
       <c r="B313" s="1" t="s">
-        <v>434</v>
+        <v>146</v>
       </c>
       <c r="C313" s="1">
         <v>1</v>
@@ -9707,7 +9914,7 @@
         <v>313</v>
       </c>
       <c r="B314" s="1" t="s">
-        <v>150</v>
+        <v>456</v>
       </c>
       <c r="C314" s="1">
         <v>1</v>
@@ -9718,7 +9925,7 @@
         <v>314</v>
       </c>
       <c r="B315" s="1" t="s">
-        <v>151</v>
+        <v>217</v>
       </c>
       <c r="C315" s="1">
         <v>1</v>
@@ -9729,7 +9936,7 @@
         <v>315</v>
       </c>
       <c r="B316" s="1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C316" s="1">
         <v>1</v>
@@ -9740,7 +9947,7 @@
         <v>316</v>
       </c>
       <c r="B317" s="1" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C317" s="1">
         <v>1</v>
@@ -9751,7 +9958,7 @@
         <v>317</v>
       </c>
       <c r="B318" s="1" t="s">
-        <v>154</v>
+        <v>287</v>
       </c>
       <c r="C318" s="1">
         <v>1</v>
@@ -9762,7 +9969,7 @@
         <v>318</v>
       </c>
       <c r="B319" s="1" t="s">
-        <v>221</v>
+        <v>434</v>
       </c>
       <c r="C319" s="1">
         <v>1</v>
@@ -9773,7 +9980,7 @@
         <v>319</v>
       </c>
       <c r="B320" s="1" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C320" s="1">
         <v>1</v>
@@ -9784,25 +9991,29 @@
         <v>320</v>
       </c>
       <c r="B321" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C321" s="1"/>
+        <v>151</v>
+      </c>
+      <c r="C321" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A322" s="1">
         <v>321</v>
       </c>
       <c r="B322" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C322" s="1"/>
+        <v>152</v>
+      </c>
+      <c r="C322" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A323" s="1">
         <v>322</v>
       </c>
       <c r="B323" s="1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C323" s="1">
         <v>1</v>
@@ -9812,57 +10023,85 @@
       <c r="A324" s="1">
         <v>323</v>
       </c>
-      <c r="B324" s="1"/>
-      <c r="C324" s="1"/>
+      <c r="B324" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C324" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A325" s="1">
         <v>324</v>
       </c>
-      <c r="B325" s="1"/>
-      <c r="C325" s="1"/>
+      <c r="B325" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="C325" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A326" s="1">
         <v>325</v>
       </c>
-      <c r="B326" s="1"/>
-      <c r="C326" s="1"/>
+      <c r="B326" s="3" t="s">
+        <v>509</v>
+      </c>
+      <c r="C326" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A327" s="1">
         <v>326</v>
       </c>
-      <c r="B327" s="1"/>
-      <c r="C327" s="1"/>
+      <c r="B327" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C327" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A328" s="1">
         <v>327</v>
       </c>
-      <c r="B328" s="1"/>
-      <c r="C328" s="1"/>
+      <c r="B328" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C328" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A329" s="1">
         <v>328</v>
       </c>
-      <c r="B329" s="1"/>
+      <c r="B329" s="1" t="s">
+        <v>156</v>
+      </c>
       <c r="C329" s="1"/>
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A330" s="1">
         <v>329</v>
       </c>
-      <c r="B330" s="1"/>
+      <c r="B330" s="1" t="s">
+        <v>157</v>
+      </c>
       <c r="C330" s="1"/>
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A331" s="1">
         <v>330</v>
       </c>
-      <c r="B331" s="1"/>
-      <c r="C331" s="1"/>
+      <c r="B331" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C331" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A332" s="1">
@@ -9932,7 +10171,9 @@
       <c r="A340" s="1">
         <v>339</v>
       </c>
-      <c r="B340" s="1"/>
+      <c r="B340" s="1" t="s">
+        <v>516</v>
+      </c>
       <c r="C340" s="1"/>
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.2">
@@ -10017,7 +10258,7 @@
         <v>347</v>
       </c>
       <c r="B348" s="1" t="s">
-        <v>163</v>
+        <v>518</v>
       </c>
       <c r="C348" s="1">
         <v>1</v>
@@ -10028,7 +10269,7 @@
         <v>348</v>
       </c>
       <c r="B349" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C349" s="1">
         <v>1</v>
@@ -10039,56 +10280,58 @@
         <v>349</v>
       </c>
       <c r="B350" s="1" t="s">
-        <v>435</v>
-      </c>
-      <c r="C350" s="1"/>
+        <v>164</v>
+      </c>
+      <c r="C350" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A351" s="1">
         <v>350</v>
       </c>
       <c r="B351" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C351" s="1">
-        <v>1</v>
-      </c>
+        <v>435</v>
+      </c>
+      <c r="C351" s="1"/>
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A352" s="1">
         <v>351</v>
       </c>
       <c r="B352" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="C352" s="1"/>
+        <v>165</v>
+      </c>
+      <c r="C352" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A353" s="1">
         <v>352</v>
       </c>
       <c r="B353" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C353" s="1">
-        <v>1</v>
-      </c>
+        <v>408</v>
+      </c>
+      <c r="C353" s="1"/>
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A354" s="1">
         <v>353</v>
       </c>
       <c r="B354" s="1" t="s">
-        <v>419</v>
-      </c>
-      <c r="C354" s="1"/>
+        <v>166</v>
+      </c>
+      <c r="C354" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="355" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A355" s="1">
         <v>354</v>
       </c>
       <c r="B355" s="1" t="s">
-        <v>436</v>
+        <v>419</v>
       </c>
       <c r="C355" s="1">
         <v>1</v>
@@ -10099,7 +10342,7 @@
         <v>355</v>
       </c>
       <c r="B356" s="1" t="s">
-        <v>167</v>
+        <v>436</v>
       </c>
       <c r="C356" s="1">
         <v>1</v>
@@ -10110,7 +10353,7 @@
         <v>356</v>
       </c>
       <c r="B357" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C357" s="1">
         <v>1</v>
@@ -10121,7 +10364,7 @@
         <v>357</v>
       </c>
       <c r="B358" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C358" s="1">
         <v>1</v>
@@ -10132,7 +10375,7 @@
         <v>358</v>
       </c>
       <c r="B359" s="1" t="s">
-        <v>460</v>
+        <v>169</v>
       </c>
       <c r="C359" s="1">
         <v>1</v>
@@ -10143,7 +10386,7 @@
         <v>359</v>
       </c>
       <c r="B360" s="1" t="s">
-        <v>314</v>
+        <v>460</v>
       </c>
       <c r="C360" s="1">
         <v>1</v>
@@ -10154,7 +10397,7 @@
         <v>360</v>
       </c>
       <c r="B361" s="1" t="s">
-        <v>170</v>
+        <v>314</v>
       </c>
       <c r="C361" s="1">
         <v>1</v>
@@ -10165,7 +10408,7 @@
         <v>361</v>
       </c>
       <c r="B362" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C362" s="1">
         <v>1</v>
@@ -10176,7 +10419,7 @@
         <v>362</v>
       </c>
       <c r="B363" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C363" s="1">
         <v>1</v>
@@ -10187,27 +10430,27 @@
         <v>363</v>
       </c>
       <c r="B364" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="C364" s="1"/>
+        <v>172</v>
+      </c>
+      <c r="C364" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="365" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A365" s="1">
         <v>364</v>
       </c>
       <c r="B365" s="1" t="s">
-        <v>461</v>
-      </c>
-      <c r="C365" s="1">
-        <v>1</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="C365" s="1"/>
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A366" s="1">
         <v>365</v>
       </c>
       <c r="B366" s="1" t="s">
-        <v>334</v>
+        <v>461</v>
       </c>
       <c r="C366" s="1">
         <v>1</v>
@@ -10218,18 +10461,16 @@
         <v>366</v>
       </c>
       <c r="B367" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C367" s="1">
-        <v>1</v>
-      </c>
+        <v>517</v>
+      </c>
+      <c r="C367" s="1"/>
     </row>
     <row r="368" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A368" s="1">
         <v>367</v>
       </c>
       <c r="B368" s="1" t="s">
-        <v>177</v>
+        <v>334</v>
       </c>
       <c r="C368" s="1">
         <v>1</v>
@@ -10240,7 +10481,7 @@
         <v>368</v>
       </c>
       <c r="B369" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C369" s="1">
         <v>1</v>
@@ -10250,15 +10491,23 @@
       <c r="A370" s="1">
         <v>369</v>
       </c>
-      <c r="B370" s="1"/>
-      <c r="C370" s="1"/>
+      <c r="B370" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C370" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A371" s="1">
         <v>370</v>
       </c>
-      <c r="B371" s="1"/>
-      <c r="C371" s="1"/>
+      <c r="B371" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C371" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A372" s="1">
@@ -10310,7 +10559,7 @@
         <v>376</v>
       </c>
       <c r="B377" s="1" t="s">
-        <v>463</v>
+        <v>523</v>
       </c>
       <c r="C377" s="1">
         <v>1</v>
@@ -10321,7 +10570,7 @@
         <v>377</v>
       </c>
       <c r="B378" s="1" t="s">
-        <v>224</v>
+        <v>463</v>
       </c>
       <c r="C378" s="1">
         <v>1</v>
@@ -10332,27 +10581,27 @@
         <v>378</v>
       </c>
       <c r="B379" s="1" t="s">
-        <v>438</v>
-      </c>
-      <c r="C379" s="1"/>
+        <v>224</v>
+      </c>
+      <c r="C379" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A380" s="1">
         <v>379</v>
       </c>
       <c r="B380" s="1" t="s">
-        <v>464</v>
-      </c>
-      <c r="C380" s="1">
-        <v>1</v>
-      </c>
+        <v>438</v>
+      </c>
+      <c r="C380" s="1"/>
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A381" s="1">
         <v>380</v>
       </c>
       <c r="B381" s="1" t="s">
-        <v>465</v>
+        <v>519</v>
       </c>
       <c r="C381" s="1">
         <v>1</v>
@@ -10363,7 +10612,7 @@
         <v>381</v>
       </c>
       <c r="B382" s="1" t="s">
-        <v>179</v>
+        <v>464</v>
       </c>
       <c r="C382" s="1">
         <v>1</v>
@@ -10374,18 +10623,16 @@
         <v>382</v>
       </c>
       <c r="B383" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="C383" s="1">
-        <v>1</v>
-      </c>
+        <v>520</v>
+      </c>
+      <c r="C383" s="1"/>
     </row>
     <row r="384" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A384" s="1">
         <v>383</v>
       </c>
       <c r="B384" s="1" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C384" s="1">
         <v>1</v>
@@ -10396,7 +10643,7 @@
         <v>384</v>
       </c>
       <c r="B385" s="1" t="s">
-        <v>467</v>
+        <v>179</v>
       </c>
       <c r="C385" s="1">
         <v>1</v>
@@ -10407,7 +10654,7 @@
         <v>385</v>
       </c>
       <c r="B386" s="1" t="s">
-        <v>396</v>
+        <v>180</v>
       </c>
       <c r="C386" s="1">
         <v>1</v>
@@ -10418,7 +10665,7 @@
         <v>386</v>
       </c>
       <c r="B387" s="1" t="s">
-        <v>218</v>
+        <v>466</v>
       </c>
       <c r="C387" s="1">
         <v>1</v>
@@ -10429,7 +10676,7 @@
         <v>387</v>
       </c>
       <c r="B388" s="1" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C388" s="1">
         <v>1</v>
@@ -10440,7 +10687,7 @@
         <v>388</v>
       </c>
       <c r="B389" s="1" t="s">
-        <v>339</v>
+        <v>396</v>
       </c>
       <c r="C389" s="1">
         <v>1</v>
@@ -10451,7 +10698,7 @@
         <v>389</v>
       </c>
       <c r="B390" s="1" t="s">
-        <v>181</v>
+        <v>218</v>
       </c>
       <c r="C390" s="1">
         <v>1</v>
@@ -10462,7 +10709,7 @@
         <v>390</v>
       </c>
       <c r="B391" s="1" t="s">
-        <v>220</v>
+        <v>468</v>
       </c>
       <c r="C391" s="1">
         <v>1</v>
@@ -10473,7 +10720,7 @@
         <v>391</v>
       </c>
       <c r="B392" s="1" t="s">
-        <v>268</v>
+        <v>339</v>
       </c>
       <c r="C392" s="1">
         <v>1</v>
@@ -10484,51 +10731,73 @@
         <v>392</v>
       </c>
       <c r="B393" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="C393" s="1"/>
+        <v>181</v>
+      </c>
+      <c r="C393" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="394" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A394" s="1">
         <v>393</v>
       </c>
-      <c r="B394" s="1"/>
+      <c r="B394" s="1" t="s">
+        <v>521</v>
+      </c>
       <c r="C394" s="1"/>
     </row>
     <row r="395" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A395" s="1">
         <v>394</v>
       </c>
-      <c r="B395" s="1"/>
-      <c r="C395" s="1"/>
+      <c r="B395" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="C395" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="396" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A396" s="1">
         <v>395</v>
       </c>
-      <c r="B396" s="1"/>
-      <c r="C396" s="1"/>
+      <c r="B396" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C396" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="397" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A397" s="1">
         <v>396</v>
       </c>
-      <c r="B397" s="1"/>
-      <c r="C397" s="1"/>
+      <c r="B397" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C397" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="398" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A398" s="1">
         <v>397</v>
       </c>
-      <c r="B398" s="1"/>
+      <c r="B398" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="C398" s="1"/>
     </row>
     <row r="399" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A399" s="1">
         <v>398</v>
       </c>
-      <c r="B399" s="1"/>
-      <c r="C399" s="1"/>
+      <c r="B399" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="C399" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="400" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A400" s="1">
@@ -10627,7 +10896,7 @@
         <v>411</v>
       </c>
       <c r="B412" s="1" t="s">
-        <v>184</v>
+        <v>525</v>
       </c>
       <c r="C412" s="1">
         <v>1</v>
@@ -10638,15 +10907,19 @@
         <v>412</v>
       </c>
       <c r="B413" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="C413" s="1"/>
+        <v>184</v>
+      </c>
+      <c r="C413" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="414" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A414" s="1">
         <v>413</v>
       </c>
-      <c r="B414" s="1"/>
+      <c r="B414" s="1" t="s">
+        <v>185</v>
+      </c>
       <c r="C414" s="1"/>
     </row>
     <row r="415" spans="1:3" x14ac:dyDescent="0.2">
@@ -10687,7 +10960,7 @@
         <v>417</v>
       </c>
       <c r="B418" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C418" s="1">
         <v>1</v>
@@ -10698,7 +10971,7 @@
         <v>418</v>
       </c>
       <c r="B419" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C419" s="1">
         <v>1</v>
@@ -10709,7 +10982,7 @@
         <v>419</v>
       </c>
       <c r="B420" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C420" s="1">
         <v>1</v>
@@ -10720,15 +10993,19 @@
         <v>420</v>
       </c>
       <c r="B421" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="C421" s="1"/>
+        <v>191</v>
+      </c>
+      <c r="C421" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="422" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A422" s="1">
         <v>421</v>
       </c>
-      <c r="B422" s="1"/>
+      <c r="B422" s="1" t="s">
+        <v>192</v>
+      </c>
       <c r="C422" s="1"/>
     </row>
     <row r="423" spans="1:3" x14ac:dyDescent="0.2">
@@ -10746,28 +11023,42 @@
       <c r="A424" s="1">
         <v>423</v>
       </c>
-      <c r="B424" s="1"/>
-      <c r="C424" s="1"/>
+      <c r="B424" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="C424" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="425" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A425" s="1">
         <v>424</v>
       </c>
-      <c r="B425" s="1"/>
-      <c r="C425" s="1"/>
+      <c r="B425" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C425" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="426" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A426" s="1">
         <v>425</v>
       </c>
-      <c r="B426" s="1"/>
-      <c r="C426" s="1"/>
+      <c r="B426" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C426" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="427" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A427" s="1">
         <v>426</v>
       </c>
-      <c r="B427" s="1"/>
+      <c r="B427" s="1" t="s">
+        <v>198</v>
+      </c>
       <c r="C427" s="1"/>
     </row>
     <row r="428" spans="1:3" x14ac:dyDescent="0.2">
@@ -10775,7 +11066,7 @@
         <v>427</v>
       </c>
       <c r="B428" s="1" t="s">
-        <v>196</v>
+        <v>293</v>
       </c>
       <c r="C428" s="1">
         <v>1</v>
@@ -10786,7 +11077,7 @@
         <v>428</v>
       </c>
       <c r="B429" s="1" t="s">
-        <v>197</v>
+        <v>294</v>
       </c>
       <c r="C429" s="1">
         <v>1</v>
@@ -10797,16 +11088,18 @@
         <v>429</v>
       </c>
       <c r="B430" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="C430" s="1"/>
+        <v>199</v>
+      </c>
+      <c r="C430" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="431" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A431" s="1">
         <v>430</v>
       </c>
       <c r="B431" s="1" t="s">
-        <v>293</v>
+        <v>231</v>
       </c>
       <c r="C431" s="1">
         <v>1</v>
@@ -10817,7 +11110,7 @@
         <v>431</v>
       </c>
       <c r="B432" s="1" t="s">
-        <v>294</v>
+        <v>200</v>
       </c>
       <c r="C432" s="1">
         <v>1</v>
@@ -10828,18 +11121,16 @@
         <v>432</v>
       </c>
       <c r="B433" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="C433" s="1">
-        <v>1</v>
-      </c>
+        <v>440</v>
+      </c>
+      <c r="C433" s="1"/>
     </row>
     <row r="434" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A434" s="1">
         <v>433</v>
       </c>
       <c r="B434" s="1" t="s">
-        <v>231</v>
+        <v>469</v>
       </c>
       <c r="C434" s="1">
         <v>1</v>
@@ -10850,7 +11141,7 @@
         <v>434</v>
       </c>
       <c r="B435" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C435" s="1">
         <v>1</v>
@@ -10861,7 +11152,7 @@
         <v>435</v>
       </c>
       <c r="B436" s="1" t="s">
-        <v>440</v>
+        <v>202</v>
       </c>
       <c r="C436" s="1"/>
     </row>
@@ -10870,18 +11161,16 @@
         <v>436</v>
       </c>
       <c r="B437" s="1" t="s">
-        <v>469</v>
-      </c>
-      <c r="C437" s="1">
-        <v>1</v>
-      </c>
+        <v>441</v>
+      </c>
+      <c r="C437" s="1"/>
     </row>
     <row r="438" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A438" s="1">
         <v>437</v>
       </c>
       <c r="B438" s="1" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C438" s="1">
         <v>1</v>
@@ -10892,23 +11181,29 @@
         <v>438</v>
       </c>
       <c r="B439" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="C439" s="1"/>
+        <v>526</v>
+      </c>
+      <c r="C439" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="440" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A440" s="1">
         <v>439</v>
       </c>
-      <c r="B440" s="1"/>
-      <c r="C440" s="1"/>
+      <c r="B440" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C440" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="441" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A441" s="1">
         <v>440</v>
       </c>
       <c r="B441" s="1" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="C441" s="1"/>
     </row>
@@ -10917,7 +11212,7 @@
         <v>441</v>
       </c>
       <c r="B442" s="1" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="C442" s="1">
         <v>1</v>
@@ -10928,7 +11223,7 @@
         <v>442</v>
       </c>
       <c r="B443" s="1" t="s">
-        <v>205</v>
+        <v>367</v>
       </c>
       <c r="C443" s="1">
         <v>1</v>
@@ -10939,16 +11234,18 @@
         <v>443</v>
       </c>
       <c r="B444" s="1" t="s">
-        <v>442</v>
-      </c>
-      <c r="C444" s="1"/>
+        <v>527</v>
+      </c>
+      <c r="C444" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="445" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A445" s="1">
         <v>444</v>
       </c>
       <c r="B445" s="1" t="s">
-        <v>206</v>
+        <v>234</v>
       </c>
       <c r="C445" s="1">
         <v>1</v>
@@ -10959,7 +11256,7 @@
         <v>445</v>
       </c>
       <c r="B446" s="1" t="s">
-        <v>234</v>
+        <v>368</v>
       </c>
       <c r="C446" s="1">
         <v>1</v>
@@ -11079,7 +11376,9 @@
       <c r="A461" s="1">
         <v>460</v>
       </c>
-      <c r="B461" s="1"/>
+      <c r="B461" s="1" t="s">
+        <v>529</v>
+      </c>
       <c r="C461" s="1"/>
     </row>
     <row r="462" spans="1:3" x14ac:dyDescent="0.2">
@@ -11087,18 +11386,16 @@
         <v>461</v>
       </c>
       <c r="B462" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="C462" s="1">
-        <v>1</v>
-      </c>
+        <v>530</v>
+      </c>
+      <c r="C462" s="1"/>
     </row>
     <row r="463" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A463" s="1">
         <v>462</v>
       </c>
       <c r="B463" s="1" t="s">
-        <v>279</v>
+        <v>472</v>
       </c>
       <c r="C463" s="1">
         <v>1</v>
@@ -11109,7 +11406,7 @@
         <v>463</v>
       </c>
       <c r="B464" s="1" t="s">
-        <v>471</v>
+        <v>279</v>
       </c>
       <c r="C464" s="1">
         <v>1</v>
@@ -11120,7 +11417,7 @@
         <v>464</v>
       </c>
       <c r="B465" s="1" t="s">
-        <v>210</v>
+        <v>471</v>
       </c>
       <c r="C465" s="1">
         <v>1</v>
@@ -11130,10 +11427,10 @@
       <c r="A466" s="1">
         <v>465</v>
       </c>
-      <c r="B466" s="3" t="s">
-        <v>313</v>
-      </c>
-      <c r="C466" s="3">
+      <c r="B466" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C466" s="1">
         <v>1</v>
       </c>
     </row>
@@ -11141,28 +11438,28 @@
       <c r="A467" s="1">
         <v>466</v>
       </c>
-      <c r="B467" s="1" t="s">
-        <v>443</v>
-      </c>
-      <c r="C467" s="1"/>
+      <c r="B467" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="C467" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="468" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A468" s="1">
         <v>467</v>
       </c>
       <c r="B468" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="C468" s="1">
-        <v>1</v>
-      </c>
+        <v>443</v>
+      </c>
+      <c r="C468" s="1"/>
     </row>
     <row r="469" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A469" s="1">
         <v>468</v>
       </c>
       <c r="B469" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C469" s="1">
         <v>1</v>
@@ -11173,7 +11470,7 @@
         <v>469</v>
       </c>
       <c r="B470" s="1" t="s">
-        <v>411</v>
+        <v>474</v>
       </c>
       <c r="C470" s="1">
         <v>1</v>
@@ -11183,8 +11480,12 @@
       <c r="A471" s="1">
         <v>470</v>
       </c>
-      <c r="B471" s="1"/>
-      <c r="C471" s="1"/>
+      <c r="B471" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="C471" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="472" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A472" s="1">

</xml_diff>

<commit_message>
Updated decks and collection. Added match function between lists.
</commit_message>
<xml_diff>
--- a/data/binder/Binder.xlsx
+++ b/data/binder/Binder.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Dados/MTG/EDH DeckHelper/EDH-DeckHelper/data/binder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38772A0A-4F99-CF4F-B9F1-D32F3FC49A6D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6252EE22-1F7D-7C41-B5B8-0DE48D2FAB63}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="15500" windowHeight="15540" activeTab="1" xr2:uid="{7ABBCC85-5F92-6F41-92E4-65212D317CF6}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="1" xr2:uid="{7ABBCC85-5F92-6F41-92E4-65212D317CF6}"/>
   </bookViews>
   <sheets>
     <sheet name="Dual" sheetId="1" r:id="rId1"/>
     <sheet name="Mono" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="Binder" localSheetId="1">Mono!$A$1:$C$481</definedName>
+  </definedNames>
   <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,8 +28,22 @@
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{7C70D46B-3370-5743-85EE-258EEB827E0E}" name="Binder1" type="6" refreshedVersion="7" background="1" saveData="1">
+    <textPr codePage="65001" sourceFile="/Volumes/Dados/MTG/EDH DeckHelper/EDH-DeckHelper/data/binder/Binder.csv" decimal="," thousands=" " tab="0" semicolon="1">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="549">
   <si>
     <t>Slot</t>
   </si>
@@ -1598,6 +1615,81 @@
   </si>
   <si>
     <t>Karn's Bastion</t>
+  </si>
+  <si>
+    <t>Choked Estuary</t>
+  </si>
+  <si>
+    <t>Foreboding Ruins</t>
+  </si>
+  <si>
+    <t>Fortified Village</t>
+  </si>
+  <si>
+    <t>Frostboil Snarl</t>
+  </si>
+  <si>
+    <t>Furycalm Snarl</t>
+  </si>
+  <si>
+    <t>Game Trail</t>
+  </si>
+  <si>
+    <t>Necroblossom Snarl</t>
+  </si>
+  <si>
+    <t>Port Town</t>
+  </si>
+  <si>
+    <t>Shineshadow Snarl</t>
+  </si>
+  <si>
+    <t>Vineglimmer Snarl</t>
+  </si>
+  <si>
+    <t>Oran-Rief, the Vastwood</t>
+  </si>
+  <si>
+    <t>Path of Ancestry</t>
+  </si>
+  <si>
+    <t>Herald's Horn</t>
+  </si>
+  <si>
+    <t>Myr Battlesphere</t>
+  </si>
+  <si>
+    <t>Spark Double</t>
+  </si>
+  <si>
+    <t>Avenger of Zendikar</t>
+  </si>
+  <si>
+    <t>Nissa, Who Shakes the World</t>
+  </si>
+  <si>
+    <t>Doubling Season</t>
+  </si>
+  <si>
+    <t>Parallel Lives</t>
+  </si>
+  <si>
+    <t>Primal Vigor</t>
+  </si>
+  <si>
+    <t>Krosan Grip</t>
+  </si>
+  <si>
+    <t>Grow from the Ashes</t>
+  </si>
+  <si>
+    <t>Rampant Growth</t>
+  </si>
+  <si>
+    <t>Skyshroud Claim</t>
+  </si>
+  <si>
+    <t>Three Visits</t>
   </si>
 </sst>
 </file>
@@ -1682,6 +1774,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Binder" connectionId="1" xr16:uid="{EADA6E5D-421F-E64D-A15E-66E3E48DBE40}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6636,15 +6732,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5953B7FC-4B75-B146-8A26-6CA09B5F3C99}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A418" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H428" sqref="H428"/>
+    <sheetView tabSelected="1" topLeftCell="A78" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.1640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -6663,28 +6759,23 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="C2" s="1"/>
+        <v>3</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>482</v>
-      </c>
-      <c r="C3" s="1"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>483</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -6692,10 +6783,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>484</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -6703,55 +6791,47 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>485</v>
-      </c>
-      <c r="C6" s="1"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="C7" s="1"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>487</v>
-      </c>
-      <c r="C8" s="1"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>488</v>
-      </c>
-      <c r="C9" s="1"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>489</v>
-      </c>
-      <c r="C10" s="1"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>490</v>
-      </c>
-      <c r="C11" s="1">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -6915,7 +6995,6 @@
       <c r="B26" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="1"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
@@ -6946,7 +7025,6 @@
       <c r="B29" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="1"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
@@ -6955,7 +7033,6 @@
       <c r="B30" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="1"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
@@ -7052,7 +7129,6 @@
       <c r="B39" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C39" s="1"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
@@ -7245,36 +7321,26 @@
       <c r="A57" s="1">
         <v>56</v>
       </c>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>57</v>
       </c>
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>58</v>
       </c>
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>59</v>
       </c>
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>60</v>
       </c>
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
@@ -7283,7 +7349,6 @@
       <c r="B62" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C62" s="1"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
@@ -7314,7 +7379,6 @@
       <c r="B65" s="1" t="s">
         <v>491</v>
       </c>
-      <c r="C65" s="1"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
@@ -7367,7 +7431,6 @@
       <c r="B70" s="1" t="s">
         <v>494</v>
       </c>
-      <c r="C70" s="1"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
@@ -7376,7 +7439,6 @@
       <c r="B71" s="1" t="s">
         <v>495</v>
       </c>
-      <c r="C71" s="1"/>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
@@ -7396,7 +7458,6 @@
       <c r="B73" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="C73" s="1"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
@@ -7427,7 +7488,6 @@
       <c r="B76" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="C76" s="1"/>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
@@ -7444,29 +7504,21 @@
       <c r="A78" s="1">
         <v>77</v>
       </c>
-      <c r="B78" s="1"/>
-      <c r="C78" s="1"/>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>78</v>
       </c>
-      <c r="B79" s="1"/>
-      <c r="C79" s="1"/>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>79</v>
       </c>
-      <c r="B80" s="1"/>
-      <c r="C80" s="1"/>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>80</v>
       </c>
-      <c r="B81" s="1"/>
-      <c r="C81" s="1"/>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
@@ -7583,10 +7635,7 @@
         <v>91</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>423</v>
-      </c>
-      <c r="C92" s="1">
-        <v>1</v>
+        <v>481</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
@@ -7594,10 +7643,7 @@
         <v>92</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="C93" s="1">
-        <v>1</v>
+        <v>482</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
@@ -7605,7 +7651,7 @@
         <v>93</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>422</v>
+        <v>483</v>
       </c>
       <c r="C94" s="1">
         <v>1</v>
@@ -7616,7 +7662,7 @@
         <v>94</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>424</v>
+        <v>484</v>
       </c>
       <c r="C95" s="1">
         <v>1</v>
@@ -7627,56 +7673,58 @@
         <v>95</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="C96" s="1">
-        <v>1</v>
+        <v>485</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>96</v>
       </c>
-      <c r="B97" s="1"/>
-      <c r="C97" s="1"/>
+      <c r="B97" s="1" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>97</v>
       </c>
-      <c r="B98" s="1"/>
-      <c r="C98" s="1"/>
+      <c r="B98" s="1" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>98</v>
       </c>
-      <c r="B99" s="1"/>
-      <c r="C99" s="1"/>
+      <c r="B99" s="1" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>99</v>
       </c>
-      <c r="B100" s="1"/>
-      <c r="C100" s="1"/>
+      <c r="B100" s="1" t="s">
+        <v>489</v>
+      </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>100</v>
       </c>
-      <c r="B101" s="1"/>
-      <c r="C101" s="1"/>
+      <c r="B101" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="C101" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>101</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C102" s="1">
-        <v>1</v>
+        <v>524</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
@@ -7684,10 +7732,7 @@
         <v>102</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C103" s="1">
-        <v>1</v>
+        <v>525</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
@@ -7695,10 +7740,7 @@
         <v>103</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C104" s="1">
-        <v>1</v>
+        <v>526</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
@@ -7706,10 +7748,7 @@
         <v>104</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C105" s="1">
-        <v>1</v>
+        <v>527</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
@@ -7717,10 +7756,7 @@
         <v>105</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C106" s="1">
-        <v>1</v>
+        <v>528</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
@@ -7728,10 +7764,7 @@
         <v>106</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C107" s="1">
-        <v>1</v>
+        <v>529</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
@@ -7739,10 +7772,7 @@
         <v>107</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C108" s="1">
-        <v>1</v>
+        <v>530</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
@@ -7750,19 +7780,15 @@
         <v>108</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C109" s="1"/>
+        <v>531</v>
+      </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>109</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="C110" s="1">
-        <v>1</v>
+        <v>532</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
@@ -7770,10 +7796,7 @@
         <v>110</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="C111" s="1">
-        <v>1</v>
+        <v>533</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
@@ -7781,7 +7804,7 @@
         <v>111</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>298</v>
+        <v>423</v>
       </c>
       <c r="C112" s="1">
         <v>1</v>
@@ -7792,7 +7815,7 @@
         <v>112</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>299</v>
+        <v>420</v>
       </c>
       <c r="C113" s="1">
         <v>1</v>
@@ -7803,7 +7826,7 @@
         <v>113</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>301</v>
+        <v>422</v>
       </c>
       <c r="C114" s="1">
         <v>1</v>
@@ -7814,7 +7837,7 @@
         <v>114</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>300</v>
+        <v>424</v>
       </c>
       <c r="C115" s="1">
         <v>1</v>
@@ -7825,7 +7848,7 @@
         <v>115</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>302</v>
+        <v>421</v>
       </c>
       <c r="C116" s="1">
         <v>1</v>
@@ -7835,61 +7858,33 @@
       <c r="A117" s="1">
         <v>116</v>
       </c>
-      <c r="B117" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="C117" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
         <v>117</v>
       </c>
-      <c r="B118" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="C118" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
         <v>118</v>
       </c>
-      <c r="B119" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="C119" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
         <v>119</v>
       </c>
-      <c r="B120" s="1" t="s">
-        <v>425</v>
-      </c>
-      <c r="C120" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
         <v>120</v>
       </c>
-      <c r="B121" s="1" t="s">
-        <v>402</v>
-      </c>
-      <c r="C121" s="1"/>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
         <v>121</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>322</v>
+        <v>73</v>
       </c>
       <c r="C122" s="1">
         <v>1</v>
@@ -7900,7 +7895,7 @@
         <v>122</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>406</v>
+        <v>74</v>
       </c>
       <c r="C123" s="1">
         <v>1</v>
@@ -7911,7 +7906,7 @@
         <v>123</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>320</v>
+        <v>75</v>
       </c>
       <c r="C124" s="1">
         <v>1</v>
@@ -7922,7 +7917,7 @@
         <v>124</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="C125" s="1">
         <v>1</v>
@@ -7933,7 +7928,7 @@
         <v>125</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="C126" s="1">
         <v>1</v>
@@ -7944,7 +7939,7 @@
         <v>126</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="C127" s="1">
         <v>1</v>
@@ -7955,7 +7950,7 @@
         <v>127</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="C128" s="1">
         <v>1</v>
@@ -7966,10 +7961,7 @@
         <v>128</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C129" s="1">
-        <v>1</v>
+        <v>78</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
@@ -7977,7 +7969,7 @@
         <v>129</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>62</v>
+        <v>296</v>
       </c>
       <c r="C130" s="1">
         <v>1</v>
@@ -7988,7 +7980,7 @@
         <v>130</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>278</v>
+        <v>297</v>
       </c>
       <c r="C131" s="1">
         <v>1</v>
@@ -7999,7 +7991,7 @@
         <v>131</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>71</v>
+        <v>298</v>
       </c>
       <c r="C132" s="1">
         <v>1</v>
@@ -8010,7 +8002,7 @@
         <v>132</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>317</v>
+        <v>299</v>
       </c>
       <c r="C133" s="1">
         <v>1</v>
@@ -8021,16 +8013,18 @@
         <v>133</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="C134" s="1"/>
+        <v>301</v>
+      </c>
+      <c r="C134" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
         <v>134</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>413</v>
+        <v>300</v>
       </c>
       <c r="C135" s="1">
         <v>1</v>
@@ -8041,7 +8035,7 @@
         <v>135</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>426</v>
+        <v>302</v>
       </c>
       <c r="C136" s="1">
         <v>1</v>
@@ -8052,7 +8046,7 @@
         <v>136</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>256</v>
+        <v>303</v>
       </c>
       <c r="C137" s="1">
         <v>1</v>
@@ -8063,7 +8057,7 @@
         <v>137</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>65</v>
+        <v>304</v>
       </c>
       <c r="C138" s="1">
         <v>1</v>
@@ -8074,7 +8068,7 @@
         <v>138</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>477</v>
+        <v>305</v>
       </c>
       <c r="C139" s="1">
         <v>1</v>
@@ -8085,7 +8079,7 @@
         <v>139</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>67</v>
+        <v>425</v>
       </c>
       <c r="C140" s="1">
         <v>1</v>
@@ -8096,10 +8090,7 @@
         <v>140</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>476</v>
-      </c>
-      <c r="C141" s="1">
-        <v>1</v>
+        <v>402</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
@@ -8107,7 +8098,7 @@
         <v>141</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>397</v>
+        <v>322</v>
       </c>
       <c r="C142" s="1">
         <v>1</v>
@@ -8118,7 +8109,7 @@
         <v>142</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>474</v>
+        <v>406</v>
       </c>
       <c r="C143" s="1">
         <v>1</v>
@@ -8129,7 +8120,7 @@
         <v>143</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>475</v>
+        <v>320</v>
       </c>
       <c r="C144" s="1">
         <v>1</v>
@@ -8140,7 +8131,7 @@
         <v>144</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>336</v>
+        <v>59</v>
       </c>
       <c r="C145" s="1">
         <v>1</v>
@@ -8151,7 +8142,7 @@
         <v>145</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>523</v>
+        <v>58</v>
       </c>
       <c r="C146" s="1">
         <v>1</v>
@@ -8162,7 +8153,7 @@
         <v>146</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C147" s="1">
         <v>1</v>
@@ -8172,17 +8163,19 @@
       <c r="A148" s="1">
         <v>147</v>
       </c>
-      <c r="B148" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C148" s="1"/>
+      <c r="B148" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C148" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
         <v>148</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>312</v>
+        <v>63</v>
       </c>
       <c r="C149" s="1">
         <v>1</v>
@@ -8193,7 +8186,7 @@
         <v>149</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>478</v>
+        <v>62</v>
       </c>
       <c r="C150" s="1">
         <v>1</v>
@@ -8203,8 +8196,8 @@
       <c r="A151" s="1">
         <v>150</v>
       </c>
-      <c r="B151" s="3" t="s">
-        <v>496</v>
+      <c r="B151" s="1" t="s">
+        <v>278</v>
       </c>
       <c r="C151" s="1">
         <v>1</v>
@@ -8215,7 +8208,7 @@
         <v>151</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="C152" s="1">
         <v>1</v>
@@ -8226,7 +8219,7 @@
         <v>152</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>479</v>
+        <v>317</v>
       </c>
       <c r="C153" s="1">
         <v>1</v>
@@ -8237,46 +8230,59 @@
         <v>153</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C154" s="1">
-        <v>1</v>
+        <v>473</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
         <v>154</v>
       </c>
-      <c r="B155" s="1"/>
-      <c r="C155" s="1"/>
+      <c r="B155" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="C155" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
         <v>155</v>
       </c>
-      <c r="B156" s="1"/>
-      <c r="C156" s="1"/>
+      <c r="B156" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="C156" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
         <v>156</v>
       </c>
-      <c r="B157" s="1"/>
-      <c r="C157" s="1"/>
+      <c r="B157" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C157" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158" s="1">
         <v>157</v>
       </c>
-      <c r="B158" s="1"/>
-      <c r="C158" s="1"/>
+      <c r="B158" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C158" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159" s="1">
         <v>158</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>427</v>
+        <v>477</v>
       </c>
       <c r="C159" s="1">
         <v>1</v>
@@ -8287,7 +8293,7 @@
         <v>159</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
       <c r="C160" s="1">
         <v>1</v>
@@ -8298,7 +8304,7 @@
         <v>160</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>497</v>
+        <v>476</v>
       </c>
       <c r="C161" s="1">
         <v>1</v>
@@ -8309,7 +8315,7 @@
         <v>161</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>104</v>
+        <v>397</v>
       </c>
       <c r="C162" s="1">
         <v>1</v>
@@ -8320,7 +8326,7 @@
         <v>162</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>374</v>
+        <v>474</v>
       </c>
       <c r="C163" s="1">
         <v>1</v>
@@ -8331,7 +8337,7 @@
         <v>163</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>82</v>
+        <v>475</v>
       </c>
       <c r="C164" s="1">
         <v>1</v>
@@ -8342,7 +8348,7 @@
         <v>164</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>444</v>
+        <v>336</v>
       </c>
       <c r="C165" s="1">
         <v>1</v>
@@ -8353,7 +8359,7 @@
         <v>165</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>225</v>
+        <v>523</v>
       </c>
       <c r="C166" s="1">
         <v>1</v>
@@ -8364,7 +8370,7 @@
         <v>166</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="C167" s="1">
         <v>1</v>
@@ -8375,7 +8381,7 @@
         <v>167</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>445</v>
+        <v>534</v>
       </c>
       <c r="C168" s="1">
         <v>1</v>
@@ -8385,18 +8391,19 @@
       <c r="A169" s="1">
         <v>168</v>
       </c>
-      <c r="B169" s="1"/>
-      <c r="C169" s="1"/>
+      <c r="B169" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="C169" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A170" s="1">
         <v>169</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C170" s="1">
-        <v>1</v>
+        <v>68</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.2">
@@ -8404,7 +8411,7 @@
         <v>170</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>376</v>
+        <v>312</v>
       </c>
       <c r="C171" s="1">
         <v>1</v>
@@ -8415,7 +8422,7 @@
         <v>171</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>108</v>
+        <v>478</v>
       </c>
       <c r="C172" s="1">
         <v>1</v>
@@ -8425,15 +8432,19 @@
       <c r="A173" s="1">
         <v>172</v>
       </c>
-      <c r="B173" s="1"/>
-      <c r="C173" s="1"/>
+      <c r="B173" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="C173" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A174" s="1">
         <v>173</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="C174" s="1">
         <v>1</v>
@@ -8444,7 +8455,7 @@
         <v>174</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>109</v>
+        <v>479</v>
       </c>
       <c r="C175" s="1">
         <v>1</v>
@@ -8455,7 +8466,7 @@
         <v>175</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>384</v>
+        <v>66</v>
       </c>
       <c r="C176" s="1">
         <v>1</v>
@@ -8465,59 +8476,33 @@
       <c r="A177" s="1">
         <v>176</v>
       </c>
-      <c r="B177" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C177" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A178" s="1">
         <v>177</v>
       </c>
-      <c r="B178" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C178" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A179" s="1">
         <v>178</v>
       </c>
-      <c r="B179" s="1" t="s">
-        <v>522</v>
-      </c>
-      <c r="C179" s="1"/>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A180" s="1">
         <v>179</v>
       </c>
-      <c r="B180" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="C180" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A181" s="1">
         <v>180</v>
       </c>
-      <c r="B181" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C181" s="1"/>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A182" s="1">
         <v>181</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>88</v>
+        <v>427</v>
       </c>
       <c r="C182" s="1">
         <v>1</v>
@@ -8528,7 +8513,7 @@
         <v>182</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>89</v>
+        <v>107</v>
       </c>
       <c r="C183" s="1">
         <v>1</v>
@@ -8539,7 +8524,7 @@
         <v>183</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>90</v>
+        <v>497</v>
       </c>
       <c r="C184" s="1">
         <v>1</v>
@@ -8550,7 +8535,7 @@
         <v>184</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="C185" s="1">
         <v>1</v>
@@ -8561,7 +8546,7 @@
         <v>185</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>446</v>
+        <v>374</v>
       </c>
       <c r="C186" s="1">
         <v>1</v>
@@ -8572,16 +8557,18 @@
         <v>186</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>498</v>
-      </c>
-      <c r="C187" s="1"/>
+        <v>82</v>
+      </c>
+      <c r="C187" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A188" s="1">
         <v>187</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>92</v>
+        <v>444</v>
       </c>
       <c r="C188" s="1">
         <v>1</v>
@@ -8592,7 +8579,7 @@
         <v>188</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>93</v>
+        <v>225</v>
       </c>
       <c r="C189" s="1">
         <v>1</v>
@@ -8603,7 +8590,7 @@
         <v>189</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>387</v>
+        <v>83</v>
       </c>
       <c r="C190" s="1">
         <v>1</v>
@@ -8614,7 +8601,7 @@
         <v>190</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>111</v>
+        <v>445</v>
       </c>
       <c r="C191" s="1">
         <v>1</v>
@@ -8625,7 +8612,7 @@
         <v>191</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="C192" s="1">
         <v>1</v>
@@ -8636,7 +8623,7 @@
         <v>192</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>388</v>
+        <v>376</v>
       </c>
       <c r="C193" s="1">
         <v>1</v>
@@ -8646,15 +8633,19 @@
       <c r="A194" s="1">
         <v>193</v>
       </c>
-      <c r="B194" s="1"/>
-      <c r="C194" s="1"/>
+      <c r="B194" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C194" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A195" s="1">
         <v>194</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>112</v>
+        <v>85</v>
       </c>
       <c r="C195" s="1">
         <v>1</v>
@@ -8665,7 +8656,7 @@
         <v>195</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="C196" s="1">
         <v>1</v>
@@ -8676,7 +8667,7 @@
         <v>196</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>106</v>
+        <v>384</v>
       </c>
       <c r="C197" s="1">
         <v>1</v>
@@ -8687,7 +8678,7 @@
         <v>197</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>447</v>
+        <v>536</v>
       </c>
       <c r="C198" s="1">
         <v>1</v>
@@ -8698,7 +8689,7 @@
         <v>198</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C199" s="1">
         <v>1</v>
@@ -8709,7 +8700,7 @@
         <v>199</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>389</v>
+        <v>110</v>
       </c>
       <c r="C200" s="1">
         <v>1</v>
@@ -8720,10 +8711,7 @@
         <v>200</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="C201" s="1">
-        <v>1</v>
+        <v>522</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.2">
@@ -8731,7 +8719,7 @@
         <v>201</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c r="C202" s="1">
         <v>1</v>
@@ -8742,10 +8730,7 @@
         <v>202</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="C203" s="1">
-        <v>1</v>
+        <v>87</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.2">
@@ -8753,7 +8738,7 @@
         <v>203</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="C204" s="1">
         <v>1</v>
@@ -8764,7 +8749,7 @@
         <v>204</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>381</v>
+        <v>89</v>
       </c>
       <c r="C205" s="1">
         <v>1</v>
@@ -8775,7 +8760,7 @@
         <v>205</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="C206" s="1">
         <v>1</v>
@@ -8786,7 +8771,7 @@
         <v>206</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C207" s="1">
         <v>1</v>
@@ -8797,7 +8782,7 @@
         <v>207</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>114</v>
+        <v>446</v>
       </c>
       <c r="C208" s="1">
         <v>1</v>
@@ -8808,10 +8793,7 @@
         <v>208</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="C209" s="1">
-        <v>1</v>
+        <v>498</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.2">
@@ -8819,7 +8801,7 @@
         <v>209</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="C210" s="1">
         <v>1</v>
@@ -8830,7 +8812,7 @@
         <v>210</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>285</v>
+        <v>93</v>
       </c>
       <c r="C211" s="1">
         <v>1</v>
@@ -8841,7 +8823,7 @@
         <v>211</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="C212" s="1">
         <v>1</v>
@@ -8852,7 +8834,7 @@
         <v>212</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>391</v>
+        <v>111</v>
       </c>
       <c r="C213" s="1">
         <v>1</v>
@@ -8863,7 +8845,7 @@
         <v>213</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>393</v>
+        <v>105</v>
       </c>
       <c r="C214" s="1">
         <v>1</v>
@@ -8873,15 +8855,19 @@
       <c r="A215" s="1">
         <v>214</v>
       </c>
-      <c r="B215" s="1"/>
-      <c r="C215" s="1"/>
+      <c r="B215" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="C215" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A216" s="1">
         <v>215</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>448</v>
+        <v>112</v>
       </c>
       <c r="C216" s="1">
         <v>1</v>
@@ -8891,15 +8877,19 @@
       <c r="A217" s="1">
         <v>216</v>
       </c>
-      <c r="B217" s="1"/>
-      <c r="C217" s="1"/>
+      <c r="B217" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C217" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A218" s="1">
         <v>217</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>449</v>
+        <v>106</v>
       </c>
       <c r="C218" s="1">
         <v>1</v>
@@ -8909,85 +8899,129 @@
       <c r="A219" s="1">
         <v>218</v>
       </c>
-      <c r="B219" s="1"/>
-      <c r="C219" s="1"/>
+      <c r="B219" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="C219" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A220" s="1">
         <v>219</v>
       </c>
-      <c r="B220" s="1"/>
-      <c r="C220" s="1"/>
+      <c r="B220" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C220" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A221" s="1">
         <v>220</v>
       </c>
-      <c r="B221" s="1"/>
-      <c r="C221" s="1"/>
+      <c r="B221" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="C221" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A222" s="1">
         <v>221</v>
       </c>
-      <c r="B222" s="1"/>
-      <c r="C222" s="1"/>
+      <c r="B222" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="C222" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A223" s="1">
         <v>222</v>
       </c>
-      <c r="B223" s="1"/>
-      <c r="C223" s="1"/>
+      <c r="B223" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="C223" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A224" s="1">
         <v>223</v>
       </c>
-      <c r="B224" s="1"/>
-      <c r="C224" s="1"/>
+      <c r="B224" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="C224" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A225" s="1">
         <v>224</v>
       </c>
-      <c r="B225" s="1"/>
-      <c r="C225" s="1"/>
+      <c r="B225" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C225" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A226" s="1">
         <v>225</v>
       </c>
-      <c r="B226" s="1"/>
-      <c r="C226" s="1"/>
+      <c r="B226" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="C226" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A227" s="1">
         <v>226</v>
       </c>
-      <c r="B227" s="1"/>
-      <c r="C227" s="1"/>
+      <c r="B227" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C227" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A228" s="1">
         <v>227</v>
       </c>
-      <c r="B228" s="1"/>
-      <c r="C228" s="1"/>
+      <c r="B228" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C228" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A229" s="1">
         <v>228</v>
       </c>
-      <c r="B229" s="1"/>
-      <c r="C229" s="1"/>
+      <c r="B229" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C229" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A230" s="1">
         <v>229</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>117</v>
+        <v>382</v>
       </c>
       <c r="C230" s="1">
         <v>1</v>
@@ -8998,7 +9032,7 @@
         <v>230</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>253</v>
+        <v>115</v>
       </c>
       <c r="C231" s="1">
         <v>1</v>
@@ -9009,7 +9043,7 @@
         <v>231</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>428</v>
+        <v>285</v>
       </c>
       <c r="C232" s="1">
         <v>1</v>
@@ -9019,15 +9053,19 @@
       <c r="A233" s="1">
         <v>232</v>
       </c>
-      <c r="B233" s="1"/>
-      <c r="C233" s="1"/>
+      <c r="B233" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="C233" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A234" s="1">
         <v>233</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>246</v>
+        <v>391</v>
       </c>
       <c r="C234" s="1">
         <v>1</v>
@@ -9038,7 +9076,7 @@
         <v>234</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>272</v>
+        <v>393</v>
       </c>
       <c r="C235" s="1">
         <v>1</v>
@@ -9049,7 +9087,7 @@
         <v>235</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>260</v>
+        <v>448</v>
       </c>
       <c r="C236" s="1">
         <v>1</v>
@@ -9060,7 +9098,7 @@
         <v>236</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>261</v>
+        <v>449</v>
       </c>
       <c r="C237" s="1">
         <v>1</v>
@@ -9071,7 +9109,7 @@
         <v>237</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>500</v>
+        <v>537</v>
       </c>
       <c r="C238" s="1">
         <v>1</v>
@@ -9081,166 +9119,94 @@
       <c r="A239" s="1">
         <v>238</v>
       </c>
-      <c r="B239" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="C239" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A240" s="1">
         <v>239</v>
       </c>
-      <c r="B240" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="C240" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A241" s="1">
         <v>240</v>
       </c>
-      <c r="B241" s="1"/>
-      <c r="C241" s="1"/>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A242" s="1">
         <v>241</v>
       </c>
-      <c r="B242" s="1"/>
-      <c r="C242" s="1"/>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A243" s="1">
         <v>242</v>
       </c>
-      <c r="B243" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="C243" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A244" s="1">
         <v>243</v>
       </c>
-      <c r="B244" s="1"/>
-      <c r="C244" s="1"/>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A245" s="1">
         <v>244</v>
       </c>
-      <c r="B245" s="1" t="s">
-        <v>405</v>
-      </c>
-      <c r="C245" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A246" s="1">
         <v>245</v>
       </c>
-      <c r="B246" s="1"/>
-      <c r="C246" s="1"/>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A247" s="1">
         <v>246</v>
       </c>
-      <c r="B247" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C247" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A248" s="1">
         <v>247</v>
       </c>
-      <c r="B248" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="C248" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A249" s="1">
         <v>248</v>
       </c>
-      <c r="B249" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C249" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A250" s="1">
         <v>249</v>
       </c>
-      <c r="B250" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C250" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A251" s="1">
         <v>250</v>
       </c>
-      <c r="B251" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="C251" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A252" s="1">
         <v>251</v>
       </c>
-      <c r="B252" s="1" t="s">
-        <v>499</v>
-      </c>
-      <c r="C252" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A253" s="1">
         <v>252</v>
       </c>
-      <c r="B253" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="C253" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A254" s="1">
         <v>253</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>501</v>
-      </c>
-      <c r="C254" s="1"/>
+        <v>117</v>
+      </c>
+      <c r="C254" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A255" s="1">
         <v>254</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C255" s="1">
         <v>1</v>
@@ -9250,103 +9216,151 @@
       <c r="A256" s="1">
         <v>255</v>
       </c>
-      <c r="B256" s="1"/>
-      <c r="C256" s="1"/>
+      <c r="B256" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="C256" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A257" s="1">
         <v>256</v>
       </c>
-      <c r="B257" s="1"/>
-      <c r="C257" s="1"/>
+      <c r="B257" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C257" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A258" s="1">
         <v>257</v>
       </c>
-      <c r="B258" s="1"/>
-      <c r="C258" s="1"/>
+      <c r="B258" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="C258" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A259" s="1">
         <v>258</v>
       </c>
-      <c r="B259" s="1"/>
-      <c r="C259" s="1"/>
+      <c r="B259" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C259" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A260" s="1">
         <v>259</v>
       </c>
-      <c r="B260" s="1"/>
-      <c r="C260" s="1"/>
+      <c r="B260" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C260" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A261" s="1">
         <v>260</v>
       </c>
-      <c r="B261" s="1"/>
-      <c r="C261" s="1"/>
+      <c r="B261" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="C261" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A262" s="1">
         <v>261</v>
       </c>
-      <c r="B262" s="1"/>
-      <c r="C262" s="1"/>
+      <c r="B262" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C262" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A263" s="1">
         <v>262</v>
       </c>
-      <c r="B263" s="1"/>
-      <c r="C263" s="1"/>
+      <c r="B263" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C263" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A264" s="1">
         <v>263</v>
       </c>
-      <c r="B264" s="1"/>
-      <c r="C264" s="1"/>
+      <c r="B264" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C264" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A265" s="1">
         <v>264</v>
       </c>
-      <c r="B265" s="1"/>
-      <c r="C265" s="1"/>
+      <c r="B265" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="C265" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A266" s="1">
         <v>265</v>
       </c>
-      <c r="B266" s="1"/>
-      <c r="C266" s="1"/>
+      <c r="B266" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C266" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A267" s="1">
         <v>266</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>414</v>
-      </c>
-      <c r="C267" s="1"/>
+        <v>450</v>
+      </c>
+      <c r="C267" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A268" s="1">
         <v>267</v>
       </c>
       <c r="B268" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="C268" s="1"/>
+        <v>119</v>
+      </c>
+      <c r="C268" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A269" s="1">
         <v>268</v>
       </c>
       <c r="B269" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C269" s="1">
         <v>1</v>
@@ -9357,16 +9371,18 @@
         <v>269</v>
       </c>
       <c r="B270" s="1" t="s">
-        <v>506</v>
-      </c>
-      <c r="C270" s="1"/>
+        <v>252</v>
+      </c>
+      <c r="C270" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A271" s="1">
         <v>270</v>
       </c>
       <c r="B271" s="1" t="s">
-        <v>122</v>
+        <v>499</v>
       </c>
       <c r="C271" s="1">
         <v>1</v>
@@ -9377,7 +9393,7 @@
         <v>271</v>
       </c>
       <c r="B272" s="1" t="s">
-        <v>415</v>
+        <v>472</v>
       </c>
       <c r="C272" s="1">
         <v>1</v>
@@ -9388,57 +9404,41 @@
         <v>272</v>
       </c>
       <c r="B273" s="1" t="s">
-        <v>429</v>
-      </c>
-      <c r="C273" s="1">
-        <v>1</v>
+        <v>501</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A274" s="1">
         <v>273</v>
       </c>
-      <c r="B274" s="1"/>
-      <c r="C274" s="1"/>
+      <c r="B274" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C274" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A275" s="1">
         <v>274</v>
       </c>
-      <c r="B275" s="1" t="s">
-        <v>416</v>
-      </c>
-      <c r="C275" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A276" s="1">
         <v>275</v>
       </c>
-      <c r="B276" s="1" t="s">
-        <v>430</v>
-      </c>
-      <c r="C276" s="1"/>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A277" s="1">
         <v>276</v>
       </c>
-      <c r="B277" s="1" t="s">
-        <v>507</v>
-      </c>
-      <c r="C277" s="1"/>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A278" s="1">
         <v>277</v>
       </c>
       <c r="B278" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="C278" s="1">
-        <v>1</v>
+        <v>414</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.2">
@@ -9446,16 +9446,15 @@
         <v>278</v>
       </c>
       <c r="B279" s="1" t="s">
-        <v>417</v>
-      </c>
-      <c r="C279" s="1"/>
+        <v>504</v>
+      </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A280" s="1">
         <v>279</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>502</v>
+        <v>121</v>
       </c>
       <c r="C280" s="1">
         <v>1</v>
@@ -9465,15 +9464,16 @@
       <c r="A281" s="1">
         <v>280</v>
       </c>
-      <c r="B281" s="1"/>
-      <c r="C281" s="1"/>
+      <c r="B281" s="1" t="s">
+        <v>506</v>
+      </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A282" s="1">
         <v>281</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C282" s="1">
         <v>1</v>
@@ -9484,7 +9484,7 @@
         <v>282</v>
       </c>
       <c r="B283" s="1" t="s">
-        <v>283</v>
+        <v>538</v>
       </c>
       <c r="C283" s="1">
         <v>1</v>
@@ -9494,15 +9494,19 @@
       <c r="A284" s="1">
         <v>283</v>
       </c>
-      <c r="B284" s="1"/>
-      <c r="C284" s="1"/>
+      <c r="B284" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="C284" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A285" s="1">
         <v>284</v>
       </c>
       <c r="B285" s="1" t="s">
-        <v>394</v>
+        <v>429</v>
       </c>
       <c r="C285" s="1">
         <v>1</v>
@@ -9513,7 +9517,7 @@
         <v>285</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>503</v>
+        <v>416</v>
       </c>
       <c r="C286" s="1">
         <v>1</v>
@@ -9524,10 +9528,7 @@
         <v>286</v>
       </c>
       <c r="B287" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="C287" s="1">
-        <v>1</v>
+        <v>430</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.2">
@@ -9535,10 +9536,7 @@
         <v>287</v>
       </c>
       <c r="B288" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C288" s="1">
-        <v>1</v>
+        <v>507</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.2">
@@ -9546,7 +9544,7 @@
         <v>288</v>
       </c>
       <c r="B289" s="1" t="s">
-        <v>127</v>
+        <v>284</v>
       </c>
       <c r="C289" s="1">
         <v>1</v>
@@ -9557,10 +9555,7 @@
         <v>289</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C290" s="1">
-        <v>1</v>
+        <v>417</v>
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.2">
@@ -9568,7 +9563,7 @@
         <v>290</v>
       </c>
       <c r="B291" s="1" t="s">
-        <v>129</v>
+        <v>502</v>
       </c>
       <c r="C291" s="1">
         <v>1</v>
@@ -9578,15 +9573,19 @@
       <c r="A292" s="1">
         <v>291</v>
       </c>
-      <c r="B292" s="1"/>
-      <c r="C292" s="1"/>
+      <c r="B292" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C292" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A293" s="1">
         <v>292</v>
       </c>
       <c r="B293" s="1" t="s">
-        <v>131</v>
+        <v>283</v>
       </c>
       <c r="C293" s="1">
         <v>1</v>
@@ -9597,7 +9596,7 @@
         <v>293</v>
       </c>
       <c r="B294" s="1" t="s">
-        <v>132</v>
+        <v>394</v>
       </c>
       <c r="C294" s="1">
         <v>1</v>
@@ -9607,15 +9606,16 @@
       <c r="A295" s="1">
         <v>294</v>
       </c>
-      <c r="B295" s="1"/>
-      <c r="C295" s="1"/>
+      <c r="B295" s="1" t="s">
+        <v>503</v>
+      </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A296" s="1">
         <v>295</v>
       </c>
       <c r="B296" s="1" t="s">
-        <v>431</v>
+        <v>125</v>
       </c>
       <c r="C296" s="1">
         <v>1</v>
@@ -9626,7 +9626,7 @@
         <v>296</v>
       </c>
       <c r="B297" s="1" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="C297" s="1">
         <v>1</v>
@@ -9637,16 +9637,18 @@
         <v>297</v>
       </c>
       <c r="B298" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="C298" s="1"/>
+        <v>127</v>
+      </c>
+      <c r="C298" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A299" s="1">
         <v>298</v>
       </c>
       <c r="B299" s="1" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C299" s="1">
         <v>1</v>
@@ -9657,7 +9659,7 @@
         <v>299</v>
       </c>
       <c r="B300" s="1" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C300" s="1">
         <v>1</v>
@@ -9667,22 +9669,30 @@
       <c r="A301" s="1">
         <v>300</v>
       </c>
-      <c r="B301" s="1"/>
-      <c r="C301" s="1"/>
+      <c r="B301" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C301" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A302" s="1">
         <v>301</v>
       </c>
-      <c r="B302" s="1"/>
-      <c r="C302" s="1"/>
+      <c r="B302" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C302" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A303" s="1">
         <v>302</v>
       </c>
       <c r="B303" s="1" t="s">
-        <v>140</v>
+        <v>431</v>
       </c>
       <c r="C303" s="1">
         <v>1</v>
@@ -9693,7 +9703,7 @@
         <v>303</v>
       </c>
       <c r="B304" s="1" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="C304" s="1">
         <v>1</v>
@@ -9704,10 +9714,7 @@
         <v>304</v>
       </c>
       <c r="B305" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C305" s="1">
-        <v>1</v>
+        <v>432</v>
       </c>
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.2">
@@ -9715,7 +9722,7 @@
         <v>305</v>
       </c>
       <c r="B306" s="1" t="s">
-        <v>505</v>
+        <v>134</v>
       </c>
       <c r="C306" s="1">
         <v>1</v>
@@ -9726,7 +9733,7 @@
         <v>306</v>
       </c>
       <c r="B307" s="1" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="C307" s="1">
         <v>1</v>
@@ -9737,7 +9744,7 @@
         <v>307</v>
       </c>
       <c r="B308" s="1" t="s">
-        <v>451</v>
+        <v>140</v>
       </c>
       <c r="C308" s="1">
         <v>1</v>
@@ -9748,7 +9755,7 @@
         <v>308</v>
       </c>
       <c r="B309" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C309" s="1">
         <v>1</v>
@@ -9759,7 +9766,7 @@
         <v>309</v>
       </c>
       <c r="B310" s="1" t="s">
-        <v>418</v>
+        <v>142</v>
       </c>
       <c r="C310" s="1">
         <v>1</v>
@@ -9770,7 +9777,7 @@
         <v>310</v>
       </c>
       <c r="B311" s="1" t="s">
-        <v>145</v>
+        <v>505</v>
       </c>
       <c r="C311" s="1">
         <v>1</v>
@@ -9780,15 +9787,19 @@
       <c r="A312" s="1">
         <v>311</v>
       </c>
-      <c r="B312" s="1"/>
-      <c r="C312" s="1"/>
+      <c r="B312" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C312" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A313" s="1">
         <v>312</v>
       </c>
       <c r="B313" s="1" t="s">
-        <v>146</v>
+        <v>451</v>
       </c>
       <c r="C313" s="1">
         <v>1</v>
@@ -9798,15 +9809,19 @@
       <c r="A314" s="1">
         <v>313</v>
       </c>
-      <c r="B314" s="1"/>
-      <c r="C314" s="1"/>
+      <c r="B314" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C314" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A315" s="1">
         <v>314</v>
       </c>
       <c r="B315" s="1" t="s">
-        <v>217</v>
+        <v>418</v>
       </c>
       <c r="C315" s="1">
         <v>1</v>
@@ -9817,7 +9832,7 @@
         <v>315</v>
       </c>
       <c r="B316" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C316" s="1">
         <v>1</v>
@@ -9828,7 +9843,7 @@
         <v>316</v>
       </c>
       <c r="B317" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C317" s="1">
         <v>1</v>
@@ -9838,15 +9853,19 @@
       <c r="A318" s="1">
         <v>317</v>
       </c>
-      <c r="B318" s="1"/>
-      <c r="C318" s="1"/>
+      <c r="B318" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C318" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A319" s="1">
         <v>318</v>
       </c>
       <c r="B319" s="1" t="s">
-        <v>433</v>
+        <v>147</v>
       </c>
       <c r="C319" s="1">
         <v>1</v>
@@ -9857,7 +9876,7 @@
         <v>319</v>
       </c>
       <c r="B320" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C320" s="1">
         <v>1</v>
@@ -9868,7 +9887,7 @@
         <v>320</v>
       </c>
       <c r="B321" s="1" t="s">
-        <v>151</v>
+        <v>433</v>
       </c>
       <c r="C321" s="1">
         <v>1</v>
@@ -9879,7 +9898,7 @@
         <v>321</v>
       </c>
       <c r="B322" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C322" s="1">
         <v>1</v>
@@ -9890,7 +9909,7 @@
         <v>322</v>
       </c>
       <c r="B323" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C323" s="1">
         <v>1</v>
@@ -9901,7 +9920,7 @@
         <v>323</v>
       </c>
       <c r="B324" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C324" s="1">
         <v>1</v>
@@ -9911,32 +9930,41 @@
       <c r="A325" s="1">
         <v>324</v>
       </c>
-      <c r="B325" s="3"/>
-      <c r="C325" s="3"/>
+      <c r="B325" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C325" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A326" s="1">
         <v>325</v>
       </c>
-      <c r="B326" s="3"/>
-      <c r="C326" s="3"/>
+      <c r="B326" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C326" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A327" s="1">
         <v>326</v>
       </c>
-      <c r="B327" s="1"/>
-      <c r="C327" s="1"/>
+      <c r="B327" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C327" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A328" s="1">
         <v>327</v>
       </c>
       <c r="B328" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C328" s="1">
-        <v>1</v>
+        <v>156</v>
       </c>
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.2">
@@ -9944,71 +9972,54 @@
         <v>328</v>
       </c>
       <c r="B329" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C329" s="1"/>
+        <v>157</v>
+      </c>
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A330" s="1">
         <v>329</v>
       </c>
       <c r="B330" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C330" s="1"/>
+        <v>158</v>
+      </c>
+      <c r="C330" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A331" s="1">
         <v>330</v>
       </c>
-      <c r="B331" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C331" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A332" s="1">
         <v>331</v>
       </c>
-      <c r="B332" s="1"/>
-      <c r="C332" s="1"/>
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A333" s="1">
         <v>332</v>
       </c>
-      <c r="B333" s="1"/>
-      <c r="C333" s="1"/>
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A334" s="1">
         <v>333</v>
       </c>
-      <c r="B334" s="1"/>
-      <c r="C334" s="1"/>
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A335" s="1">
         <v>334</v>
       </c>
-      <c r="B335" s="1"/>
-      <c r="C335" s="1"/>
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A336" s="1">
         <v>335</v>
       </c>
-      <c r="B336" s="1"/>
-      <c r="C336" s="1"/>
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A337" s="1">
         <v>336</v>
       </c>
-      <c r="B337" s="1"/>
-      <c r="C337" s="1"/>
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A338" s="1">
@@ -10039,7 +10050,6 @@
       <c r="B340" s="1" t="s">
         <v>508</v>
       </c>
-      <c r="C340" s="1"/>
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A341" s="1">
@@ -10100,10 +10110,10 @@
       <c r="A346" s="1">
         <v>345</v>
       </c>
-      <c r="B346" s="3" t="s">
+      <c r="B346" s="1" t="s">
         <v>480</v>
       </c>
-      <c r="C346" s="3">
+      <c r="C346" s="1">
         <v>1</v>
       </c>
     </row>
@@ -10158,7 +10168,6 @@
       <c r="B351" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="C351" s="1"/>
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A352" s="1">
@@ -10178,7 +10187,6 @@
       <c r="B353" s="1" t="s">
         <v>408</v>
       </c>
-      <c r="C353" s="1"/>
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A354" s="1">
@@ -10272,15 +10280,19 @@
       <c r="A362" s="1">
         <v>361</v>
       </c>
-      <c r="B362" s="1"/>
-      <c r="C362" s="1"/>
+      <c r="B362" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C362" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="363" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A363" s="1">
         <v>362</v>
       </c>
       <c r="B363" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C363" s="1">
         <v>1</v>
@@ -10291,10 +10303,7 @@
         <v>363</v>
       </c>
       <c r="B364" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="C364" s="1">
-        <v>1</v>
+        <v>175</v>
       </c>
     </row>
     <row r="365" spans="1:3" x14ac:dyDescent="0.2">
@@ -10302,19 +10311,18 @@
         <v>364</v>
       </c>
       <c r="B365" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="C365" s="1"/>
+        <v>456</v>
+      </c>
+      <c r="C365" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A366" s="1">
         <v>365</v>
       </c>
       <c r="B366" s="1" t="s">
-        <v>456</v>
-      </c>
-      <c r="C366" s="1">
-        <v>1</v>
+        <v>509</v>
       </c>
     </row>
     <row r="367" spans="1:3" x14ac:dyDescent="0.2">
@@ -10322,16 +10330,18 @@
         <v>366</v>
       </c>
       <c r="B367" s="1" t="s">
-        <v>509</v>
-      </c>
-      <c r="C367" s="1"/>
+        <v>334</v>
+      </c>
+      <c r="C367" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="368" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A368" s="1">
         <v>367</v>
       </c>
       <c r="B368" s="1" t="s">
-        <v>334</v>
+        <v>176</v>
       </c>
       <c r="C368" s="1">
         <v>1</v>
@@ -10342,7 +10352,7 @@
         <v>368</v>
       </c>
       <c r="B369" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C369" s="1">
         <v>1</v>
@@ -10353,7 +10363,7 @@
         <v>369</v>
       </c>
       <c r="B370" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C370" s="1">
         <v>1</v>
@@ -10363,26 +10373,16 @@
       <c r="A371" s="1">
         <v>370</v>
       </c>
-      <c r="B371" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C371" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A372" s="1">
         <v>371</v>
       </c>
-      <c r="B372" s="1"/>
-      <c r="C372" s="1"/>
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A373" s="1">
         <v>372</v>
       </c>
-      <c r="B373" s="1"/>
-      <c r="C373" s="1"/>
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A374" s="1">
@@ -10391,7 +10391,6 @@
       <c r="B374" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="C374" s="1"/>
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A375" s="1">
@@ -10455,7 +10454,6 @@
       <c r="B380" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="C380" s="1"/>
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A381" s="1">
@@ -10486,7 +10484,6 @@
       <c r="B383" s="1" t="s">
         <v>512</v>
       </c>
-      <c r="C383" s="1"/>
     </row>
     <row r="384" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A384" s="1">
@@ -10605,7 +10602,6 @@
       <c r="B394" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="C394" s="1"/>
     </row>
     <row r="395" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A395" s="1">
@@ -10647,7 +10643,6 @@
       <c r="B398" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="C398" s="1"/>
     </row>
     <row r="399" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A399" s="1">
@@ -10664,71 +10659,51 @@
       <c r="A400" s="1">
         <v>399</v>
       </c>
-      <c r="B400" s="1"/>
-      <c r="C400" s="1"/>
     </row>
     <row r="401" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A401" s="1">
         <v>400</v>
       </c>
-      <c r="B401" s="1"/>
-      <c r="C401" s="1"/>
     </row>
     <row r="402" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A402" s="1">
         <v>401</v>
       </c>
-      <c r="B402" s="1"/>
-      <c r="C402" s="1"/>
     </row>
     <row r="403" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A403" s="1">
         <v>402</v>
       </c>
-      <c r="B403" s="1"/>
-      <c r="C403" s="1"/>
     </row>
     <row r="404" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A404" s="1">
         <v>403</v>
       </c>
-      <c r="B404" s="1"/>
-      <c r="C404" s="1"/>
     </row>
     <row r="405" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A405" s="1">
         <v>404</v>
       </c>
-      <c r="B405" s="1"/>
-      <c r="C405" s="1"/>
     </row>
     <row r="406" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A406" s="1">
         <v>405</v>
       </c>
-      <c r="B406" s="1"/>
-      <c r="C406" s="1"/>
     </row>
     <row r="407" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A407" s="1">
         <v>406</v>
       </c>
-      <c r="B407" s="1"/>
-      <c r="C407" s="1"/>
     </row>
     <row r="408" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A408" s="1">
         <v>407</v>
       </c>
-      <c r="B408" s="1"/>
-      <c r="C408" s="1"/>
     </row>
     <row r="409" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A409" s="1">
         <v>408</v>
       </c>
-      <c r="B409" s="1"/>
-      <c r="C409" s="1"/>
     </row>
     <row r="410" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A410" s="1">
@@ -10757,7 +10732,7 @@
         <v>411</v>
       </c>
       <c r="B412" s="1" t="s">
-        <v>517</v>
+        <v>539</v>
       </c>
       <c r="C412" s="1">
         <v>1</v>
@@ -10768,7 +10743,7 @@
         <v>412</v>
       </c>
       <c r="B413" s="1" t="s">
-        <v>184</v>
+        <v>517</v>
       </c>
       <c r="C413" s="1">
         <v>1</v>
@@ -10779,19 +10754,18 @@
         <v>413</v>
       </c>
       <c r="B414" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="C414" s="1"/>
+        <v>184</v>
+      </c>
+      <c r="C414" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="415" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A415" s="1">
         <v>414</v>
       </c>
       <c r="B415" s="1" t="s">
-        <v>438</v>
-      </c>
-      <c r="C415" s="1">
-        <v>1</v>
+        <v>185</v>
       </c>
     </row>
     <row r="416" spans="1:3" x14ac:dyDescent="0.2">
@@ -10799,7 +10773,7 @@
         <v>415</v>
       </c>
       <c r="B416" s="1" t="s">
-        <v>186</v>
+        <v>438</v>
       </c>
       <c r="C416" s="1">
         <v>1</v>
@@ -10810,7 +10784,7 @@
         <v>416</v>
       </c>
       <c r="B417" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C417" s="1">
         <v>1</v>
@@ -10821,7 +10795,7 @@
         <v>417</v>
       </c>
       <c r="B418" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C418" s="1">
         <v>1</v>
@@ -10832,7 +10806,7 @@
         <v>418</v>
       </c>
       <c r="B419" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C419" s="1">
         <v>1</v>
@@ -10843,7 +10817,7 @@
         <v>419</v>
       </c>
       <c r="B420" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C420" s="1">
         <v>1</v>
@@ -10854,7 +10828,7 @@
         <v>420</v>
       </c>
       <c r="B421" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C421" s="1">
         <v>1</v>
@@ -10865,37 +10839,37 @@
         <v>421</v>
       </c>
       <c r="B422" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="C422" s="1"/>
+        <v>191</v>
+      </c>
+      <c r="C422" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="423" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A423" s="1">
         <v>422</v>
       </c>
       <c r="B423" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="C423" s="1">
-        <v>1</v>
+        <v>192</v>
       </c>
     </row>
     <row r="424" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A424" s="1">
         <v>423</v>
       </c>
-      <c r="B424" s="1"/>
-      <c r="C424" s="1"/>
+      <c r="B424" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C424" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="425" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A425" s="1">
         <v>424</v>
       </c>
       <c r="B425" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C425" s="1">
-        <v>1</v>
+        <v>540</v>
       </c>
     </row>
     <row r="426" spans="1:3" x14ac:dyDescent="0.2">
@@ -10903,7 +10877,7 @@
         <v>425</v>
       </c>
       <c r="B426" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C426" s="1">
         <v>1</v>
@@ -10914,16 +10888,15 @@
         <v>426</v>
       </c>
       <c r="B427" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="C427" s="1"/>
+        <v>541</v>
+      </c>
     </row>
     <row r="428" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A428" s="1">
         <v>427</v>
       </c>
       <c r="B428" s="1" t="s">
-        <v>293</v>
+        <v>542</v>
       </c>
       <c r="C428" s="1">
         <v>1</v>
@@ -10934,10 +10907,7 @@
         <v>428</v>
       </c>
       <c r="B429" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="C429" s="1">
-        <v>1</v>
+        <v>543</v>
       </c>
     </row>
     <row r="430" spans="1:3" x14ac:dyDescent="0.2">
@@ -10945,7 +10915,7 @@
         <v>429</v>
       </c>
       <c r="B430" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C430" s="1">
         <v>1</v>
@@ -10956,10 +10926,7 @@
         <v>430</v>
       </c>
       <c r="B431" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="C431" s="1">
-        <v>1</v>
+        <v>198</v>
       </c>
     </row>
     <row r="432" spans="1:3" x14ac:dyDescent="0.2">
@@ -10967,7 +10934,7 @@
         <v>431</v>
       </c>
       <c r="B432" s="1" t="s">
-        <v>200</v>
+        <v>293</v>
       </c>
       <c r="C432" s="1">
         <v>1</v>
@@ -10978,16 +10945,18 @@
         <v>432</v>
       </c>
       <c r="B433" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="C433" s="1"/>
+        <v>294</v>
+      </c>
+      <c r="C433" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="434" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A434" s="1">
         <v>433</v>
       </c>
       <c r="B434" s="1" t="s">
-        <v>464</v>
+        <v>199</v>
       </c>
       <c r="C434" s="1">
         <v>1</v>
@@ -10998,7 +10967,7 @@
         <v>434</v>
       </c>
       <c r="B435" s="1" t="s">
-        <v>201</v>
+        <v>231</v>
       </c>
       <c r="C435" s="1">
         <v>1</v>
@@ -11009,25 +10978,26 @@
         <v>435</v>
       </c>
       <c r="B436" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="C436" s="1"/>
+        <v>200</v>
+      </c>
+      <c r="C436" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="437" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A437" s="1">
         <v>436</v>
       </c>
       <c r="B437" s="1" t="s">
-        <v>440</v>
-      </c>
-      <c r="C437" s="1"/>
+        <v>439</v>
+      </c>
     </row>
     <row r="438" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A438" s="1">
         <v>437</v>
       </c>
       <c r="B438" s="1" t="s">
-        <v>203</v>
+        <v>464</v>
       </c>
       <c r="C438" s="1">
         <v>1</v>
@@ -11038,7 +11008,7 @@
         <v>438</v>
       </c>
       <c r="B439" s="1" t="s">
-        <v>518</v>
+        <v>544</v>
       </c>
       <c r="C439" s="1">
         <v>1</v>
@@ -11049,7 +11019,7 @@
         <v>439</v>
       </c>
       <c r="B440" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C440" s="1">
         <v>1</v>
@@ -11060,34 +11030,34 @@
         <v>440</v>
       </c>
       <c r="B441" s="1" t="s">
-        <v>441</v>
-      </c>
-      <c r="C441" s="1"/>
+        <v>202</v>
+      </c>
     </row>
     <row r="442" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A442" s="1">
         <v>441</v>
       </c>
       <c r="B442" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="C442" s="1">
-        <v>1</v>
+        <v>440</v>
       </c>
     </row>
     <row r="443" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A443" s="1">
         <v>442</v>
       </c>
-      <c r="B443" s="1"/>
-      <c r="C443" s="1"/>
+      <c r="B443" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C443" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="444" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A444" s="1">
         <v>443</v>
       </c>
       <c r="B444" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C444" s="1">
         <v>1</v>
@@ -11097,96 +11067,117 @@
       <c r="A445" s="1">
         <v>444</v>
       </c>
-      <c r="B445" s="1"/>
-      <c r="C445" s="1"/>
+      <c r="B445" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C445" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="446" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A446" s="1">
         <v>445</v>
       </c>
       <c r="B446" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="C446" s="1">
-        <v>1</v>
+        <v>441</v>
       </c>
     </row>
     <row r="447" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A447" s="1">
         <v>446</v>
       </c>
-      <c r="B447" s="1"/>
-      <c r="C447" s="1"/>
+      <c r="B447" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C447" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="448" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A448" s="1">
         <v>447</v>
       </c>
-      <c r="B448" s="1"/>
-      <c r="C448" s="1"/>
+      <c r="B448" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="C448" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="449" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A449" s="1">
         <v>448</v>
       </c>
-      <c r="B449" s="1"/>
-      <c r="C449" s="1"/>
+      <c r="B449" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="C449" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="450" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A450" s="1">
         <v>449</v>
       </c>
-      <c r="B450" s="1"/>
-      <c r="C450" s="1"/>
+      <c r="B450" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="C450" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="451" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A451" s="1">
         <v>450</v>
       </c>
-      <c r="B451" s="1"/>
-      <c r="C451" s="1"/>
+      <c r="B451" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="C451" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="452" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A452" s="1">
         <v>451</v>
       </c>
-      <c r="B452" s="1"/>
-      <c r="C452" s="1"/>
+      <c r="B452" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="C452" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="453" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A453" s="1">
         <v>452</v>
       </c>
-      <c r="B453" s="1"/>
-      <c r="C453" s="1"/>
+      <c r="B453" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="C453" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="454" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A454" s="1">
         <v>453</v>
       </c>
-      <c r="B454" s="1"/>
-      <c r="C454" s="1"/>
     </row>
     <row r="455" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A455" s="1">
         <v>454</v>
       </c>
-      <c r="B455" s="1"/>
-      <c r="C455" s="1"/>
     </row>
     <row r="456" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A456" s="1">
         <v>455</v>
       </c>
-      <c r="B456" s="1"/>
-      <c r="C456" s="1"/>
     </row>
     <row r="457" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A457" s="1">
         <v>456</v>
       </c>
-      <c r="B457" s="1"/>
-      <c r="C457" s="1"/>
     </row>
     <row r="458" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A458" s="1">
@@ -11228,7 +11219,6 @@
       <c r="B461" s="1" t="s">
         <v>520</v>
       </c>
-      <c r="C461" s="1"/>
     </row>
     <row r="462" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A462" s="1">
@@ -11237,7 +11227,6 @@
       <c r="B462" s="1" t="s">
         <v>521</v>
       </c>
-      <c r="C462" s="1"/>
     </row>
     <row r="463" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A463" s="1">
@@ -11287,10 +11276,10 @@
       <c r="A467" s="1">
         <v>466</v>
       </c>
-      <c r="B467" s="3" t="s">
+      <c r="B467" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="C467" s="3">
+      <c r="C467" s="1">
         <v>1</v>
       </c>
     </row>
@@ -11301,7 +11290,6 @@
       <c r="B468" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="C468" s="1"/>
     </row>
     <row r="469" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A469" s="1">
@@ -11409,7 +11397,6 @@
       <c r="B478" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="C478" s="1"/>
     </row>
     <row r="479" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A479" s="1">
@@ -11426,15 +11413,11 @@
       <c r="A480" s="1">
         <v>479</v>
       </c>
-      <c r="B480" s="1"/>
-      <c r="C480" s="1"/>
-    </row>
-    <row r="481" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="481" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A481" s="1">
         <v>480</v>
       </c>
-      <c r="B481" s="1"/>
-      <c r="C481" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updating decks and binder
</commit_message>
<xml_diff>
--- a/data/binder/Binder.xlsx
+++ b/data/binder/Binder.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Dados/MTG/EDH DeckHelper/EDH-DeckHelper/data/binder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB8C596F-4205-E94A-B220-A17AE16E4D2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEDDEB50-26AB-9243-8FBB-9325B0E75852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="12660" windowHeight="15540" activeTab="1" xr2:uid="{7ABBCC85-5F92-6F41-92E4-65212D317CF6}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="548">
   <si>
     <t>Slot</t>
   </si>
@@ -1663,6 +1663,30 @@
   </si>
   <si>
     <t>Heartwarming Redemption</t>
+  </si>
+  <si>
+    <t>Ghostly Prison</t>
+  </si>
+  <si>
+    <t>Sphere of Safety</t>
+  </si>
+  <si>
+    <t>Propaganda</t>
+  </si>
+  <si>
+    <t>Fierce Guardianship</t>
+  </si>
+  <si>
+    <t>Wheel of Misfortune</t>
+  </si>
+  <si>
+    <t>Volrath's Stronghold</t>
+  </si>
+  <si>
+    <t>Kozilek, Butcher of Truth</t>
+  </si>
+  <si>
+    <t>Helm of Obidience</t>
   </si>
 </sst>
 </file>
@@ -6705,8 +6729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5953B7FC-4B75-B146-8A26-6CA09B5F3C99}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A309" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B335" sqref="B335"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8796,7 +8820,7 @@
         <v>211</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C212" s="1">
         <v>1</v>
@@ -8807,7 +8831,7 @@
         <v>212</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C213" s="1">
         <v>1</v>
@@ -8818,7 +8842,7 @@
         <v>213</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>91</v>
+        <v>422</v>
       </c>
       <c r="C214" s="1">
         <v>1</v>
@@ -8829,7 +8853,7 @@
         <v>214</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>422</v>
+        <v>387</v>
       </c>
       <c r="C215" s="1">
         <v>1</v>
@@ -8840,7 +8864,7 @@
         <v>215</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>387</v>
+        <v>111</v>
       </c>
       <c r="C216" s="1">
         <v>1</v>
@@ -8851,7 +8875,7 @@
         <v>216</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C217" s="1">
         <v>1</v>
@@ -8862,7 +8886,7 @@
         <v>217</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>105</v>
+        <v>388</v>
       </c>
       <c r="C218" s="1">
         <v>1</v>
@@ -8873,7 +8897,7 @@
         <v>218</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>388</v>
+        <v>112</v>
       </c>
       <c r="C219" s="1">
         <v>1</v>
@@ -8884,7 +8908,7 @@
         <v>219</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="C220" s="1">
         <v>1</v>
@@ -8895,7 +8919,7 @@
         <v>220</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="C221" s="1">
         <v>1</v>
@@ -8906,7 +8930,7 @@
         <v>221</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>106</v>
+        <v>423</v>
       </c>
       <c r="C222" s="1">
         <v>1</v>
@@ -8917,7 +8941,7 @@
         <v>222</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>423</v>
+        <v>97</v>
       </c>
       <c r="C223" s="1">
         <v>1</v>
@@ -8928,7 +8952,7 @@
         <v>223</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>97</v>
+        <v>389</v>
       </c>
       <c r="C224" s="1">
         <v>1</v>
@@ -8939,7 +8963,7 @@
         <v>224</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>389</v>
+        <v>378</v>
       </c>
       <c r="C225" s="1">
         <v>1</v>
@@ -8950,7 +8974,7 @@
         <v>225</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C226" s="1">
         <v>1</v>
@@ -8961,7 +8985,7 @@
         <v>226</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C227" s="1">
         <v>1</v>
@@ -8972,7 +8996,7 @@
         <v>227</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>380</v>
+        <v>99</v>
       </c>
       <c r="C228" s="1">
         <v>1</v>
@@ -8983,7 +9007,7 @@
         <v>228</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>99</v>
+        <v>381</v>
       </c>
       <c r="C229" s="1">
         <v>1</v>
@@ -8994,7 +9018,7 @@
         <v>229</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>381</v>
+        <v>113</v>
       </c>
       <c r="C230" s="1">
         <v>1</v>
@@ -9005,7 +9029,7 @@
         <v>230</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="C231" s="1">
         <v>1</v>
@@ -9016,7 +9040,7 @@
         <v>231</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="C232" s="1">
         <v>1</v>
@@ -9027,7 +9051,7 @@
         <v>232</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>114</v>
+        <v>382</v>
       </c>
       <c r="C233" s="1">
         <v>1</v>
@@ -9038,7 +9062,7 @@
         <v>233</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>382</v>
+        <v>115</v>
       </c>
       <c r="C234" s="1">
         <v>1</v>
@@ -9049,7 +9073,7 @@
         <v>234</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>115</v>
+        <v>522</v>
       </c>
       <c r="C235" s="1">
         <v>1</v>
@@ -9060,7 +9084,7 @@
         <v>235</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>522</v>
+        <v>285</v>
       </c>
       <c r="C236" s="1">
         <v>1</v>
@@ -9071,7 +9095,7 @@
         <v>236</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>285</v>
+        <v>390</v>
       </c>
       <c r="C237" s="1">
         <v>1</v>
@@ -9082,7 +9106,7 @@
         <v>237</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C238" s="1">
         <v>1</v>
@@ -9093,7 +9117,7 @@
         <v>238</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="C239" s="1">
         <v>1</v>
@@ -9104,7 +9128,7 @@
         <v>239</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>393</v>
+        <v>424</v>
       </c>
       <c r="C240" s="1">
         <v>1</v>
@@ -9115,7 +9139,7 @@
         <v>240</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C241" s="1">
         <v>1</v>
@@ -9126,7 +9150,7 @@
         <v>241</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>425</v>
+        <v>492</v>
       </c>
       <c r="C242" s="1">
         <v>1</v>
@@ -9136,12 +9160,6 @@
       <c r="A243" s="1">
         <v>242</v>
       </c>
-      <c r="B243" s="1" t="s">
-        <v>492</v>
-      </c>
-      <c r="C243" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A244" s="1">
@@ -9231,7 +9249,7 @@
         <v>256</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>405</v>
+        <v>540</v>
       </c>
       <c r="C257" s="1">
         <v>1</v>
@@ -9242,7 +9260,7 @@
         <v>257</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>118</v>
+        <v>405</v>
       </c>
       <c r="C258" s="1">
         <v>1</v>
@@ -9253,7 +9271,7 @@
         <v>258</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>525</v>
+        <v>541</v>
       </c>
       <c r="C259" s="1">
         <v>1</v>
@@ -9264,7 +9282,7 @@
         <v>259</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>426</v>
+        <v>118</v>
       </c>
       <c r="C260" s="1">
         <v>1</v>
@@ -9275,7 +9293,7 @@
         <v>260</v>
       </c>
       <c r="B261" s="1" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="C261" s="1">
         <v>1</v>
@@ -9286,7 +9304,7 @@
         <v>261</v>
       </c>
       <c r="B262" s="1" t="s">
-        <v>120</v>
+        <v>426</v>
       </c>
       <c r="C262" s="1">
         <v>1</v>
@@ -9297,7 +9315,7 @@
         <v>262</v>
       </c>
       <c r="B263" s="1" t="s">
-        <v>472</v>
+        <v>524</v>
       </c>
       <c r="C263" s="1">
         <v>1</v>
@@ -9308,7 +9326,7 @@
         <v>263</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>447</v>
+        <v>120</v>
       </c>
       <c r="C264" s="1">
         <v>1</v>
@@ -9318,11 +9336,23 @@
       <c r="A265" s="1">
         <v>264</v>
       </c>
+      <c r="B265" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="C265" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A266" s="1">
         <v>265</v>
       </c>
+      <c r="B266" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="C266" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A267" s="1">
@@ -9439,7 +9469,7 @@
         <v>282</v>
       </c>
       <c r="B283" s="1" t="s">
-        <v>283</v>
+        <v>542</v>
       </c>
       <c r="C283" s="1">
         <v>1</v>
@@ -9450,7 +9480,7 @@
         <v>283</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>394</v>
+        <v>283</v>
       </c>
       <c r="C284" s="1">
         <v>1</v>
@@ -9461,7 +9491,7 @@
         <v>284</v>
       </c>
       <c r="B285" s="1" t="s">
-        <v>125</v>
+        <v>394</v>
       </c>
       <c r="C285" s="1">
         <v>1</v>
@@ -9472,7 +9502,7 @@
         <v>285</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C286" s="1">
         <v>1</v>
@@ -9483,7 +9513,7 @@
         <v>286</v>
       </c>
       <c r="B287" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C287" s="1">
         <v>1</v>
@@ -9494,7 +9524,7 @@
         <v>287</v>
       </c>
       <c r="B288" s="1" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C288" s="1">
         <v>1</v>
@@ -9505,7 +9535,7 @@
         <v>288</v>
       </c>
       <c r="B289" s="1" t="s">
-        <v>141</v>
+        <v>543</v>
       </c>
       <c r="C289" s="1">
         <v>1</v>
@@ -9516,7 +9546,7 @@
         <v>289</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>427</v>
+        <v>135</v>
       </c>
       <c r="C290" s="1">
         <v>1</v>
@@ -9527,7 +9557,7 @@
         <v>290</v>
       </c>
       <c r="B291" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C291" s="1">
         <v>1</v>
@@ -9538,7 +9568,7 @@
         <v>291</v>
       </c>
       <c r="B292" s="1" t="s">
-        <v>145</v>
+        <v>427</v>
       </c>
       <c r="C292" s="1">
         <v>1</v>
@@ -9549,7 +9579,7 @@
         <v>292</v>
       </c>
       <c r="B293" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C293" s="1">
         <v>1</v>
@@ -9560,7 +9590,7 @@
         <v>293</v>
       </c>
       <c r="B294" s="1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C294" s="1">
         <v>1</v>
@@ -9571,7 +9601,7 @@
         <v>294</v>
       </c>
       <c r="B295" s="1" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="C295" s="1">
         <v>1</v>
@@ -9582,7 +9612,7 @@
         <v>295</v>
       </c>
       <c r="B296" s="1" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="C296" s="1">
         <v>1</v>
@@ -9592,6 +9622,12 @@
       <c r="A297" s="1">
         <v>296</v>
       </c>
+      <c r="B297" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C297" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A298" s="1">
@@ -9897,12 +9933,6 @@
       <c r="A334" s="1">
         <v>333</v>
       </c>
-      <c r="B334" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C334" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A335" s="1">
@@ -10126,6 +10156,12 @@
       <c r="A363" s="1">
         <v>362</v>
       </c>
+      <c r="B363" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="C363" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="364" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A364" s="1">
@@ -10441,354 +10477,354 @@
         <v>399</v>
       </c>
     </row>
-    <row r="401" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A401" s="1">
         <v>400</v>
       </c>
     </row>
-    <row r="402" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A402" s="1">
         <v>401</v>
       </c>
     </row>
-    <row r="403" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="403" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A403" s="1">
         <v>402</v>
       </c>
     </row>
-    <row r="404" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="404" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A404" s="1">
         <v>403</v>
       </c>
     </row>
-    <row r="405" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A405" s="1">
         <v>404</v>
       </c>
     </row>
-    <row r="406" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A406" s="1">
         <v>405</v>
       </c>
     </row>
-    <row r="407" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A407" s="1">
         <v>406</v>
       </c>
     </row>
-    <row r="408" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A408" s="1">
         <v>407</v>
       </c>
     </row>
-    <row r="409" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A409" s="1">
         <v>408</v>
       </c>
     </row>
-    <row r="410" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A410" s="1">
         <v>409</v>
       </c>
-    </row>
-    <row r="411" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B410" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="C410" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="411" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A411" s="1">
         <v>410</v>
       </c>
-    </row>
-    <row r="412" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B411" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="C411" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="412" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A412" s="1">
         <v>411</v>
       </c>
-    </row>
-    <row r="413" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B412" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="C412" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="413" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A413" s="1">
         <v>412</v>
       </c>
-    </row>
-    <row r="414" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B413" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="C413" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="414" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A414" s="1">
         <v>413</v>
       </c>
-    </row>
-    <row r="415" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B414" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="C414" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="415" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A415" s="1">
         <v>414</v>
       </c>
-    </row>
-    <row r="416" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B415" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="C415" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="416" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A416" s="1">
         <v>415</v>
       </c>
-    </row>
-    <row r="417" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B416" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="C416" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="417" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A417" s="1">
         <v>416</v>
       </c>
-    </row>
-    <row r="418" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B417" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C417" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="418" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A418" s="1">
         <v>417</v>
       </c>
-    </row>
-    <row r="419" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B418" s="1" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="419" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A419" s="1">
         <v>418</v>
       </c>
-    </row>
-    <row r="420" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B419" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="C419" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="420" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A420" s="1">
         <v>419</v>
       </c>
-    </row>
-    <row r="421" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B420" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="C420" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="421" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A421" s="1">
         <v>420</v>
       </c>
-    </row>
-    <row r="422" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B421" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="C421" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="422" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A422" s="1">
         <v>421</v>
       </c>
-    </row>
-    <row r="423" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B422" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="C422" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="423" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A423" s="1">
         <v>422</v>
       </c>
-    </row>
-    <row r="424" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B423" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="C423" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="424" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A424" s="1">
         <v>423</v>
       </c>
-    </row>
-    <row r="425" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B424" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="C424" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="425" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A425" s="1">
         <v>424</v>
       </c>
-    </row>
-    <row r="426" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B425" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C425" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="426" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A426" s="1">
         <v>425</v>
       </c>
-    </row>
-    <row r="427" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B426" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="C426" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="427" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A427" s="1">
         <v>426</v>
       </c>
     </row>
-    <row r="428" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="428" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A428" s="1">
         <v>427</v>
       </c>
     </row>
-    <row r="429" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="429" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A429" s="1">
         <v>428</v>
       </c>
     </row>
-    <row r="430" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="430" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A430" s="1">
         <v>429</v>
       </c>
     </row>
-    <row r="431" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="431" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A431" s="1">
         <v>430</v>
       </c>
     </row>
-    <row r="432" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="432" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A432" s="1">
         <v>431</v>
       </c>
     </row>
-    <row r="433" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="433" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A433" s="1">
         <v>432</v>
       </c>
     </row>
-    <row r="434" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="434" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A434" s="1">
         <v>433</v>
       </c>
-      <c r="B434" s="1" t="s">
-        <v>440</v>
-      </c>
-      <c r="C434" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="435" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="435" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A435" s="1">
         <v>434</v>
       </c>
-      <c r="B435" s="1" t="s">
-        <v>477</v>
-      </c>
-      <c r="C435" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="436" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="436" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A436" s="1">
         <v>435</v>
       </c>
-      <c r="B436" s="1" t="s">
-        <v>442</v>
-      </c>
-      <c r="C436" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="437" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="437" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A437" s="1">
         <v>436</v>
       </c>
-      <c r="B437" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="C437" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="438" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="438" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A438" s="1">
         <v>437</v>
       </c>
-      <c r="B438" s="1" t="s">
-        <v>536</v>
-      </c>
-      <c r="C438" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="439" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="439" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A439" s="1">
         <v>438</v>
       </c>
-      <c r="B439" s="1" t="s">
-        <v>537</v>
-      </c>
-      <c r="C439" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="440" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="440" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A440" s="1">
         <v>439</v>
       </c>
-      <c r="B440" s="1" t="s">
-        <v>441</v>
-      </c>
-      <c r="C440" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="441" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="441" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A441" s="1">
         <v>440</v>
       </c>
-      <c r="B441" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="C441" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="442" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="442" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A442" s="1">
         <v>441</v>
       </c>
-      <c r="B442" s="1" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="443" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="443" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A443" s="1">
         <v>442</v>
       </c>
-      <c r="B443" s="1" t="s">
-        <v>443</v>
-      </c>
-      <c r="C443" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="444" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="444" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A444" s="1">
         <v>443</v>
       </c>
-      <c r="B444" s="1" t="s">
-        <v>444</v>
-      </c>
-      <c r="C444" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="445" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="445" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A445" s="1">
         <v>444</v>
       </c>
-      <c r="B445" s="1" t="s">
-        <v>539</v>
-      </c>
-      <c r="C445" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="446" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="446" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A446" s="1">
         <v>445</v>
       </c>
-      <c r="B446" s="1" t="s">
-        <v>445</v>
-      </c>
-      <c r="C446" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="447" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="447" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A447" s="1">
         <v>446</v>
       </c>
-      <c r="B447" s="1" t="s">
-        <v>446</v>
-      </c>
-      <c r="C447" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="448" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="448" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A448" s="1">
         <v>447</v>
-      </c>
-      <c r="B448" s="1" t="s">
-        <v>538</v>
-      </c>
-      <c r="C448" s="1">
-        <v>1</v>
       </c>
     </row>
     <row r="449" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A449" s="1">
         <v>448</v>
       </c>
-      <c r="B449" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="C449" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="450" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A450" s="1">
         <v>449</v>
       </c>
-      <c r="B450" s="1" t="s">
-        <v>535</v>
-      </c>
-      <c r="C450" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="451" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A451" s="1">
@@ -10829,113 +10865,197 @@
       <c r="A458" s="1">
         <v>457</v>
       </c>
+      <c r="B458" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="C458" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="459" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A459" s="1">
         <v>458</v>
       </c>
+      <c r="B459" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C459" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="460" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A460" s="1">
         <v>459</v>
       </c>
+      <c r="B460" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C460" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="461" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A461" s="1">
         <v>460</v>
       </c>
+      <c r="B461" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C461" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="462" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A462" s="1">
         <v>461</v>
       </c>
+      <c r="B462" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="C462" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="463" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A463" s="1">
         <v>462</v>
       </c>
+      <c r="B463" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C463" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="464" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A464" s="1">
         <v>463</v>
       </c>
-    </row>
-    <row r="465" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B464" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="C464" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="465" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A465" s="1">
         <v>464</v>
       </c>
-    </row>
-    <row r="466" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B465" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C465" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="466" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A466" s="1">
         <v>465</v>
       </c>
-    </row>
-    <row r="467" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B466" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C466" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="467" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A467" s="1">
         <v>466</v>
       </c>
-    </row>
-    <row r="468" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B467" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C467" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="468" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A468" s="1">
         <v>467</v>
       </c>
-    </row>
-    <row r="469" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B468" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C468" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="469" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A469" s="1">
         <v>468</v>
       </c>
-    </row>
-    <row r="470" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B469" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="C469" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="470" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A470" s="1">
         <v>469</v>
       </c>
-    </row>
-    <row r="471" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B470" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="C470" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="471" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A471" s="1">
         <v>470</v>
       </c>
-    </row>
-    <row r="472" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B471" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C471" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="472" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A472" s="1">
         <v>471</v>
       </c>
     </row>
-    <row r="473" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="473" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A473" s="1">
         <v>472</v>
       </c>
     </row>
-    <row r="474" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="474" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A474" s="1">
         <v>473</v>
       </c>
     </row>
-    <row r="475" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="475" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A475" s="1">
         <v>474</v>
       </c>
     </row>
-    <row r="476" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="476" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A476" s="1">
         <v>475</v>
       </c>
     </row>
-    <row r="477" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="477" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A477" s="1">
         <v>476</v>
       </c>
     </row>
-    <row r="478" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="478" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A478" s="1">
         <v>477</v>
       </c>
     </row>
-    <row r="479" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="479" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A479" s="1">
         <v>478</v>
       </c>
     </row>
-    <row r="480" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="480" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A480" s="1">
         <v>479</v>
       </c>

</xml_diff>

<commit_message>
Updating binder and collection
</commit_message>
<xml_diff>
--- a/data/binder/Binder.xlsx
+++ b/data/binder/Binder.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Dados/MTG/EDH DeckHelper/EDH-DeckHelper/data/binder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEDDEB50-26AB-9243-8FBB-9325B0E75852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3896E3D-8D54-D04D-A3C5-F1BE114305B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="12660" windowHeight="15540" activeTab="1" xr2:uid="{7ABBCC85-5F92-6F41-92E4-65212D317CF6}"/>
+    <workbookView xWindow="-23720" yWindow="460" windowWidth="13780" windowHeight="21140" activeTab="1" xr2:uid="{7ABBCC85-5F92-6F41-92E4-65212D317CF6}"/>
   </bookViews>
   <sheets>
     <sheet name="Dual" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="542">
   <si>
     <t>Slot</t>
   </si>
@@ -1476,9 +1476,6 @@
     <t>Kodama's Reach</t>
   </si>
   <si>
-    <t>Tymna the Weaver</t>
-  </si>
-  <si>
     <t>Karn's Bastion</t>
   </si>
   <si>
@@ -1611,9 +1608,6 @@
     <t>Alhammarret's Archive</t>
   </si>
   <si>
-    <t>The Chain Veil</t>
-  </si>
-  <si>
     <t>Authority of the Consuls</t>
   </si>
   <si>
@@ -1632,33 +1626,12 @@
     <t>Haunting Voyage</t>
   </si>
   <si>
-    <t>Liliana Vess</t>
-  </si>
-  <si>
-    <t>Liliana, Dreadhorde General</t>
-  </si>
-  <si>
-    <t>Ob Nixilis Reignited</t>
-  </si>
-  <si>
-    <t>The Elderspell</t>
-  </si>
-  <si>
-    <t>Sarkhan the Masterless</t>
-  </si>
-  <si>
     <t>Nature's Lore</t>
   </si>
   <si>
     <t>Vindicate</t>
   </si>
   <si>
-    <t>Nicol Bolas, Dragon-God</t>
-  </si>
-  <si>
-    <t>Nicol Bolas, God-Pharaoh</t>
-  </si>
-  <si>
     <t>Eerie Ultimatum</t>
   </si>
   <si>
@@ -1687,6 +1660,15 @@
   </si>
   <si>
     <t>Helm of Obidience</t>
+  </si>
+  <si>
+    <t>Dovin's Veto</t>
+  </si>
+  <si>
+    <t>Solemn Simulacrum</t>
+  </si>
+  <si>
+    <t>Nihil Spellbomb</t>
   </si>
 </sst>
 </file>
@@ -6729,8 +6711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5953B7FC-4B75-B146-8A26-6CA09B5F3C99}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A309" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B335" sqref="B335"/>
+    <sheetView tabSelected="1" topLeftCell="A117" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B180" sqref="B180:C189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7376,6 +7358,9 @@
       <c r="B65" s="1" t="s">
         <v>466</v>
       </c>
+      <c r="C65" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
@@ -7745,7 +7730,7 @@
         <v>101</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C102" s="1">
         <v>1</v>
@@ -7756,7 +7741,7 @@
         <v>102</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
@@ -7764,7 +7749,7 @@
         <v>103</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
@@ -7772,7 +7757,7 @@
         <v>104</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C105" s="1">
         <v>1</v>
@@ -7783,7 +7768,7 @@
         <v>105</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C106" s="1">
         <v>1</v>
@@ -7794,7 +7779,7 @@
         <v>106</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
@@ -7802,7 +7787,7 @@
         <v>107</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C108" s="1">
         <v>1</v>
@@ -7813,7 +7798,7 @@
         <v>108</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
@@ -7821,7 +7806,7 @@
         <v>109</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C110" s="1">
         <v>1</v>
@@ -7832,7 +7817,7 @@
         <v>110</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C111" s="1">
         <v>1</v>
@@ -7843,7 +7828,7 @@
         <v>111</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
@@ -7851,7 +7836,7 @@
         <v>112</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
@@ -7859,7 +7844,7 @@
         <v>113</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
@@ -7867,7 +7852,7 @@
         <v>114</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
@@ -7875,7 +7860,7 @@
         <v>115</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
@@ -7908,7 +7893,7 @@
         <v>121</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C122" s="1">
         <v>1</v>
@@ -8301,7 +8286,10 @@
         <v>160</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
+      </c>
+      <c r="C161" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">
@@ -8309,7 +8297,7 @@
         <v>161</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C162" s="1">
         <v>1</v>
@@ -8320,7 +8308,10 @@
         <v>162</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
+      </c>
+      <c r="C163" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.2">
@@ -8328,7 +8319,7 @@
         <v>163</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C164" s="1">
         <v>1</v>
@@ -8339,7 +8330,10 @@
         <v>164</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
+      </c>
+      <c r="C165" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.2">
@@ -8347,7 +8341,7 @@
         <v>165</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.2">
@@ -8355,7 +8349,7 @@
         <v>166</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C167" s="1">
         <v>1</v>
@@ -8366,7 +8360,10 @@
         <v>167</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
+      </c>
+      <c r="C168" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.2">
@@ -8374,7 +8371,7 @@
         <v>168</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.2">
@@ -8382,7 +8379,10 @@
         <v>169</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
+      </c>
+      <c r="C170" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.2">
@@ -8486,7 +8486,7 @@
         <v>179</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>336</v>
+        <v>477</v>
       </c>
       <c r="C180" s="1">
         <v>1</v>
@@ -8497,7 +8497,7 @@
         <v>180</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>478</v>
+        <v>70</v>
       </c>
       <c r="C181" s="1">
         <v>1</v>
@@ -8508,7 +8508,7 @@
         <v>181</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>70</v>
+        <v>488</v>
       </c>
       <c r="C182" s="1">
         <v>1</v>
@@ -8530,7 +8530,7 @@
         <v>183</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>490</v>
+        <v>312</v>
       </c>
       <c r="C184" s="1">
         <v>1</v>
@@ -8541,7 +8541,7 @@
         <v>184</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>312</v>
+        <v>453</v>
       </c>
       <c r="C185" s="1">
         <v>1</v>
@@ -8552,7 +8552,7 @@
         <v>185</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>453</v>
+        <v>64</v>
       </c>
       <c r="C186" s="1">
         <v>1</v>
@@ -8563,7 +8563,7 @@
         <v>186</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>64</v>
+        <v>454</v>
       </c>
       <c r="C187" s="1">
         <v>1</v>
@@ -8574,7 +8574,7 @@
         <v>187</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>454</v>
+        <v>66</v>
       </c>
       <c r="C188" s="1">
         <v>1</v>
@@ -8585,7 +8585,7 @@
         <v>188</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>66</v>
+        <v>519</v>
       </c>
       <c r="C189" s="1">
         <v>1</v>
@@ -8595,12 +8595,6 @@
       <c r="A190" s="1">
         <v>189</v>
       </c>
-      <c r="B190" s="1" t="s">
-        <v>520</v>
-      </c>
-      <c r="C190" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A191" s="1">
@@ -8621,140 +8615,68 @@
       <c r="A194" s="1">
         <v>193</v>
       </c>
-      <c r="B194" s="1" t="s">
-        <v>521</v>
-      </c>
-      <c r="C194" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A195" s="1">
         <v>194</v>
       </c>
-      <c r="B195" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="C195" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A196" s="1">
         <v>195</v>
       </c>
-      <c r="B196" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C196" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A197" s="1">
         <v>196</v>
       </c>
-      <c r="B197" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="C197" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A198" s="1">
         <v>197</v>
       </c>
-      <c r="B198" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C198" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A199" s="1">
         <v>198</v>
       </c>
-      <c r="B199" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="C199" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A200" s="1">
         <v>199</v>
       </c>
-      <c r="B200" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C200" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A201" s="1">
         <v>200</v>
       </c>
-      <c r="B201" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="C201" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A202" s="1">
         <v>201</v>
       </c>
-      <c r="B202" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C202" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A203" s="1">
         <v>202</v>
       </c>
-      <c r="B203" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="C203" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A204" s="1">
         <v>203</v>
       </c>
-      <c r="B204" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C204" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A205" s="1">
         <v>204</v>
       </c>
-      <c r="B205" s="1" t="s">
-        <v>376</v>
-      </c>
-      <c r="C205" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A206" s="1">
         <v>205</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>108</v>
+        <v>520</v>
       </c>
       <c r="C206" s="1">
         <v>1</v>
@@ -8765,7 +8687,7 @@
         <v>206</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>109</v>
+        <v>418</v>
       </c>
       <c r="C207" s="1">
         <v>1</v>
@@ -8776,7 +8698,7 @@
         <v>207</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>384</v>
+        <v>107</v>
       </c>
       <c r="C208" s="1">
         <v>1</v>
@@ -8787,7 +8709,7 @@
         <v>208</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>491</v>
+        <v>471</v>
       </c>
       <c r="C209" s="1">
         <v>1</v>
@@ -8798,7 +8720,7 @@
         <v>209</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C210" s="1">
         <v>1</v>
@@ -8809,7 +8731,7 @@
         <v>210</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>385</v>
+        <v>374</v>
       </c>
       <c r="C211" s="1">
         <v>1</v>
@@ -8820,7 +8742,7 @@
         <v>211</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C212" s="1">
         <v>1</v>
@@ -8831,7 +8753,7 @@
         <v>212</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>91</v>
+        <v>420</v>
       </c>
       <c r="C213" s="1">
         <v>1</v>
@@ -8842,7 +8764,7 @@
         <v>213</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>422</v>
+        <v>83</v>
       </c>
       <c r="C214" s="1">
         <v>1</v>
@@ -8853,7 +8775,7 @@
         <v>214</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>387</v>
+        <v>421</v>
       </c>
       <c r="C215" s="1">
         <v>1</v>
@@ -8864,7 +8786,7 @@
         <v>215</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>111</v>
+        <v>84</v>
       </c>
       <c r="C216" s="1">
         <v>1</v>
@@ -8875,7 +8797,7 @@
         <v>216</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C217" s="1">
         <v>1</v>
@@ -8886,7 +8808,7 @@
         <v>217</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>388</v>
+        <v>109</v>
       </c>
       <c r="C218" s="1">
         <v>1</v>
@@ -8897,7 +8819,7 @@
         <v>218</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>112</v>
+        <v>384</v>
       </c>
       <c r="C219" s="1">
         <v>1</v>
@@ -8908,7 +8830,7 @@
         <v>219</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>96</v>
+        <v>490</v>
       </c>
       <c r="C220" s="1">
         <v>1</v>
@@ -8919,7 +8841,7 @@
         <v>220</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C221" s="1">
         <v>1</v>
@@ -8930,7 +8852,7 @@
         <v>221</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>423</v>
+        <v>385</v>
       </c>
       <c r="C222" s="1">
         <v>1</v>
@@ -8941,7 +8863,7 @@
         <v>222</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C223" s="1">
         <v>1</v>
@@ -8952,7 +8874,7 @@
         <v>223</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>389</v>
+        <v>91</v>
       </c>
       <c r="C224" s="1">
         <v>1</v>
@@ -8963,7 +8885,7 @@
         <v>224</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>378</v>
+        <v>422</v>
       </c>
       <c r="C225" s="1">
         <v>1</v>
@@ -8974,10 +8896,7 @@
         <v>225</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="C226" s="1">
-        <v>1</v>
+        <v>541</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.2">
@@ -8985,7 +8904,7 @@
         <v>226</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>380</v>
+        <v>111</v>
       </c>
       <c r="C227" s="1">
         <v>1</v>
@@ -8996,7 +8915,7 @@
         <v>227</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="C228" s="1">
         <v>1</v>
@@ -9007,7 +8926,7 @@
         <v>228</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>381</v>
+        <v>388</v>
       </c>
       <c r="C229" s="1">
         <v>1</v>
@@ -9018,7 +8937,7 @@
         <v>229</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C230" s="1">
         <v>1</v>
@@ -9029,7 +8948,7 @@
         <v>230</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C231" s="1">
         <v>1</v>
@@ -9040,7 +8959,7 @@
         <v>231</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C232" s="1">
         <v>1</v>
@@ -9051,7 +8970,7 @@
         <v>232</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>382</v>
+        <v>423</v>
       </c>
       <c r="C233" s="1">
         <v>1</v>
@@ -9062,7 +8981,7 @@
         <v>233</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="C234" s="1">
         <v>1</v>
@@ -9073,7 +8992,7 @@
         <v>234</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>522</v>
+        <v>389</v>
       </c>
       <c r="C235" s="1">
         <v>1</v>
@@ -9084,7 +9003,7 @@
         <v>235</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>285</v>
+        <v>378</v>
       </c>
       <c r="C236" s="1">
         <v>1</v>
@@ -9095,7 +9014,7 @@
         <v>236</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>390</v>
+        <v>379</v>
       </c>
       <c r="C237" s="1">
         <v>1</v>
@@ -9106,7 +9025,7 @@
         <v>237</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>391</v>
+        <v>380</v>
       </c>
       <c r="C238" s="1">
         <v>1</v>
@@ -9117,7 +9036,7 @@
         <v>238</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>393</v>
+        <v>99</v>
       </c>
       <c r="C239" s="1">
         <v>1</v>
@@ -9128,7 +9047,7 @@
         <v>239</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>424</v>
+        <v>381</v>
       </c>
       <c r="C240" s="1">
         <v>1</v>
@@ -9139,7 +9058,7 @@
         <v>240</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>425</v>
+        <v>113</v>
       </c>
       <c r="C241" s="1">
         <v>1</v>
@@ -9150,7 +9069,7 @@
         <v>241</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>492</v>
+        <v>100</v>
       </c>
       <c r="C242" s="1">
         <v>1</v>
@@ -9160,46 +9079,100 @@
       <c r="A243" s="1">
         <v>242</v>
       </c>
+      <c r="B243" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C243" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A244" s="1">
         <v>243</v>
       </c>
+      <c r="B244" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="C244" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A245" s="1">
         <v>244</v>
       </c>
+      <c r="B245" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C245" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A246" s="1">
         <v>245</v>
       </c>
+      <c r="B246" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C246" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A247" s="1">
         <v>246</v>
       </c>
+      <c r="B247" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="C247" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A248" s="1">
         <v>247</v>
       </c>
+      <c r="B248" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="C248" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A249" s="1">
         <v>248</v>
       </c>
+      <c r="B249" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="C249" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A250" s="1">
         <v>249</v>
       </c>
+      <c r="B250" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="C250" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A251" s="1">
         <v>250</v>
       </c>
+      <c r="B251" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="C251" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A252" s="1">
@@ -9215,140 +9188,68 @@
       <c r="A254" s="1">
         <v>253</v>
       </c>
-      <c r="B254" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="C254" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A255" s="1">
         <v>254</v>
       </c>
-      <c r="B255" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="C255" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A256" s="1">
         <v>255</v>
       </c>
-      <c r="B256" s="1" t="s">
-        <v>523</v>
-      </c>
-      <c r="C256" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A257" s="1">
         <v>256</v>
       </c>
-      <c r="B257" s="1" t="s">
-        <v>540</v>
-      </c>
-      <c r="C257" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A258" s="1">
         <v>257</v>
       </c>
-      <c r="B258" s="1" t="s">
-        <v>405</v>
-      </c>
-      <c r="C258" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A259" s="1">
         <v>258</v>
       </c>
-      <c r="B259" s="1" t="s">
-        <v>541</v>
-      </c>
-      <c r="C259" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A260" s="1">
         <v>259</v>
       </c>
-      <c r="B260" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C260" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A261" s="1">
         <v>260</v>
       </c>
-      <c r="B261" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="C261" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A262" s="1">
         <v>261</v>
       </c>
-      <c r="B262" s="1" t="s">
-        <v>426</v>
-      </c>
-      <c r="C262" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A263" s="1">
         <v>262</v>
       </c>
-      <c r="B263" s="1" t="s">
-        <v>524</v>
-      </c>
-      <c r="C263" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A264" s="1">
         <v>263</v>
       </c>
-      <c r="B264" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C264" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A265" s="1">
         <v>264</v>
       </c>
-      <c r="B265" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="C265" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A266" s="1">
         <v>265</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>447</v>
+        <v>246</v>
       </c>
       <c r="C266" s="1">
         <v>1</v>
@@ -9358,63 +9259,129 @@
       <c r="A267" s="1">
         <v>266</v>
       </c>
+      <c r="B267" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C267" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A268" s="1">
         <v>267</v>
       </c>
+      <c r="B268" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="C268" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A269" s="1">
         <v>268</v>
       </c>
+      <c r="B269" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="C269" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A270" s="1">
         <v>269</v>
       </c>
+      <c r="B270" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="C270" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A271" s="1">
         <v>270</v>
       </c>
+      <c r="B271" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="C271" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A272" s="1">
         <v>271</v>
       </c>
+      <c r="B272" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C272" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A273" s="1">
         <v>272</v>
       </c>
+      <c r="B273" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="C273" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A274" s="1">
         <v>273</v>
       </c>
+      <c r="B274" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="C274" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A275" s="1">
         <v>274</v>
       </c>
+      <c r="B275" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="C275" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A276" s="1">
         <v>275</v>
       </c>
+      <c r="B276" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C276" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A277" s="1">
         <v>276</v>
       </c>
+      <c r="B277" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="C277" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A278" s="1">
         <v>277</v>
       </c>
       <c r="B278" s="1" t="s">
-        <v>493</v>
+        <v>447</v>
       </c>
       <c r="C278" s="1">
         <v>1</v>
@@ -9424,129 +9391,63 @@
       <c r="A279" s="1">
         <v>278</v>
       </c>
-      <c r="B279" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="C279" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A280" s="1">
         <v>279</v>
       </c>
-      <c r="B280" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C280" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A281" s="1">
         <v>280</v>
       </c>
-      <c r="B281" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="C281" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A282" s="1">
         <v>281</v>
       </c>
-      <c r="B282" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="C282" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A283" s="1">
         <v>282</v>
       </c>
-      <c r="B283" s="1" t="s">
-        <v>542</v>
-      </c>
-      <c r="C283" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A284" s="1">
         <v>283</v>
       </c>
-      <c r="B284" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="C284" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A285" s="1">
         <v>284</v>
       </c>
-      <c r="B285" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="C285" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A286" s="1">
         <v>285</v>
       </c>
-      <c r="B286" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="C286" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A287" s="1">
         <v>286</v>
       </c>
-      <c r="B287" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C287" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A288" s="1">
         <v>287</v>
       </c>
-      <c r="B288" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C288" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A289" s="1">
         <v>288</v>
       </c>
-      <c r="B289" s="1" t="s">
-        <v>543</v>
-      </c>
-      <c r="C289" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A290" s="1">
         <v>289</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>135</v>
+        <v>492</v>
       </c>
       <c r="C290" s="1">
         <v>1</v>
@@ -9557,7 +9458,7 @@
         <v>290</v>
       </c>
       <c r="B291" s="1" t="s">
-        <v>141</v>
+        <v>411</v>
       </c>
       <c r="C291" s="1">
         <v>1</v>
@@ -9568,7 +9469,7 @@
         <v>291</v>
       </c>
       <c r="B292" s="1" t="s">
-        <v>427</v>
+        <v>412</v>
       </c>
       <c r="C292" s="1">
         <v>1</v>
@@ -9579,7 +9480,7 @@
         <v>292</v>
       </c>
       <c r="B293" s="1" t="s">
-        <v>144</v>
+        <v>284</v>
       </c>
       <c r="C293" s="1">
         <v>1</v>
@@ -9590,7 +9491,7 @@
         <v>293</v>
       </c>
       <c r="B294" s="1" t="s">
-        <v>145</v>
+        <v>473</v>
       </c>
       <c r="C294" s="1">
         <v>1</v>
@@ -9601,7 +9502,7 @@
         <v>294</v>
       </c>
       <c r="B295" s="1" t="s">
-        <v>148</v>
+        <v>533</v>
       </c>
       <c r="C295" s="1">
         <v>1</v>
@@ -9612,7 +9513,7 @@
         <v>295</v>
       </c>
       <c r="B296" s="1" t="s">
-        <v>150</v>
+        <v>283</v>
       </c>
       <c r="C296" s="1">
         <v>1</v>
@@ -9623,7 +9524,7 @@
         <v>296</v>
       </c>
       <c r="B297" s="1" t="s">
-        <v>158</v>
+        <v>125</v>
       </c>
       <c r="C297" s="1">
         <v>1</v>
@@ -9633,56 +9534,122 @@
       <c r="A298" s="1">
         <v>297</v>
       </c>
+      <c r="B298" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C298" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A299" s="1">
         <v>298</v>
       </c>
+      <c r="B299" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C299" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A300" s="1">
         <v>299</v>
       </c>
+      <c r="B300" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="C300" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A301" s="1">
         <v>300</v>
       </c>
+      <c r="B301" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C301" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A302" s="1">
         <v>301</v>
       </c>
+      <c r="B302" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C302" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A303" s="1">
         <v>302</v>
       </c>
+      <c r="B303" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="C303" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A304" s="1">
         <v>303</v>
       </c>
+      <c r="B304" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C304" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A305" s="1">
         <v>304</v>
       </c>
+      <c r="B305" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C305" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A306" s="1">
         <v>305</v>
       </c>
+      <c r="B306" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C306" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A307" s="1">
         <v>306</v>
       </c>
+      <c r="B307" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C307" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A308" s="1">
         <v>307</v>
       </c>
+      <c r="B308" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C308" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A309" s="1">
@@ -9713,140 +9680,68 @@
       <c r="A314" s="1">
         <v>313</v>
       </c>
-      <c r="B314" s="1" t="s">
-        <v>428</v>
-      </c>
-      <c r="C314" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A315" s="1">
         <v>314</v>
       </c>
-      <c r="B315" s="1" t="s">
-        <v>429</v>
-      </c>
-      <c r="C315" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A316" s="1">
         <v>315</v>
       </c>
-      <c r="B316" s="1" t="s">
-        <v>529</v>
-      </c>
-      <c r="C316" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A317" s="1">
         <v>316</v>
       </c>
-      <c r="B317" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="C317" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A318" s="1">
         <v>317</v>
       </c>
-      <c r="B318" s="1" t="s">
-        <v>531</v>
-      </c>
-      <c r="C318" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A319" s="1">
         <v>318</v>
       </c>
-      <c r="B319" s="1" t="s">
-        <v>526</v>
-      </c>
-      <c r="C319" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A320" s="1">
         <v>319</v>
       </c>
-      <c r="B320" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="C320" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A321" s="1">
         <v>320</v>
       </c>
-      <c r="B321" s="1" t="s">
-        <v>455</v>
-      </c>
-      <c r="C321" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A322" s="1">
         <v>321</v>
       </c>
-      <c r="B322" s="1" t="s">
-        <v>430</v>
-      </c>
-      <c r="C322" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A323" s="1">
         <v>322</v>
       </c>
-      <c r="B323" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C323" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A324" s="1">
         <v>323</v>
       </c>
-      <c r="B324" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="C324" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A325" s="1">
         <v>324</v>
       </c>
-      <c r="B325" s="1" t="s">
-        <v>431</v>
-      </c>
-      <c r="C325" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A326" s="1">
         <v>325</v>
       </c>
       <c r="B326" s="1" t="s">
-        <v>527</v>
+        <v>428</v>
       </c>
       <c r="C326" s="1">
         <v>1</v>
@@ -9857,7 +9752,7 @@
         <v>326</v>
       </c>
       <c r="B327" s="1" t="s">
-        <v>314</v>
+        <v>429</v>
       </c>
       <c r="C327" s="1">
         <v>1</v>
@@ -9868,7 +9763,7 @@
         <v>327</v>
       </c>
       <c r="B328" s="1" t="s">
-        <v>171</v>
+        <v>524</v>
       </c>
       <c r="C328" s="1">
         <v>1</v>
@@ -9879,7 +9774,7 @@
         <v>328</v>
       </c>
       <c r="B329" s="1" t="s">
-        <v>528</v>
+        <v>160</v>
       </c>
       <c r="C329" s="1">
         <v>1</v>
@@ -9890,7 +9785,7 @@
         <v>329</v>
       </c>
       <c r="B330" s="1" t="s">
-        <v>432</v>
+        <v>455</v>
       </c>
       <c r="C330" s="1">
         <v>1</v>
@@ -9901,7 +9796,7 @@
         <v>330</v>
       </c>
       <c r="B331" s="1" t="s">
-        <v>176</v>
+        <v>430</v>
       </c>
       <c r="C331" s="1">
         <v>1</v>
@@ -9912,7 +9807,7 @@
         <v>331</v>
       </c>
       <c r="B332" s="1" t="s">
-        <v>532</v>
+        <v>168</v>
       </c>
       <c r="C332" s="1">
         <v>1</v>
@@ -9923,7 +9818,7 @@
         <v>332</v>
       </c>
       <c r="B333" s="1" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="C333" s="1">
         <v>1</v>
@@ -9933,41 +9828,89 @@
       <c r="A334" s="1">
         <v>333</v>
       </c>
+      <c r="B334" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="C334" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A335" s="1">
         <v>334</v>
       </c>
+      <c r="B335" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="C335" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A336" s="1">
         <v>335</v>
       </c>
+      <c r="B336" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C336" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A337" s="1">
         <v>336</v>
       </c>
+      <c r="B337" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C337" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A338" s="1">
         <v>337</v>
       </c>
+      <c r="B338" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="C338" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A339" s="1">
         <v>338</v>
       </c>
+      <c r="B339" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C339" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A340" s="1">
         <v>339</v>
       </c>
+      <c r="B340" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C340" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A341" s="1">
         <v>340</v>
       </c>
+      <c r="B341" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C341" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A342" s="1">
@@ -10013,140 +9956,68 @@
       <c r="A350" s="1">
         <v>349</v>
       </c>
-      <c r="B350" s="1" t="s">
-        <v>433</v>
-      </c>
-      <c r="C350" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A351" s="1">
         <v>350</v>
       </c>
-      <c r="B351" s="1" t="s">
-        <v>533</v>
-      </c>
-      <c r="C351" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A352" s="1">
         <v>351</v>
       </c>
-      <c r="B352" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="C352" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A353" s="1">
         <v>352</v>
       </c>
-      <c r="B353" s="1" t="s">
-        <v>435</v>
-      </c>
-      <c r="C353" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A354" s="1">
         <v>353</v>
       </c>
-      <c r="B354" s="1" t="s">
-        <v>436</v>
-      </c>
-      <c r="C354" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="355" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A355" s="1">
         <v>354</v>
       </c>
-      <c r="B355" s="1" t="s">
-        <v>437</v>
-      </c>
-      <c r="C355" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="356" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A356" s="1">
         <v>355</v>
       </c>
-      <c r="B356" s="1" t="s">
-        <v>396</v>
-      </c>
-      <c r="C356" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="357" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A357" s="1">
         <v>356</v>
       </c>
-      <c r="B357" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="C357" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="358" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A358" s="1">
         <v>357</v>
       </c>
-      <c r="B358" s="1" t="s">
-        <v>438</v>
-      </c>
-      <c r="C358" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="359" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A359" s="1">
         <v>358</v>
       </c>
-      <c r="B359" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="C359" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A360" s="1">
         <v>359</v>
       </c>
-      <c r="B360" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="C360" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="361" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A361" s="1">
         <v>360</v>
       </c>
-      <c r="B361" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="C361" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="362" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A362" s="1">
         <v>361</v>
       </c>
       <c r="B362" s="1" t="s">
-        <v>268</v>
+        <v>433</v>
       </c>
       <c r="C362" s="1">
         <v>1</v>
@@ -10157,7 +10028,7 @@
         <v>362</v>
       </c>
       <c r="B363" s="1" t="s">
-        <v>544</v>
+        <v>434</v>
       </c>
       <c r="C363" s="1">
         <v>1</v>
@@ -10167,46 +10038,100 @@
       <c r="A364" s="1">
         <v>363</v>
       </c>
+      <c r="B364" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="C364" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="365" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A365" s="1">
         <v>364</v>
       </c>
+      <c r="B365" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="C365" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A366" s="1">
         <v>365</v>
       </c>
+      <c r="B366" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="C366" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="367" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A367" s="1">
         <v>366</v>
       </c>
+      <c r="B367" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C367" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="368" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A368" s="1">
         <v>367</v>
       </c>
+      <c r="B368" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="C368" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A369" s="1">
         <v>368</v>
       </c>
+      <c r="B369" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="C369" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A370" s="1">
         <v>369</v>
       </c>
+      <c r="B370" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C370" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A371" s="1">
         <v>370</v>
       </c>
+      <c r="B371" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C371" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A372" s="1">
         <v>371</v>
       </c>
+      <c r="B372" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="C372" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A373" s="1">
@@ -10217,137 +10142,68 @@
       <c r="A374" s="1">
         <v>373</v>
       </c>
-      <c r="B374" s="1" t="s">
-        <v>494</v>
-      </c>
-      <c r="C374" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A375" s="1">
         <v>374</v>
       </c>
-      <c r="B375" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="C375" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A376" s="1">
         <v>375</v>
       </c>
-      <c r="B376" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="C376" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A377" s="1">
         <v>376</v>
       </c>
-      <c r="B377" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="C377" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A378" s="1">
         <v>377</v>
       </c>
-      <c r="B378" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="C378" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A379" s="1">
         <v>378</v>
       </c>
-      <c r="B379" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="C379" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A380" s="1">
         <v>379</v>
       </c>
-      <c r="B380" s="1" t="s">
-        <v>495</v>
-      </c>
-      <c r="C380" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A381" s="1">
         <v>380</v>
       </c>
-      <c r="B381" s="1" t="s">
-        <v>496</v>
-      </c>
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A382" s="1">
         <v>381</v>
       </c>
-      <c r="B382" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="C382" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A383" s="1">
         <v>382</v>
       </c>
-      <c r="B383" s="1" t="s">
-        <v>498</v>
-      </c>
-      <c r="C383" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="384" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A384" s="1">
         <v>383</v>
       </c>
-      <c r="B384" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="C384" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="385" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A385" s="1">
         <v>384</v>
       </c>
-      <c r="B385" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="C385" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="386" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A386" s="1">
         <v>385</v>
       </c>
       <c r="B386" s="1" t="s">
-        <v>439</v>
+        <v>493</v>
       </c>
       <c r="C386" s="1">
         <v>1</v>
@@ -10358,7 +10214,7 @@
         <v>386</v>
       </c>
       <c r="B387" s="1" t="s">
-        <v>499</v>
+        <v>474</v>
       </c>
       <c r="C387" s="1">
         <v>1</v>
@@ -10369,7 +10225,7 @@
         <v>387</v>
       </c>
       <c r="B388" s="1" t="s">
-        <v>475</v>
+        <v>186</v>
       </c>
       <c r="C388" s="1">
         <v>1</v>
@@ -10380,7 +10236,7 @@
         <v>388</v>
       </c>
       <c r="B389" s="1" t="s">
-        <v>500</v>
+        <v>187</v>
       </c>
       <c r="C389" s="1">
         <v>1</v>
@@ -10391,7 +10247,7 @@
         <v>389</v>
       </c>
       <c r="B390" s="1" t="s">
-        <v>476</v>
+        <v>189</v>
       </c>
       <c r="C390" s="1">
         <v>1</v>
@@ -10402,7 +10258,7 @@
         <v>390</v>
       </c>
       <c r="B391" s="1" t="s">
-        <v>534</v>
+        <v>191</v>
       </c>
       <c r="C391" s="1">
         <v>1</v>
@@ -10413,7 +10269,7 @@
         <v>391</v>
       </c>
       <c r="B392" s="1" t="s">
-        <v>501</v>
+        <v>494</v>
       </c>
       <c r="C392" s="1">
         <v>1</v>
@@ -10424,10 +10280,7 @@
         <v>392</v>
       </c>
       <c r="B393" s="1" t="s">
-        <v>502</v>
-      </c>
-      <c r="C393" s="1">
-        <v>1</v>
+        <v>495</v>
       </c>
     </row>
     <row r="394" spans="1:3" x14ac:dyDescent="0.2">
@@ -10435,7 +10288,7 @@
         <v>393</v>
       </c>
       <c r="B394" s="1" t="s">
-        <v>503</v>
+        <v>496</v>
       </c>
       <c r="C394" s="1">
         <v>1</v>
@@ -10446,7 +10299,7 @@
         <v>394</v>
       </c>
       <c r="B395" s="1" t="s">
-        <v>368</v>
+        <v>497</v>
       </c>
       <c r="C395" s="1">
         <v>1</v>
@@ -10456,61 +10309,133 @@
       <c r="A396" s="1">
         <v>395</v>
       </c>
+      <c r="B396" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="C396" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="397" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A397" s="1">
         <v>396</v>
       </c>
+      <c r="B397" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C397" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="398" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A398" s="1">
         <v>397</v>
       </c>
+      <c r="B398" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="C398" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="399" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A399" s="1">
         <v>398</v>
       </c>
+      <c r="B399" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="C399" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="400" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A400" s="1">
         <v>399</v>
       </c>
+      <c r="B400" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="C400" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="401" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A401" s="1">
         <v>400</v>
       </c>
+      <c r="B401" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="C401" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="402" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A402" s="1">
         <v>401</v>
       </c>
+      <c r="B402" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="C402" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="403" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A403" s="1">
         <v>402</v>
       </c>
+      <c r="B403" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="C403" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="404" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A404" s="1">
         <v>403</v>
       </c>
+      <c r="B404" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="C404" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="405" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A405" s="1">
         <v>404</v>
       </c>
+      <c r="B405" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="C405" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="406" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A406" s="1">
         <v>405</v>
       </c>
+      <c r="B406" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="C406" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="407" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A407" s="1">
         <v>406</v>
       </c>
+      <c r="B407" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="C407" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="408" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A408" s="1">
@@ -10526,137 +10451,68 @@
       <c r="A410" s="1">
         <v>409</v>
       </c>
-      <c r="B410" s="1" t="s">
-        <v>440</v>
-      </c>
-      <c r="C410" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="411" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A411" s="1">
         <v>410</v>
       </c>
-      <c r="B411" s="1" t="s">
-        <v>477</v>
-      </c>
-      <c r="C411" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="412" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A412" s="1">
         <v>411</v>
       </c>
-      <c r="B412" s="1" t="s">
-        <v>442</v>
-      </c>
-      <c r="C412" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="413" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A413" s="1">
         <v>412</v>
       </c>
-      <c r="B413" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="C413" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="414" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A414" s="1">
         <v>413</v>
       </c>
-      <c r="B414" s="1" t="s">
-        <v>536</v>
-      </c>
-      <c r="C414" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="415" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A415" s="1">
         <v>414</v>
       </c>
-      <c r="B415" s="1" t="s">
-        <v>537</v>
-      </c>
-      <c r="C415" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="416" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A416" s="1">
         <v>415</v>
       </c>
-      <c r="B416" s="1" t="s">
-        <v>441</v>
-      </c>
-      <c r="C416" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="417" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A417" s="1">
         <v>416</v>
       </c>
-      <c r="B417" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="C417" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="418" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A418" s="1">
         <v>417</v>
       </c>
-      <c r="B418" s="1" t="s">
-        <v>419</v>
-      </c>
     </row>
     <row r="419" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A419" s="1">
         <v>418</v>
       </c>
-      <c r="B419" s="1" t="s">
-        <v>443</v>
-      </c>
-      <c r="C419" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="420" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A420" s="1">
         <v>419</v>
       </c>
-      <c r="B420" s="1" t="s">
-        <v>444</v>
-      </c>
-      <c r="C420" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="421" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A421" s="1">
         <v>420</v>
       </c>
-      <c r="B421" s="1" t="s">
-        <v>539</v>
-      </c>
-      <c r="C421" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="422" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A422" s="1">
         <v>421</v>
       </c>
       <c r="B422" s="1" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="C422" s="1">
         <v>1</v>
@@ -10667,7 +10523,7 @@
         <v>422</v>
       </c>
       <c r="B423" s="1" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="C423" s="1">
         <v>1</v>
@@ -10678,7 +10534,7 @@
         <v>423</v>
       </c>
       <c r="B424" s="1" t="s">
-        <v>538</v>
+        <v>279</v>
       </c>
       <c r="C424" s="1">
         <v>1</v>
@@ -10689,7 +10545,7 @@
         <v>424</v>
       </c>
       <c r="B425" s="1" t="s">
-        <v>292</v>
+        <v>441</v>
       </c>
       <c r="C425" s="1">
         <v>1</v>
@@ -10700,7 +10556,7 @@
         <v>425</v>
       </c>
       <c r="B426" s="1" t="s">
-        <v>535</v>
+        <v>313</v>
       </c>
       <c r="C426" s="1">
         <v>1</v>
@@ -10710,108 +10566,159 @@
       <c r="A427" s="1">
         <v>426</v>
       </c>
+      <c r="B427" s="1" t="s">
+        <v>419</v>
+      </c>
     </row>
     <row r="428" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A428" s="1">
         <v>427</v>
       </c>
+      <c r="B428" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="C428" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="429" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A429" s="1">
         <v>428</v>
       </c>
+      <c r="B429" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="C429" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="430" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A430" s="1">
         <v>429</v>
       </c>
+      <c r="B430" s="1" t="s">
+        <v>539</v>
+      </c>
     </row>
     <row r="431" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A431" s="1">
         <v>430</v>
       </c>
+      <c r="B431" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="C431" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="432" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A432" s="1">
         <v>431</v>
       </c>
-    </row>
-    <row r="433" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B432" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="C432" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="433" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A433" s="1">
         <v>432</v>
       </c>
-    </row>
-    <row r="434" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B433" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="C433" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="434" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A434" s="1">
         <v>433</v>
       </c>
-    </row>
-    <row r="435" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B434" s="1" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="435" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A435" s="1">
         <v>434</v>
       </c>
-    </row>
-    <row r="436" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B435" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C435" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="436" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A436" s="1">
         <v>435</v>
       </c>
-    </row>
-    <row r="437" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B436" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="C436" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="437" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A437" s="1">
         <v>436</v>
       </c>
     </row>
-    <row r="438" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="438" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A438" s="1">
         <v>437</v>
       </c>
     </row>
-    <row r="439" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="439" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A439" s="1">
         <v>438</v>
       </c>
     </row>
-    <row r="440" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="440" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A440" s="1">
         <v>439</v>
       </c>
     </row>
-    <row r="441" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="441" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A441" s="1">
         <v>440</v>
       </c>
     </row>
-    <row r="442" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="442" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A442" s="1">
         <v>441</v>
       </c>
     </row>
-    <row r="443" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="443" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A443" s="1">
         <v>442</v>
       </c>
     </row>
-    <row r="444" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="444" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A444" s="1">
         <v>443</v>
       </c>
     </row>
-    <row r="445" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="445" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A445" s="1">
         <v>444</v>
       </c>
     </row>
-    <row r="446" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="446" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A446" s="1">
         <v>445</v>
       </c>
     </row>
-    <row r="447" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="447" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A447" s="1">
         <v>446</v>
       </c>
     </row>
-    <row r="448" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="448" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A448" s="1">
         <v>447</v>
       </c>
@@ -10910,7 +10817,7 @@
         <v>461</v>
       </c>
       <c r="B462" s="1" t="s">
-        <v>547</v>
+        <v>538</v>
       </c>
       <c r="C462" s="1">
         <v>1</v>
@@ -10932,7 +10839,7 @@
         <v>463</v>
       </c>
       <c r="B464" s="1" t="s">
-        <v>546</v>
+        <v>537</v>
       </c>
       <c r="C464" s="1">
         <v>1</v>
@@ -10987,7 +10894,7 @@
         <v>468</v>
       </c>
       <c r="B469" s="1" t="s">
-        <v>545</v>
+        <v>536</v>
       </c>
       <c r="C469" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
Updating decks and collection
</commit_message>
<xml_diff>
--- a/data/binder/Binder.xlsx
+++ b/data/binder/Binder.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Dados/MTG/EDH DeckHelper/EDH-DeckHelper/data/binder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E606081-8AE0-5340-AE8D-7060C1DBB2D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0052D1A0-D2C1-3E4B-85FF-C223F4B75621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{7ABBCC85-5F92-6F41-92E4-65212D317CF6}"/>
+    <workbookView xWindow="9520" yWindow="460" windowWidth="15340" windowHeight="15540" xr2:uid="{7ABBCC85-5F92-6F41-92E4-65212D317CF6}"/>
   </bookViews>
   <sheets>
-    <sheet name="single-column" sheetId="2" r:id="rId1"/>
+    <sheet name="Binder" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Binder" localSheetId="0">'single-column'!$A$1:$C$481</definedName>
+    <definedName name="Binder" localSheetId="0">Binder!$A$1:$C$481</definedName>
   </definedNames>
   <calcPr calcId="179021"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="304">
   <si>
     <t>Slot</t>
   </si>
@@ -233,9 +233,6 @@
     <t>Tree of Tales</t>
   </si>
   <si>
-    <t>Strip Mine</t>
-  </si>
-  <si>
     <t>Gaea's Cradle</t>
   </si>
   <si>
@@ -257,24 +254,9 @@
     <t>Command Tower</t>
   </si>
   <si>
-    <t>Forbidden Orchard</t>
-  </si>
-  <si>
     <t>Mana Confluence</t>
   </si>
   <si>
-    <t>Tarnished Citadel</t>
-  </si>
-  <si>
-    <t>Exotic Orchard</t>
-  </si>
-  <si>
-    <t>Reflecting Pool</t>
-  </si>
-  <si>
-    <t>Chrome Mox</t>
-  </si>
-  <si>
     <t>Dimir Signet</t>
   </si>
   <si>
@@ -287,9 +269,6 @@
     <t>Mana Crypt</t>
   </si>
   <si>
-    <t>Mana Vault</t>
-  </si>
-  <si>
     <t>Mind Stone</t>
   </si>
   <si>
@@ -350,9 +329,6 @@
     <t>Swords to Plowshares</t>
   </si>
   <si>
-    <t>Brainstorm</t>
-  </si>
-  <si>
     <t>Counterspell</t>
   </si>
   <si>
@@ -374,15 +350,9 @@
     <t>Mystical Tutor</t>
   </si>
   <si>
-    <t>Negate</t>
-  </si>
-  <si>
     <t>Swan Song</t>
   </si>
   <si>
-    <t>Fabricate</t>
-  </si>
-  <si>
     <t>Time Spiral</t>
   </si>
   <si>
@@ -410,9 +380,6 @@
     <t>Yawgmoth's Will</t>
   </si>
   <si>
-    <t>Gamble</t>
-  </si>
-  <si>
     <t>Elves of Deep Shadow</t>
   </si>
   <si>
@@ -431,30 +398,15 @@
     <t>Beast Within</t>
   </si>
   <si>
-    <t>By Force</t>
-  </si>
-  <si>
-    <t>Rolling Earthquake</t>
-  </si>
-  <si>
-    <t>Grand Abolisher</t>
-  </si>
-  <si>
     <t>Mother of Runes</t>
   </si>
   <si>
-    <t>Academy Ruins</t>
-  </si>
-  <si>
     <t>Dack Fayden</t>
   </si>
   <si>
     <t>Rhystic Study</t>
   </si>
   <si>
-    <t>Tezzeret the Seeker</t>
-  </si>
-  <si>
     <t>Thought Vessel</t>
   </si>
   <si>
@@ -599,12 +551,6 @@
     <t>Swiftfoot Boots</t>
   </si>
   <si>
-    <t>Thran Dynamo</t>
-  </si>
-  <si>
-    <t>Hall of the Bandit Lord</t>
-  </si>
-  <si>
     <t>Nurturing Peatland</t>
   </si>
   <si>
@@ -635,9 +581,6 @@
     <t>Have</t>
   </si>
   <si>
-    <t>Spellseeker</t>
-  </si>
-  <si>
     <t>Jace, Wielder of Mysteries</t>
   </si>
   <si>
@@ -662,63 +605,24 @@
     <t>Assassin's Trophy</t>
   </si>
   <si>
-    <t>Commander's Sphere</t>
-  </si>
-  <si>
     <t>Elixir of Immortality</t>
   </si>
   <si>
-    <t>Mindcrank</t>
-  </si>
-  <si>
     <t>Skullclamp</t>
   </si>
   <si>
     <t>Vanquisher's Banner</t>
   </si>
   <si>
-    <t>Whispersilk Cloak</t>
-  </si>
-  <si>
     <t>Generous Gift</t>
   </si>
   <si>
-    <t>Mystic Confluence</t>
-  </si>
-  <si>
-    <t>Doom Whisperer</t>
-  </si>
-  <si>
-    <t>Vilis, Broker of Blood</t>
-  </si>
-  <si>
-    <t>Whip of Erebos</t>
-  </si>
-  <si>
     <t>Command the Dreadhorde</t>
   </si>
   <si>
-    <t>Living Death</t>
-  </si>
-  <si>
     <t>Glint-Horn Buccaneer</t>
   </si>
   <si>
-    <t>Aggravated Assault</t>
-  </si>
-  <si>
-    <t>Chaos Warp</t>
-  </si>
-  <si>
-    <t>Fling</t>
-  </si>
-  <si>
-    <t>Temur Battle Rage</t>
-  </si>
-  <si>
-    <t>Chandra's Ignition</t>
-  </si>
-  <si>
     <t>Heroic Intervention</t>
   </si>
   <si>
@@ -734,27 +638,6 @@
     <t>Boros Charm</t>
   </si>
   <si>
-    <t>Counterflux</t>
-  </si>
-  <si>
-    <t>Rakdos Charm</t>
-  </si>
-  <si>
-    <t>Terminate</t>
-  </si>
-  <si>
-    <t>Mythos of Snapdax</t>
-  </si>
-  <si>
-    <t>Cabal Coffers</t>
-  </si>
-  <si>
-    <t>Hanweir Battlements</t>
-  </si>
-  <si>
-    <t>Homeward Path</t>
-  </si>
-  <si>
     <t>Hall of Heliod's Generosity</t>
   </si>
   <si>
@@ -767,9 +650,6 @@
     <t>Tolaria West</t>
   </si>
   <si>
-    <t>Phyrexian Reclamation</t>
-  </si>
-  <si>
     <t>Barkchannel Pathway // Tidechannel Pathway</t>
   </si>
   <si>
@@ -875,9 +755,6 @@
     <t>Herald's Horn</t>
   </si>
   <si>
-    <t>Myr Battlesphere</t>
-  </si>
-  <si>
     <t>Spark Double</t>
   </si>
   <si>
@@ -974,9 +851,6 @@
     <t>Flawless Maneuver</t>
   </si>
   <si>
-    <t>Bolas's Citadel</t>
-  </si>
-  <si>
     <t>Damn</t>
   </si>
   <si>
@@ -992,9 +866,6 @@
     <t>Eerie Ultimatum</t>
   </si>
   <si>
-    <t>Heartwarming Redemption</t>
-  </si>
-  <si>
     <t>Ghostly Prison</t>
   </si>
   <si>
@@ -1007,9 +878,6 @@
     <t>Fierce Guardianship</t>
   </si>
   <si>
-    <t>Wheel of Misfortune</t>
-  </si>
-  <si>
     <t>Volrath's Stronghold</t>
   </si>
   <si>
@@ -1019,15 +887,6 @@
     <t>Helm of Obidience</t>
   </si>
   <si>
-    <t>Dovin's Veto</t>
-  </si>
-  <si>
-    <t>Solemn Simulacrum</t>
-  </si>
-  <si>
-    <t>Nihil Spellbomb</t>
-  </si>
-  <si>
     <t>Sundown Pass</t>
   </si>
   <si>
@@ -1041,6 +900,60 @@
   </si>
   <si>
     <t>Deathcap Glade</t>
+  </si>
+  <si>
+    <t>Alchemist's Refuge</t>
+  </si>
+  <si>
+    <t>Castle Garenbrig</t>
+  </si>
+  <si>
+    <t>Desolate Lighthouse</t>
+  </si>
+  <si>
+    <t>Grim Backwoods</t>
+  </si>
+  <si>
+    <t>Slayers' Stronghold</t>
+  </si>
+  <si>
+    <t>Birds of Paradise</t>
+  </si>
+  <si>
+    <t>Freyalise, Llanowar's Fury</t>
+  </si>
+  <si>
+    <t>Fyndhorn Elves</t>
+  </si>
+  <si>
+    <t>Sylvan Library</t>
+  </si>
+  <si>
+    <t>Tireless Provisioner</t>
+  </si>
+  <si>
+    <t>Wood Elves</t>
+  </si>
+  <si>
+    <t>Weirding Wood</t>
+  </si>
+  <si>
+    <t>Second Harvest</t>
+  </si>
+  <si>
+    <t>Vanquish the Horde</t>
+  </si>
+  <si>
+    <t>Putrefy</t>
+  </si>
+  <si>
+    <t>Necromancy</t>
+  </si>
+  <si>
+    <t>Pongify</t>
+  </si>
+  <si>
+    <t>Adrix and Nev, Twincasters</t>
   </si>
 </sst>
 </file>
@@ -1414,8 +1327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5953B7FC-4B75-B146-8A26-6CA09B5F3C99}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A415" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G427" sqref="G427"/>
+    <sheetView tabSelected="1" topLeftCell="A390" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E398" sqref="E398"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1433,7 +1346,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -1715,6 +1628,9 @@
       <c r="B30" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="C30" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
@@ -1811,6 +1727,9 @@
       <c r="B39" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="C39" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
@@ -1949,7 +1868,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
       <c r="C52" s="1">
         <v>1</v>
@@ -1960,7 +1879,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
       <c r="C53" s="1">
         <v>1</v>
@@ -1971,7 +1890,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
       <c r="C54" s="1">
         <v>1</v>
@@ -1982,7 +1901,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
       <c r="C55" s="1">
         <v>1</v>
@@ -1993,7 +1912,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="C56" s="1">
         <v>1</v>
@@ -2059,7 +1978,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>252</v>
+        <v>212</v>
       </c>
       <c r="C65" s="1">
         <v>1</v>
@@ -2081,7 +2000,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>253</v>
+        <v>213</v>
       </c>
       <c r="C67" s="1">
         <v>1</v>
@@ -2103,7 +2022,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>254</v>
+        <v>214</v>
       </c>
       <c r="C69" s="1">
         <v>1</v>
@@ -2114,7 +2033,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>255</v>
+        <v>215</v>
       </c>
       <c r="C70" s="1">
         <v>1</v>
@@ -2125,7 +2044,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>256</v>
+        <v>216</v>
       </c>
       <c r="C71" s="1">
         <v>1</v>
@@ -2136,7 +2055,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>192</v>
+        <v>174</v>
       </c>
       <c r="C72" s="1">
         <v>1</v>
@@ -2147,7 +2066,7 @@
         <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>193</v>
+        <v>175</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -2155,7 +2074,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>187</v>
+        <v>169</v>
       </c>
       <c r="C74" s="1">
         <v>1</v>
@@ -2166,7 +2085,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>188</v>
+        <v>170</v>
       </c>
       <c r="C75" s="1">
         <v>1</v>
@@ -2177,7 +2096,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>189</v>
+        <v>171</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
@@ -2185,7 +2104,7 @@
         <v>76</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>190</v>
+        <v>172</v>
       </c>
       <c r="C77" s="1">
         <v>1</v>
@@ -2216,7 +2135,7 @@
         <v>81</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="C82" s="1">
         <v>1</v>
@@ -2227,7 +2146,7 @@
         <v>82</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="C83" s="1">
         <v>1</v>
@@ -2238,7 +2157,7 @@
         <v>83</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="C84" s="1">
         <v>1</v>
@@ -2249,7 +2168,7 @@
         <v>84</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="C85" s="1">
         <v>1</v>
@@ -2260,7 +2179,7 @@
         <v>85</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
       <c r="C86" s="1">
         <v>1</v>
@@ -2271,7 +2190,7 @@
         <v>86</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="C87" s="1">
         <v>1</v>
@@ -2282,7 +2201,7 @@
         <v>87</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="C88" s="1">
         <v>1</v>
@@ -2293,7 +2212,7 @@
         <v>88</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="C89" s="1">
         <v>1</v>
@@ -2304,7 +2223,7 @@
         <v>89</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
       <c r="C90" s="1">
         <v>1</v>
@@ -2315,7 +2234,7 @@
         <v>90</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="C91" s="1">
         <v>1</v>
@@ -2326,7 +2245,7 @@
         <v>91</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>242</v>
+        <v>202</v>
       </c>
       <c r="C92" s="1">
         <v>1</v>
@@ -2337,7 +2256,7 @@
         <v>92</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>243</v>
+        <v>203</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
@@ -2345,7 +2264,7 @@
         <v>93</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>244</v>
+        <v>204</v>
       </c>
       <c r="C94" s="1">
         <v>1</v>
@@ -2356,7 +2275,7 @@
         <v>94</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
       <c r="C95" s="1">
         <v>1</v>
@@ -2367,7 +2286,7 @@
         <v>95</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>246</v>
+        <v>206</v>
       </c>
       <c r="C96" s="1">
         <v>1</v>
@@ -2378,7 +2297,7 @@
         <v>96</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>247</v>
+        <v>207</v>
       </c>
       <c r="C97" s="1">
         <v>1</v>
@@ -2389,7 +2308,7 @@
         <v>97</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>248</v>
+        <v>208</v>
       </c>
       <c r="C98" s="1">
         <v>1</v>
@@ -2400,7 +2319,7 @@
         <v>98</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>249</v>
+        <v>209</v>
       </c>
       <c r="C99" s="1">
         <v>1</v>
@@ -2411,7 +2330,7 @@
         <v>99</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>250</v>
+        <v>210</v>
       </c>
       <c r="C100" s="1">
         <v>1</v>
@@ -2422,7 +2341,7 @@
         <v>100</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>251</v>
+        <v>211</v>
       </c>
       <c r="C101" s="1">
         <v>1</v>
@@ -2433,7 +2352,7 @@
         <v>101</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>264</v>
+        <v>224</v>
       </c>
       <c r="C102" s="1">
         <v>1</v>
@@ -2444,7 +2363,7 @@
         <v>102</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>265</v>
+        <v>225</v>
       </c>
       <c r="C103" s="1">
         <v>1</v>
@@ -2455,7 +2374,7 @@
         <v>103</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>266</v>
+        <v>226</v>
       </c>
       <c r="C104" s="1">
         <v>1</v>
@@ -2466,7 +2385,7 @@
         <v>104</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>267</v>
+        <v>227</v>
       </c>
       <c r="C105" s="1">
         <v>1</v>
@@ -2477,7 +2396,7 @@
         <v>105</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>268</v>
+        <v>228</v>
       </c>
       <c r="C106" s="1">
         <v>1</v>
@@ -2488,7 +2407,7 @@
         <v>106</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>269</v>
+        <v>229</v>
       </c>
       <c r="C107" s="1">
         <v>1</v>
@@ -2499,7 +2418,7 @@
         <v>107</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>270</v>
+        <v>230</v>
       </c>
       <c r="C108" s="1">
         <v>1</v>
@@ -2510,7 +2429,7 @@
         <v>108</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>271</v>
+        <v>231</v>
       </c>
       <c r="C109" s="1">
         <v>1</v>
@@ -2521,7 +2440,7 @@
         <v>109</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>272</v>
+        <v>232</v>
       </c>
       <c r="C110" s="1">
         <v>1</v>
@@ -2532,7 +2451,7 @@
         <v>110</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>273</v>
+        <v>233</v>
       </c>
       <c r="C111" s="1">
         <v>1</v>
@@ -2543,7 +2462,7 @@
         <v>111</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>332</v>
+        <v>285</v>
       </c>
       <c r="C112" s="1">
         <v>1</v>
@@ -2554,7 +2473,7 @@
         <v>112</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>289</v>
+        <v>248</v>
       </c>
       <c r="C113" s="1">
         <v>1</v>
@@ -2565,7 +2484,7 @@
         <v>113</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>331</v>
+        <v>284</v>
       </c>
       <c r="C114" s="1">
         <v>1</v>
@@ -2576,7 +2495,10 @@
         <v>114</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>290</v>
+        <v>249</v>
+      </c>
+      <c r="C115" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
@@ -2584,7 +2506,7 @@
         <v>115</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>291</v>
+        <v>250</v>
       </c>
       <c r="C116" s="1">
         <v>1</v>
@@ -2595,7 +2517,7 @@
         <v>116</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>292</v>
+        <v>251</v>
       </c>
       <c r="C117" s="1">
         <v>1</v>
@@ -2606,7 +2528,7 @@
         <v>117</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>330</v>
+        <v>283</v>
       </c>
       <c r="C118" s="1">
         <v>1</v>
@@ -2617,7 +2539,7 @@
         <v>118</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>293</v>
+        <v>252</v>
       </c>
       <c r="C119" s="1">
         <v>1</v>
@@ -2628,7 +2550,7 @@
         <v>119</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>329</v>
+        <v>282</v>
       </c>
       <c r="C120" s="1">
         <v>1</v>
@@ -2639,7 +2561,7 @@
         <v>120</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>328</v>
+        <v>281</v>
       </c>
       <c r="C121" s="1">
         <v>1</v>
@@ -2650,7 +2572,7 @@
         <v>121</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>294</v>
+        <v>253</v>
       </c>
       <c r="C122" s="1">
         <v>1</v>
@@ -2661,7 +2583,7 @@
         <v>122</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>199</v>
+        <v>180</v>
       </c>
       <c r="C123" s="1">
         <v>1</v>
@@ -2672,7 +2594,7 @@
         <v>123</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>201</v>
+        <v>182</v>
       </c>
       <c r="C124" s="1">
         <v>1</v>
@@ -2683,7 +2605,7 @@
         <v>124</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>202</v>
+        <v>183</v>
       </c>
       <c r="C125" s="1">
         <v>1</v>
@@ -2694,7 +2616,7 @@
         <v>125</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
       <c r="C126" s="1">
         <v>1</v>
@@ -2763,7 +2685,7 @@
         <v>134</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>74</v>
+        <v>124</v>
       </c>
       <c r="C135" s="1">
         <v>1</v>
@@ -2774,7 +2696,7 @@
         <v>135</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>71</v>
+        <v>125</v>
       </c>
       <c r="C136" s="1">
         <v>1</v>
@@ -2785,7 +2707,7 @@
         <v>136</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>72</v>
+        <v>126</v>
       </c>
       <c r="C137" s="1">
         <v>1</v>
@@ -2796,7 +2718,7 @@
         <v>137</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>75</v>
+        <v>127</v>
       </c>
       <c r="C138" s="1">
         <v>1</v>
@@ -2807,7 +2729,10 @@
         <v>138</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>73</v>
+        <v>129</v>
+      </c>
+      <c r="C139" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
@@ -2815,7 +2740,7 @@
         <v>139</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="C140" s="1">
         <v>1</v>
@@ -2826,7 +2751,7 @@
         <v>140</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="C141" s="1">
         <v>1</v>
@@ -2837,7 +2762,7 @@
         <v>141</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="C142" s="1">
         <v>1</v>
@@ -2848,7 +2773,7 @@
         <v>142</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="C143" s="1">
         <v>1</v>
@@ -2859,7 +2784,7 @@
         <v>143</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="C144" s="1">
         <v>1</v>
@@ -2870,7 +2795,7 @@
         <v>144</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>144</v>
+        <v>184</v>
       </c>
       <c r="C145" s="1">
         <v>1</v>
@@ -2881,10 +2806,7 @@
         <v>145</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C146" s="1">
-        <v>1</v>
+        <v>173</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
@@ -2892,7 +2814,7 @@
         <v>146</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="C147" s="1">
         <v>1</v>
@@ -2903,7 +2825,7 @@
         <v>147</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>148</v>
+        <v>177</v>
       </c>
       <c r="C148" s="1">
         <v>1</v>
@@ -2914,7 +2836,7 @@
         <v>148</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="C149" s="1">
         <v>1</v>
@@ -2925,7 +2847,7 @@
         <v>149</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>203</v>
+        <v>58</v>
       </c>
       <c r="C150" s="1">
         <v>1</v>
@@ -2936,7 +2858,10 @@
         <v>150</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>191</v>
+        <v>57</v>
+      </c>
+      <c r="C151" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
@@ -2944,7 +2869,7 @@
         <v>151</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>156</v>
+        <v>59</v>
       </c>
       <c r="C152" s="1">
         <v>1</v>
@@ -2955,7 +2880,7 @@
         <v>152</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>195</v>
+        <v>60</v>
       </c>
       <c r="C153" s="1">
         <v>1</v>
@@ -2966,7 +2891,7 @@
         <v>153</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>155</v>
+        <v>62</v>
       </c>
       <c r="C154" s="1">
         <v>1</v>
@@ -2977,7 +2902,7 @@
         <v>154</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C155" s="1">
         <v>1</v>
@@ -2988,7 +2913,7 @@
         <v>155</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>57</v>
+        <v>254</v>
       </c>
       <c r="C156" s="1">
         <v>1</v>
@@ -2999,7 +2924,7 @@
         <v>156</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>59</v>
+        <v>255</v>
       </c>
       <c r="C157" s="1">
         <v>1</v>
@@ -3010,7 +2935,7 @@
         <v>157</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>60</v>
+        <v>256</v>
       </c>
       <c r="C158" s="1">
         <v>1</v>
@@ -3021,7 +2946,7 @@
         <v>158</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>62</v>
+        <v>257</v>
       </c>
       <c r="C159" s="1">
         <v>1</v>
@@ -3032,7 +2957,7 @@
         <v>159</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>61</v>
+        <v>258</v>
       </c>
       <c r="C160" s="1">
         <v>1</v>
@@ -3043,10 +2968,7 @@
         <v>160</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="C161" s="1">
-        <v>1</v>
+        <v>259</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">
@@ -3054,7 +2976,7 @@
         <v>161</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>296</v>
+        <v>260</v>
       </c>
       <c r="C162" s="1">
         <v>1</v>
@@ -3065,7 +2987,7 @@
         <v>162</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>297</v>
+        <v>261</v>
       </c>
       <c r="C163" s="1">
         <v>1</v>
@@ -3076,7 +2998,7 @@
         <v>163</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>298</v>
+        <v>262</v>
       </c>
       <c r="C164" s="1">
         <v>1</v>
@@ -3087,7 +3009,7 @@
         <v>164</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>299</v>
+        <v>263</v>
       </c>
       <c r="C165" s="1">
         <v>1</v>
@@ -3098,7 +3020,10 @@
         <v>165</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>300</v>
+        <v>286</v>
+      </c>
+      <c r="C166" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.2">
@@ -3106,7 +3031,7 @@
         <v>166</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>301</v>
+        <v>66</v>
       </c>
       <c r="C167" s="1">
         <v>1</v>
@@ -3117,7 +3042,7 @@
         <v>167</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>302</v>
+        <v>138</v>
       </c>
       <c r="C168" s="1">
         <v>1</v>
@@ -3128,7 +3053,7 @@
         <v>168</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>303</v>
+        <v>287</v>
       </c>
       <c r="C169" s="1">
         <v>1</v>
@@ -3139,7 +3064,7 @@
         <v>169</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>304</v>
+        <v>288</v>
       </c>
       <c r="C170" s="1">
         <v>1</v>
@@ -3150,7 +3075,7 @@
         <v>170</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>133</v>
+        <v>199</v>
       </c>
       <c r="C171" s="1">
         <v>1</v>
@@ -3161,7 +3086,7 @@
         <v>171</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>67</v>
+        <v>289</v>
       </c>
       <c r="C172" s="1">
         <v>1</v>
@@ -3172,7 +3097,7 @@
         <v>172</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>154</v>
+        <v>198</v>
       </c>
       <c r="C173" s="1">
         <v>1</v>
@@ -3183,7 +3108,10 @@
         <v>173</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>234</v>
+        <v>223</v>
+      </c>
+      <c r="C174" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.2">
@@ -3191,7 +3119,7 @@
         <v>174</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>238</v>
+        <v>65</v>
       </c>
       <c r="C175" s="1">
         <v>1</v>
@@ -3202,7 +3130,7 @@
         <v>175</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C176" s="1">
         <v>1</v>
@@ -3213,7 +3141,7 @@
         <v>176</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>186</v>
+        <v>235</v>
       </c>
       <c r="C177" s="1">
         <v>1</v>
@@ -3224,7 +3152,7 @@
         <v>177</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>235</v>
+        <v>135</v>
       </c>
       <c r="C178" s="1">
         <v>1</v>
@@ -3235,7 +3163,7 @@
         <v>178</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>236</v>
+        <v>200</v>
       </c>
       <c r="C179" s="1">
         <v>1</v>
@@ -3246,7 +3174,7 @@
         <v>179</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>263</v>
+        <v>290</v>
       </c>
       <c r="C180" s="1">
         <v>1</v>
@@ -3257,7 +3185,7 @@
         <v>180</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>66</v>
+        <v>201</v>
       </c>
       <c r="C181" s="1">
         <v>1</v>
@@ -3268,7 +3196,7 @@
         <v>181</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>274</v>
+        <v>64</v>
       </c>
       <c r="C182" s="1">
         <v>1</v>
@@ -3279,7 +3207,7 @@
         <v>182</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
       <c r="C183" s="1">
         <v>1</v>
@@ -3289,67 +3217,31 @@
       <c r="A184" s="1">
         <v>183</v>
       </c>
-      <c r="B184" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C184" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A185" s="1">
         <v>184</v>
       </c>
-      <c r="B185" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="C185" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A186" s="1">
         <v>185</v>
       </c>
-      <c r="B186" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C186" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A187" s="1">
         <v>186</v>
       </c>
-      <c r="B187" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="C187" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A188" s="1">
         <v>187</v>
       </c>
-      <c r="B188" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C188" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A189" s="1">
         <v>188</v>
       </c>
-      <c r="B189" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="C189" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A190" s="1">
@@ -3375,68 +3267,140 @@
       <c r="A194" s="1">
         <v>193</v>
       </c>
+      <c r="B194" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C194" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A195" s="1">
         <v>194</v>
       </c>
+      <c r="B195" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C195" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A196" s="1">
         <v>195</v>
       </c>
+      <c r="B196" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C196" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A197" s="1">
         <v>196</v>
       </c>
+      <c r="B197" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C197" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A198" s="1">
         <v>197</v>
       </c>
+      <c r="B198" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C198" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A199" s="1">
         <v>198</v>
       </c>
+      <c r="B199" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C199" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A200" s="1">
         <v>199</v>
       </c>
+      <c r="B200" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C200" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A201" s="1">
         <v>200</v>
       </c>
+      <c r="B201" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C201" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A202" s="1">
         <v>201</v>
       </c>
+      <c r="B202" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C202" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A203" s="1">
         <v>202</v>
       </c>
+      <c r="B203" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C203" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A204" s="1">
         <v>203</v>
       </c>
+      <c r="B204" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C204" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A205" s="1">
         <v>204</v>
       </c>
+      <c r="B205" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C205" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A206" s="1">
         <v>205</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>306</v>
+        <v>236</v>
       </c>
       <c r="C206" s="1">
         <v>1</v>
@@ -3447,7 +3411,7 @@
         <v>206</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>204</v>
+        <v>87</v>
       </c>
       <c r="C207" s="1">
         <v>1</v>
@@ -3458,7 +3422,7 @@
         <v>207</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>91</v>
+        <v>166</v>
       </c>
       <c r="C208" s="1">
         <v>1</v>
@@ -3469,7 +3433,7 @@
         <v>208</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>257</v>
+        <v>75</v>
       </c>
       <c r="C209" s="1">
         <v>1</v>
@@ -3491,7 +3455,7 @@
         <v>210</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>175</v>
+        <v>82</v>
       </c>
       <c r="C211" s="1">
         <v>1</v>
@@ -3502,7 +3466,7 @@
         <v>211</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>76</v>
+        <v>167</v>
       </c>
       <c r="C212" s="1">
         <v>1</v>
@@ -3513,7 +3477,7 @@
         <v>212</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>206</v>
+        <v>89</v>
       </c>
       <c r="C213" s="1">
         <v>1</v>
@@ -3535,7 +3499,7 @@
         <v>214</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>207</v>
+        <v>83</v>
       </c>
       <c r="C215" s="1">
         <v>1</v>
@@ -3546,7 +3510,7 @@
         <v>215</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>78</v>
+        <v>188</v>
       </c>
       <c r="C216" s="1">
         <v>1</v>
@@ -3557,7 +3521,7 @@
         <v>216</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="C217" s="1">
         <v>1</v>
@@ -3568,7 +3532,7 @@
         <v>217</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>93</v>
+        <v>168</v>
       </c>
       <c r="C218" s="1">
         <v>1</v>
@@ -3579,7 +3543,7 @@
         <v>218</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>181</v>
+        <v>160</v>
       </c>
       <c r="C219" s="1">
         <v>1</v>
@@ -3590,7 +3554,7 @@
         <v>219</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>276</v>
+        <v>161</v>
       </c>
       <c r="C220" s="1">
         <v>1</v>
@@ -3601,7 +3565,7 @@
         <v>220</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>94</v>
+        <v>162</v>
       </c>
       <c r="C221" s="1">
         <v>1</v>
@@ -3612,7 +3576,7 @@
         <v>221</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>182</v>
+        <v>79</v>
       </c>
       <c r="C222" s="1">
         <v>1</v>
@@ -3623,7 +3587,7 @@
         <v>222</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>81</v>
+        <v>163</v>
       </c>
       <c r="C223" s="1">
         <v>1</v>
@@ -3634,7 +3598,7 @@
         <v>223</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="C224" s="1">
         <v>1</v>
@@ -3645,7 +3609,7 @@
         <v>224</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>208</v>
+        <v>80</v>
       </c>
       <c r="C225" s="1">
         <v>1</v>
@@ -3656,7 +3620,10 @@
         <v>225</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>327</v>
+        <v>91</v>
+      </c>
+      <c r="C226" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.2">
@@ -3664,7 +3631,7 @@
         <v>226</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>95</v>
+        <v>164</v>
       </c>
       <c r="C227" s="1">
         <v>1</v>
@@ -3675,7 +3642,7 @@
         <v>227</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C228" s="1">
         <v>1</v>
@@ -3686,7 +3653,7 @@
         <v>228</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>183</v>
+        <v>121</v>
       </c>
       <c r="C229" s="1">
         <v>1</v>
@@ -3697,7 +3664,7 @@
         <v>229</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>96</v>
+        <v>189</v>
       </c>
       <c r="C230" s="1">
         <v>1</v>
@@ -3707,232 +3674,106 @@
       <c r="A231" s="1">
         <v>230</v>
       </c>
-      <c r="B231" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C231" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A232" s="1">
         <v>231</v>
       </c>
-      <c r="B232" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C232" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A233" s="1">
         <v>232</v>
       </c>
-      <c r="B233" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="C233" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A234" s="1">
         <v>233</v>
       </c>
-      <c r="B234" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C234" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A235" s="1">
         <v>234</v>
       </c>
-      <c r="B235" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C235" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A236" s="1">
         <v>235</v>
       </c>
-      <c r="B236" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C236" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A237" s="1">
         <v>236</v>
       </c>
-      <c r="B237" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="C237" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A238" s="1">
         <v>237</v>
       </c>
-      <c r="B238" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C238" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A239" s="1">
         <v>238</v>
       </c>
-      <c r="B239" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C239" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A240" s="1">
         <v>239</v>
       </c>
-      <c r="B240" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="C240" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A241" s="1">
         <v>240</v>
       </c>
-      <c r="B241" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C241" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A242" s="1">
         <v>241</v>
       </c>
-      <c r="B242" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C242" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A243" s="1">
         <v>242</v>
       </c>
-      <c r="B243" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C243" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A244" s="1">
         <v>243</v>
       </c>
-      <c r="B244" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="C244" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A245" s="1">
         <v>244</v>
       </c>
-      <c r="B245" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C245" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A246" s="1">
         <v>245</v>
       </c>
-      <c r="B246" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C246" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A247" s="1">
         <v>246</v>
       </c>
-      <c r="B247" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="C247" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A248" s="1">
         <v>247</v>
       </c>
-      <c r="B248" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="C248" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A249" s="1">
         <v>248</v>
       </c>
-      <c r="B249" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="C249" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A250" s="1">
         <v>249</v>
       </c>
-      <c r="B250" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="C250" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A251" s="1">
         <v>250</v>
       </c>
-      <c r="B251" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="C251" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A252" s="1">
@@ -3948,200 +3789,197 @@
       <c r="A254" s="1">
         <v>253</v>
       </c>
+      <c r="B254" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C254" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A255" s="1">
         <v>254</v>
       </c>
+      <c r="B255" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C255" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A256" s="1">
         <v>255</v>
       </c>
+      <c r="B256" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C256" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A257" s="1">
         <v>256</v>
       </c>
+      <c r="B257" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C257" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A258" s="1">
         <v>257</v>
       </c>
+      <c r="B258" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C258" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A259" s="1">
         <v>258</v>
       </c>
+      <c r="B259" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C259" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A260" s="1">
         <v>259</v>
       </c>
+      <c r="B260" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C260" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A261" s="1">
         <v>260</v>
       </c>
+      <c r="B261" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C261" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A262" s="1">
         <v>261</v>
       </c>
+      <c r="B262" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="C262" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A263" s="1">
         <v>262</v>
       </c>
+      <c r="B263" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C263" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A264" s="1">
         <v>263</v>
       </c>
+      <c r="B264" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C264" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A265" s="1">
         <v>264</v>
       </c>
+      <c r="B265" s="1" t="s">
+        <v>299</v>
+      </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A266" s="1">
         <v>265</v>
       </c>
-      <c r="B266" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C266" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A267" s="1">
         <v>266</v>
       </c>
-      <c r="B267" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C267" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A268" s="1">
         <v>267</v>
       </c>
-      <c r="B268" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="C268" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A269" s="1">
         <v>268</v>
       </c>
-      <c r="B269" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="C269" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A270" s="1">
         <v>269</v>
       </c>
-      <c r="B270" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="C270" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A271" s="1">
         <v>270</v>
       </c>
-      <c r="B271" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="C271" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A272" s="1">
         <v>271</v>
       </c>
-      <c r="B272" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C272" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A273" s="1">
         <v>272</v>
       </c>
-      <c r="B273" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="C273" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A274" s="1">
         <v>273</v>
       </c>
-      <c r="B274" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="C274" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A275" s="1">
         <v>274</v>
       </c>
-      <c r="B275" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="C275" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A276" s="1">
         <v>275</v>
       </c>
-      <c r="B276" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C276" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A277" s="1">
         <v>276</v>
       </c>
-      <c r="B277" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="C277" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A278" s="1">
         <v>277</v>
       </c>
       <c r="B278" s="1" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="C278" s="1">
         <v>1</v>
@@ -4151,63 +3989,129 @@
       <c r="A279" s="1">
         <v>278</v>
       </c>
+      <c r="B279" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C279" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A280" s="1">
         <v>279</v>
       </c>
+      <c r="B280" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C280" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A281" s="1">
         <v>280</v>
       </c>
+      <c r="B281" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C281" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A282" s="1">
         <v>281</v>
       </c>
+      <c r="B282" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C282" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A283" s="1">
         <v>282</v>
       </c>
+      <c r="B283" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C283" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A284" s="1">
         <v>283</v>
       </c>
+      <c r="B284" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C284" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A285" s="1">
         <v>284</v>
       </c>
+      <c r="B285" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="C285" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A286" s="1">
         <v>285</v>
       </c>
+      <c r="B286" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C286" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A287" s="1">
         <v>286</v>
       </c>
+      <c r="B287" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C287" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A288" s="1">
         <v>287</v>
       </c>
+      <c r="B288" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C288" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A289" s="1">
         <v>288</v>
       </c>
+      <c r="B289" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="C289" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A290" s="1">
         <v>289</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>278</v>
+        <v>102</v>
       </c>
       <c r="C290" s="1">
         <v>1</v>
@@ -4218,7 +4122,7 @@
         <v>290</v>
       </c>
       <c r="B291" s="1" t="s">
-        <v>197</v>
+        <v>104</v>
       </c>
       <c r="C291" s="1">
         <v>1</v>
@@ -4228,188 +4132,86 @@
       <c r="A292" s="1">
         <v>291</v>
       </c>
-      <c r="B292" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="C292" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A293" s="1">
         <v>292</v>
       </c>
-      <c r="B293" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C293" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A294" s="1">
         <v>293</v>
       </c>
-      <c r="B294" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="C294" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A295" s="1">
         <v>294</v>
       </c>
-      <c r="B295" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="C295" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A296" s="1">
         <v>295</v>
       </c>
-      <c r="B296" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C296" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A297" s="1">
         <v>296</v>
       </c>
-      <c r="B297" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C297" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A298" s="1">
         <v>297</v>
       </c>
-      <c r="B298" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C298" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A299" s="1">
         <v>298</v>
       </c>
-      <c r="B299" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C299" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A300" s="1">
         <v>299</v>
       </c>
-      <c r="B300" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="C300" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A301" s="1">
         <v>300</v>
       </c>
-      <c r="B301" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C301" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A302" s="1">
         <v>301</v>
       </c>
-      <c r="B302" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C302" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A303" s="1">
         <v>302</v>
       </c>
-      <c r="B303" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="C303" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A304" s="1">
         <v>303</v>
       </c>
-      <c r="B304" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C304" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A305" s="1">
         <v>304</v>
       </c>
-      <c r="B305" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C305" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A306" s="1">
         <v>305</v>
       </c>
-      <c r="B306" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C306" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A307" s="1">
         <v>306</v>
       </c>
-      <c r="B307" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C307" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A308" s="1">
         <v>307</v>
       </c>
-      <c r="B308" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C308" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A309" s="1">
@@ -4440,56 +4242,122 @@
       <c r="A314" s="1">
         <v>313</v>
       </c>
+      <c r="B314" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C314" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A315" s="1">
         <v>314</v>
       </c>
+      <c r="B315" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C315" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A316" s="1">
         <v>315</v>
       </c>
+      <c r="B316" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C316" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A317" s="1">
         <v>316</v>
       </c>
+      <c r="B317" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C317" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A318" s="1">
         <v>317</v>
       </c>
+      <c r="B318" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C318" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A319" s="1">
         <v>318</v>
       </c>
+      <c r="B319" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C319" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A320" s="1">
         <v>319</v>
       </c>
+      <c r="B320" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C320" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A321" s="1">
         <v>320</v>
       </c>
+      <c r="B321" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C321" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A322" s="1">
         <v>321</v>
       </c>
+      <c r="B322" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C322" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A323" s="1">
         <v>322</v>
       </c>
+      <c r="B323" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C323" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A324" s="1">
         <v>323</v>
       </c>
+      <c r="B324" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C324" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A325" s="1">
@@ -4500,140 +4368,68 @@
       <c r="A326" s="1">
         <v>325</v>
       </c>
-      <c r="B326" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="C326" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A327" s="1">
         <v>326</v>
       </c>
-      <c r="B327" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="C327" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A328" s="1">
         <v>327</v>
       </c>
-      <c r="B328" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="C328" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A329" s="1">
         <v>328</v>
       </c>
-      <c r="B329" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C329" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A330" s="1">
         <v>329</v>
       </c>
-      <c r="B330" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="C330" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A331" s="1">
         <v>330</v>
       </c>
-      <c r="B331" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C331" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A332" s="1">
         <v>331</v>
       </c>
-      <c r="B332" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C332" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A333" s="1">
         <v>332</v>
       </c>
-      <c r="B333" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C333" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A334" s="1">
         <v>333</v>
       </c>
-      <c r="B334" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="C334" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A335" s="1">
         <v>334</v>
       </c>
-      <c r="B335" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="C335" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A336" s="1">
         <v>335</v>
       </c>
-      <c r="B336" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C336" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A337" s="1">
         <v>336</v>
       </c>
-      <c r="B337" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C337" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A338" s="1">
         <v>337</v>
       </c>
       <c r="B338" s="1" t="s">
-        <v>312</v>
+        <v>192</v>
       </c>
       <c r="C338" s="1">
         <v>1</v>
@@ -4644,7 +4440,7 @@
         <v>338</v>
       </c>
       <c r="B339" s="1" t="s">
-        <v>218</v>
+        <v>151</v>
       </c>
       <c r="C339" s="1">
         <v>1</v>
@@ -4654,23 +4450,11 @@
       <c r="A340" s="1">
         <v>339</v>
       </c>
-      <c r="B340" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C340" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A341" s="1">
         <v>340</v>
       </c>
-      <c r="B341" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C341" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A342" s="1">
@@ -4716,68 +4500,140 @@
       <c r="A350" s="1">
         <v>349</v>
       </c>
+      <c r="B350" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C350" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A351" s="1">
         <v>350</v>
       </c>
+      <c r="B351" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C351" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A352" s="1">
         <v>351</v>
       </c>
+      <c r="B352" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="C352" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A353" s="1">
         <v>352</v>
       </c>
+      <c r="B353" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C353" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A354" s="1">
         <v>353</v>
       </c>
+      <c r="B354" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C354" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="355" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A355" s="1">
         <v>354</v>
       </c>
+      <c r="B355" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C355" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="356" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A356" s="1">
         <v>355</v>
       </c>
+      <c r="B356" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="C356" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="357" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A357" s="1">
         <v>356</v>
       </c>
+      <c r="B357" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C357" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="358" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A358" s="1">
         <v>357</v>
       </c>
+      <c r="B358" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="C358" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="359" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A359" s="1">
         <v>358</v>
       </c>
+      <c r="B359" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="C359" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A360" s="1">
         <v>359</v>
       </c>
+      <c r="B360" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C360" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="361" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A361" s="1">
         <v>360</v>
       </c>
+      <c r="B361" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C361" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="362" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A362" s="1">
         <v>361</v>
       </c>
       <c r="B362" s="1" t="s">
-        <v>219</v>
+        <v>240</v>
       </c>
       <c r="C362" s="1">
         <v>1</v>
@@ -4788,7 +4644,7 @@
         <v>362</v>
       </c>
       <c r="B363" s="1" t="s">
-        <v>220</v>
+        <v>241</v>
       </c>
       <c r="C363" s="1">
         <v>1</v>
@@ -4799,7 +4655,7 @@
         <v>363</v>
       </c>
       <c r="B364" s="1" t="s">
-        <v>221</v>
+        <v>242</v>
       </c>
       <c r="C364" s="1">
         <v>1</v>
@@ -4810,7 +4666,7 @@
         <v>364</v>
       </c>
       <c r="B365" s="1" t="s">
-        <v>222</v>
+        <v>294</v>
       </c>
       <c r="C365" s="1">
         <v>1</v>
@@ -4821,7 +4677,7 @@
         <v>365</v>
       </c>
       <c r="B366" s="1" t="s">
-        <v>223</v>
+        <v>297</v>
       </c>
       <c r="C366" s="1">
         <v>1</v>
@@ -4832,7 +4688,7 @@
         <v>366</v>
       </c>
       <c r="B367" s="1" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="C367" s="1">
         <v>1</v>
@@ -4843,7 +4699,7 @@
         <v>367</v>
       </c>
       <c r="B368" s="1" t="s">
-        <v>224</v>
+        <v>117</v>
       </c>
       <c r="C368" s="1">
         <v>1</v>
@@ -4854,7 +4710,7 @@
         <v>368</v>
       </c>
       <c r="B369" s="1" t="s">
-        <v>167</v>
+        <v>193</v>
       </c>
       <c r="C369" s="1">
         <v>1</v>
@@ -4865,7 +4721,7 @@
         <v>369</v>
       </c>
       <c r="B370" s="1" t="s">
-        <v>122</v>
+        <v>243</v>
       </c>
       <c r="C370" s="1">
         <v>1</v>
@@ -4876,7 +4732,7 @@
         <v>370</v>
       </c>
       <c r="B371" s="1" t="s">
-        <v>130</v>
+        <v>298</v>
       </c>
       <c r="C371" s="1">
         <v>1</v>
@@ -4887,7 +4743,7 @@
         <v>371</v>
       </c>
       <c r="B372" s="1" t="s">
-        <v>321</v>
+        <v>221</v>
       </c>
       <c r="C372" s="1">
         <v>1</v>
@@ -4897,36 +4753,78 @@
       <c r="A373" s="1">
         <v>372</v>
       </c>
+      <c r="B373" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C373" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A374" s="1">
         <v>373</v>
       </c>
+      <c r="B374" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C374" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A375" s="1">
         <v>374</v>
       </c>
+      <c r="B375" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C375" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A376" s="1">
         <v>375</v>
       </c>
+      <c r="B376" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C376" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A377" s="1">
         <v>376</v>
       </c>
+      <c r="B377" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C377" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A378" s="1">
         <v>377</v>
       </c>
+      <c r="B378" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C378" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A379" s="1">
         <v>378</v>
       </c>
+      <c r="B379" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C379" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A380" s="1">
@@ -4963,7 +4861,7 @@
         <v>385</v>
       </c>
       <c r="B386" s="1" t="s">
-        <v>279</v>
+        <v>303</v>
       </c>
       <c r="C386" s="1">
         <v>1</v>
@@ -4974,7 +4872,7 @@
         <v>386</v>
       </c>
       <c r="B387" s="1" t="s">
-        <v>260</v>
+        <v>194</v>
       </c>
       <c r="C387" s="1">
         <v>1</v>
@@ -4985,7 +4883,7 @@
         <v>387</v>
       </c>
       <c r="B388" s="1" t="s">
-        <v>123</v>
+        <v>196</v>
       </c>
       <c r="C388" s="1">
         <v>1</v>
@@ -4996,7 +4894,7 @@
         <v>388</v>
       </c>
       <c r="B389" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C389" s="1">
         <v>1</v>
@@ -5007,7 +4905,7 @@
         <v>389</v>
       </c>
       <c r="B390" s="1" t="s">
-        <v>125</v>
+        <v>195</v>
       </c>
       <c r="C390" s="1">
         <v>1</v>
@@ -5018,7 +4916,7 @@
         <v>390</v>
       </c>
       <c r="B391" s="1" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="C391" s="1">
         <v>1</v>
@@ -5029,10 +4927,7 @@
         <v>391</v>
       </c>
       <c r="B392" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="C392" s="1">
-        <v>1</v>
+        <v>186</v>
       </c>
     </row>
     <row r="393" spans="1:3" x14ac:dyDescent="0.2">
@@ -5040,7 +4935,10 @@
         <v>392</v>
       </c>
       <c r="B393" s="1" t="s">
-        <v>281</v>
+        <v>197</v>
+      </c>
+      <c r="C393" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="394" spans="1:3" x14ac:dyDescent="0.2">
@@ -5048,7 +4946,7 @@
         <v>393</v>
       </c>
       <c r="B394" s="1" t="s">
-        <v>282</v>
+        <v>300</v>
       </c>
       <c r="C394" s="1">
         <v>1</v>
@@ -5059,7 +4957,7 @@
         <v>394</v>
       </c>
       <c r="B395" s="1" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="C395" s="1">
         <v>1</v>
@@ -5070,7 +4968,7 @@
         <v>395</v>
       </c>
       <c r="B396" s="1" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="C396" s="1">
         <v>1</v>
@@ -5081,7 +4979,7 @@
         <v>396</v>
       </c>
       <c r="B397" s="1" t="s">
-        <v>128</v>
+        <v>272</v>
       </c>
       <c r="C397" s="1">
         <v>1</v>
@@ -5091,111 +4989,51 @@
       <c r="A398" s="1">
         <v>397</v>
       </c>
-      <c r="B398" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="C398" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="399" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A399" s="1">
         <v>398</v>
       </c>
-      <c r="B399" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="C399" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="400" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A400" s="1">
         <v>399</v>
       </c>
-      <c r="B400" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="C400" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="401" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A401" s="1">
         <v>400</v>
       </c>
-      <c r="B401" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="C401" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="402" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A402" s="1">
         <v>401</v>
       </c>
-      <c r="B402" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="C402" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="403" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A403" s="1">
         <v>402</v>
       </c>
-      <c r="B403" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="C403" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="404" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A404" s="1">
         <v>403</v>
       </c>
-      <c r="B404" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="C404" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="405" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A405" s="1">
         <v>404</v>
       </c>
-      <c r="B405" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="C405" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="406" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A406" s="1">
         <v>405</v>
       </c>
-      <c r="B406" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="C406" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="407" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A407" s="1">
         <v>406</v>
       </c>
-      <c r="B407" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="C407" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="408" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A408" s="1">
@@ -5211,68 +5049,140 @@
       <c r="A410" s="1">
         <v>409</v>
       </c>
+      <c r="B410" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C410" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="411" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A411" s="1">
         <v>410</v>
       </c>
+      <c r="B411" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C411" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="412" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A412" s="1">
         <v>411</v>
       </c>
+      <c r="B412" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C412" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="413" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A413" s="1">
         <v>412</v>
       </c>
+      <c r="B413" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C413" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="414" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A414" s="1">
         <v>413</v>
       </c>
+      <c r="B414" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C414" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="415" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A415" s="1">
         <v>414</v>
       </c>
+      <c r="B415" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C415" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="416" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A416" s="1">
         <v>415</v>
       </c>
+      <c r="B416" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C416" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="417" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A417" s="1">
         <v>416</v>
       </c>
+      <c r="B417" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="C417" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="418" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A418" s="1">
         <v>417</v>
       </c>
+      <c r="B418" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C418" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="419" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A419" s="1">
         <v>418</v>
       </c>
+      <c r="B419" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C419" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="420" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A420" s="1">
         <v>419</v>
       </c>
+      <c r="B420" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C420" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="421" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A421" s="1">
         <v>420</v>
       </c>
+      <c r="B421" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C421" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="422" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A422" s="1">
         <v>421</v>
       </c>
       <c r="B422" s="1" t="s">
-        <v>226</v>
+        <v>278</v>
       </c>
       <c r="C422" s="1">
         <v>1</v>
@@ -5283,7 +5193,7 @@
         <v>422</v>
       </c>
       <c r="B423" s="1" t="s">
-        <v>228</v>
+        <v>152</v>
       </c>
       <c r="C423" s="1">
         <v>1</v>
@@ -5294,7 +5204,7 @@
         <v>423</v>
       </c>
       <c r="B424" s="1" t="s">
-        <v>134</v>
+        <v>111</v>
       </c>
       <c r="C424" s="1">
         <v>1</v>
@@ -5304,425 +5214,278 @@
       <c r="A425" s="1">
         <v>424</v>
       </c>
-      <c r="B425" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="C425" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="426" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A426" s="1">
         <v>425</v>
       </c>
-      <c r="B426" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C426" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="427" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A427" s="1">
         <v>426</v>
       </c>
-      <c r="B427" s="1" t="s">
-        <v>205</v>
-      </c>
     </row>
     <row r="428" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A428" s="1">
         <v>427</v>
       </c>
-      <c r="B428" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="C428" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="429" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A429" s="1">
         <v>428</v>
       </c>
-      <c r="B429" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="C429" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="430" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A430" s="1">
         <v>429</v>
       </c>
-      <c r="B430" s="1" t="s">
-        <v>325</v>
-      </c>
     </row>
     <row r="431" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A431" s="1">
         <v>430</v>
       </c>
-      <c r="B431" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="C431" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="432" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A432" s="1">
         <v>431</v>
       </c>
-      <c r="B432" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="C432" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="433" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="433" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A433" s="1">
         <v>432</v>
       </c>
-      <c r="B433" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="C433" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="434" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="434" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A434" s="1">
         <v>433</v>
       </c>
-      <c r="B434" s="1" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="435" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="435" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A435" s="1">
         <v>434</v>
       </c>
-      <c r="B435" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C435" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="436" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="436" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A436" s="1">
         <v>435</v>
       </c>
-      <c r="B436" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="C436" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="437" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="437" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A437" s="1">
         <v>436</v>
       </c>
     </row>
-    <row r="438" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="438" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A438" s="1">
         <v>437</v>
       </c>
     </row>
-    <row r="439" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="439" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A439" s="1">
         <v>438</v>
       </c>
     </row>
-    <row r="440" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="440" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A440" s="1">
         <v>439</v>
       </c>
     </row>
-    <row r="441" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="441" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A441" s="1">
         <v>440</v>
       </c>
     </row>
-    <row r="442" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="442" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A442" s="1">
         <v>441</v>
       </c>
     </row>
-    <row r="443" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="443" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A443" s="1">
         <v>442</v>
       </c>
     </row>
-    <row r="444" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="444" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A444" s="1">
         <v>443</v>
       </c>
     </row>
-    <row r="445" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="445" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A445" s="1">
         <v>444</v>
       </c>
     </row>
-    <row r="446" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="446" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A446" s="1">
         <v>445</v>
       </c>
     </row>
-    <row r="447" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="447" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A447" s="1">
         <v>446</v>
       </c>
     </row>
-    <row r="448" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="448" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A448" s="1">
         <v>447</v>
       </c>
     </row>
-    <row r="449" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="449" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A449" s="1">
         <v>448</v>
       </c>
     </row>
-    <row r="450" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="450" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A450" s="1">
         <v>449</v>
       </c>
     </row>
-    <row r="451" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="451" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A451" s="1">
         <v>450</v>
       </c>
     </row>
-    <row r="452" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="452" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A452" s="1">
         <v>451</v>
       </c>
     </row>
-    <row r="453" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="453" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A453" s="1">
         <v>452</v>
       </c>
     </row>
-    <row r="454" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="454" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A454" s="1">
         <v>453</v>
       </c>
     </row>
-    <row r="455" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="455" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A455" s="1">
         <v>454</v>
       </c>
     </row>
-    <row r="456" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="456" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A456" s="1">
         <v>455</v>
       </c>
     </row>
-    <row r="457" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="457" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A457" s="1">
         <v>456</v>
       </c>
     </row>
-    <row r="458" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="458" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A458" s="1">
         <v>457</v>
       </c>
-      <c r="B458" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="C458" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="459" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="459" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A459" s="1">
         <v>458</v>
       </c>
-      <c r="B459" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C459" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="460" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="460" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A460" s="1">
         <v>459</v>
       </c>
-      <c r="B460" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C460" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="461" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="461" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A461" s="1">
         <v>460</v>
       </c>
-      <c r="B461" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C461" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="462" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="462" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A462" s="1">
         <v>461</v>
       </c>
-      <c r="B462" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="C462" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="463" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="463" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A463" s="1">
         <v>462</v>
       </c>
-      <c r="B463" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C463" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="464" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="464" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A464" s="1">
         <v>463</v>
       </c>
-      <c r="B464" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="C464" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="465" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="465" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A465" s="1">
         <v>464</v>
       </c>
-      <c r="B465" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C465" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="466" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="466" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A466" s="1">
         <v>465</v>
       </c>
-      <c r="B466" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C466" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="467" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="467" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A467" s="1">
         <v>466</v>
       </c>
-      <c r="B467" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C467" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="468" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="468" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A468" s="1">
         <v>467</v>
       </c>
-      <c r="B468" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C468" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="469" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="469" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A469" s="1">
         <v>468</v>
       </c>
-      <c r="B469" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="C469" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="470" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="470" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A470" s="1">
         <v>469</v>
       </c>
-      <c r="B470" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C470" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="471" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="471" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A471" s="1">
         <v>470</v>
       </c>
-      <c r="B471" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C471" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="472" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="472" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A472" s="1">
         <v>471</v>
       </c>
     </row>
-    <row r="473" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="473" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A473" s="1">
         <v>472</v>
       </c>
     </row>
-    <row r="474" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="474" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A474" s="1">
         <v>473</v>
       </c>
     </row>
-    <row r="475" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="475" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A475" s="1">
         <v>474</v>
       </c>
     </row>
-    <row r="476" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="476" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A476" s="1">
         <v>475</v>
       </c>
     </row>
-    <row r="477" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="477" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A477" s="1">
         <v>476</v>
       </c>
     </row>
-    <row r="478" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="478" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A478" s="1">
         <v>477</v>
       </c>
     </row>
-    <row r="479" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="479" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A479" s="1">
         <v>478</v>
       </c>
     </row>
-    <row r="480" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="480" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A480" s="1">
         <v>479</v>
       </c>

</xml_diff>